<commit_message>
fix: handle field multiple
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7482AC3-D844-4F1A-A4CA-BEDFA30C9E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2954448D-E85A-4A00-B8E1-93BA2CAD2648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="1" activeTab="1" xr2:uid="{812734FB-07EB-41F2-BC3F-FD4E85E7589A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="1" activeTab="3" xr2:uid="{812734FB-07EB-41F2-BC3F-FD4E85E7589A}"/>
   </bookViews>
   <sheets>
     <sheet name="LIBRARY INDUSTRY CLASSIFICATION" sheetId="27" state="hidden" r:id="rId1"/>
@@ -2234,55 +2234,10 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="35" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="35" borderId="13" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
@@ -2296,6 +2251,51 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="35" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="35" borderId="13" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -4468,8 +4468,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="A2:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4529,8 +4529,8 @@
       <c r="A4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="82"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -4546,10 +4546,10 @@
       <c r="A5" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -4565,10 +4565,10 @@
       <c r="A6" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="84"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -4601,8 +4601,8 @@
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="86"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4615,8 +4615,8 @@
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="86"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4629,8 +4629,8 @@
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="86"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -4643,8 +4643,8 @@
       <c r="A11" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -4660,8 +4660,8 @@
       <c r="A12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="88"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -4677,8 +4677,8 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="85"/>
-      <c r="C13" s="86"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="71"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -4850,8 +4850,8 @@
       <c r="A24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="71"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -5266,7 +5266,8 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A25:C25"/>
@@ -5327,12 +5328,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
       <c r="X1" t="s">
         <v>11</v>
       </c>
@@ -5952,7 +5953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811D0212-0F7E-4B31-B4FD-59C950AC3207}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -5965,10 +5966,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="74"/>
       <c r="C1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -6339,10 +6340,10 @@
       <c r="C3" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="56" t="s">
@@ -6363,12 +6364,12 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="56"/>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="75" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="57"/>
@@ -6426,20 +6427,20 @@
       <c r="F10" s="46"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="80"/>
-      <c r="C11" s="78" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="80"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="57"/>
@@ -6993,12 +6994,12 @@
       </c>
     </row>
     <row r="64" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="79" t="s">
+      <c r="C64" s="76" t="s">
         <v>292</v>
       </c>
-      <c r="D64" s="79"/>
-      <c r="E64" s="79"/>
-      <c r="F64" s="79"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="59"/>
@@ -7017,10 +7018,10 @@
       <c r="B71" s="53" t="s">
         <v>293</v>
       </c>
-      <c r="C71" s="74" t="s">
+      <c r="C71" s="78" t="s">
         <v>294</v>
       </c>
-      <c r="D71" s="74"/>
+      <c r="D71" s="78"/>
       <c r="E71" s="55" t="s">
         <v>167</v>
       </c>
@@ -7032,13 +7033,13 @@
       <c r="K71" s="54"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B72" s="77" t="s">
+      <c r="B72" s="79" t="s">
         <v>295</v>
       </c>
-      <c r="C72" s="74" t="s">
+      <c r="C72" s="78" t="s">
         <v>296</v>
       </c>
-      <c r="D72" s="74"/>
+      <c r="D72" s="78"/>
       <c r="E72" s="54" t="s">
         <v>165</v>
       </c>
@@ -7050,11 +7051,11 @@
       <c r="K72" s="54"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B73" s="77"/>
-      <c r="C73" s="74" t="s">
+      <c r="B73" s="79"/>
+      <c r="C73" s="78" t="s">
         <v>297</v>
       </c>
-      <c r="D73" s="74"/>
+      <c r="D73" s="78"/>
       <c r="E73" s="54" t="s">
         <v>165</v>
       </c>
@@ -7066,11 +7067,11 @@
       <c r="K73" s="54"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B74" s="77"/>
-      <c r="C74" s="74" t="s">
+      <c r="B74" s="79"/>
+      <c r="C74" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="D74" s="74"/>
+      <c r="D74" s="78"/>
       <c r="E74" s="54" t="s">
         <v>165</v>
       </c>
@@ -7082,11 +7083,11 @@
       <c r="K74" s="54"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B75" s="77"/>
-      <c r="C75" s="74" t="s">
+      <c r="B75" s="79"/>
+      <c r="C75" s="78" t="s">
         <v>299</v>
       </c>
-      <c r="D75" s="74"/>
+      <c r="D75" s="78"/>
       <c r="E75" s="54" t="s">
         <v>165</v>
       </c>
@@ -7101,10 +7102,10 @@
       <c r="B76" s="53" t="s">
         <v>303</v>
       </c>
-      <c r="C76" s="74" t="s">
+      <c r="C76" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="D76" s="74"/>
+      <c r="D76" s="78"/>
       <c r="E76" s="55" t="s">
         <v>166</v>
       </c>
@@ -7119,147 +7120,147 @@
       <c r="B77" s="53" t="s">
         <v>304</v>
       </c>
-      <c r="C77" s="69" t="s">
+      <c r="C77" s="84" t="s">
         <v>301</v>
       </c>
-      <c r="D77" s="69"/>
+      <c r="D77" s="84"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="53" t="s">
         <v>305</v>
       </c>
-      <c r="C78" s="69" t="s">
+      <c r="C78" s="84" t="s">
         <v>302</v>
       </c>
-      <c r="D78" s="69"/>
+      <c r="D78" s="84"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B79" s="75" t="s">
+      <c r="B79" s="80" t="s">
         <v>306</v>
       </c>
-      <c r="C79" s="71" t="s">
+      <c r="C79" s="81" t="s">
         <v>307</v>
       </c>
-      <c r="D79" s="71"/>
+      <c r="D79" s="81"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B80" s="75"/>
-      <c r="C80" s="73" t="s">
+      <c r="B80" s="80"/>
+      <c r="C80" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="D80" s="71"/>
+      <c r="D80" s="81"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="75"/>
-      <c r="C81" s="73" t="s">
+      <c r="B81" s="80"/>
+      <c r="C81" s="82" t="s">
         <v>315</v>
       </c>
-      <c r="D81" s="71"/>
+      <c r="D81" s="81"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="75"/>
-      <c r="C82" s="73" t="s">
+      <c r="B82" s="80"/>
+      <c r="C82" s="82" t="s">
         <v>316</v>
       </c>
-      <c r="D82" s="71"/>
+      <c r="D82" s="81"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="75"/>
-      <c r="C83" s="73" t="s">
+      <c r="B83" s="80"/>
+      <c r="C83" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="D83" s="71"/>
+      <c r="D83" s="81"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="75"/>
-      <c r="C84" s="71" t="s">
+      <c r="B84" s="80"/>
+      <c r="C84" s="81" t="s">
         <v>318</v>
       </c>
-      <c r="D84" s="71"/>
+      <c r="D84" s="81"/>
     </row>
     <row r="85" spans="2:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="75"/>
-      <c r="C85" s="72" t="s">
+      <c r="B85" s="80"/>
+      <c r="C85" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="D85" s="72"/>
+      <c r="D85" s="86"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="75"/>
-      <c r="C86" s="71" t="s">
+      <c r="B86" s="80"/>
+      <c r="C86" s="81" t="s">
         <v>320</v>
       </c>
-      <c r="D86" s="71"/>
+      <c r="D86" s="81"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="75"/>
-      <c r="C87" s="73" t="s">
+      <c r="B87" s="80"/>
+      <c r="C87" s="82" t="s">
         <v>321</v>
       </c>
-      <c r="D87" s="71"/>
+      <c r="D87" s="81"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B88" s="75"/>
-      <c r="C88" s="73" t="s">
+      <c r="B88" s="80"/>
+      <c r="C88" s="82" t="s">
         <v>322</v>
       </c>
-      <c r="D88" s="71"/>
+      <c r="D88" s="81"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="75"/>
-      <c r="C89" s="73" t="s">
+      <c r="B89" s="80"/>
+      <c r="C89" s="82" t="s">
         <v>323</v>
       </c>
-      <c r="D89" s="71"/>
+      <c r="D89" s="81"/>
     </row>
     <row r="90" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="75"/>
-      <c r="C90" s="73" t="s">
+      <c r="B90" s="80"/>
+      <c r="C90" s="82" t="s">
         <v>324</v>
       </c>
-      <c r="D90" s="71"/>
+      <c r="D90" s="81"/>
     </row>
     <row r="91" spans="2:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="75"/>
-      <c r="C91" s="71" t="s">
+      <c r="B91" s="80"/>
+      <c r="C91" s="81" t="s">
         <v>325</v>
       </c>
-      <c r="D91" s="71"/>
+      <c r="D91" s="81"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="75"/>
-      <c r="C92" s="71" t="s">
+      <c r="B92" s="80"/>
+      <c r="C92" s="81" t="s">
         <v>326</v>
       </c>
-      <c r="D92" s="71"/>
+      <c r="D92" s="81"/>
     </row>
     <row r="93" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="75" t="s">
+      <c r="B93" s="80" t="s">
         <v>308</v>
       </c>
-      <c r="C93" s="71" t="s">
+      <c r="C93" s="81" t="s">
         <v>327</v>
       </c>
-      <c r="D93" s="71"/>
+      <c r="D93" s="81"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="75"/>
-      <c r="C94" s="71" t="s">
+      <c r="B94" s="80"/>
+      <c r="C94" s="81" t="s">
         <v>328</v>
       </c>
-      <c r="D94" s="71"/>
+      <c r="D94" s="81"/>
     </row>
     <row r="95" spans="2:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="76" t="s">
+      <c r="B95" s="83" t="s">
         <v>309</v>
       </c>
-      <c r="C95" s="69" t="s">
+      <c r="C95" s="84" t="s">
         <v>329</v>
       </c>
-      <c r="D95" s="69"/>
+      <c r="D95" s="84"/>
     </row>
     <row r="96" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B96" s="76"/>
+      <c r="B96" s="83"/>
       <c r="C96" s="51" t="s">
         <v>330</v>
       </c>
@@ -7268,7 +7269,7 @@
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="76"/>
+      <c r="B97" s="83"/>
       <c r="C97" s="51" t="s">
         <v>331</v>
       </c>
@@ -7277,7 +7278,7 @@
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="76"/>
+      <c r="B98" s="83"/>
       <c r="C98" s="51" t="s">
         <v>332</v>
       </c>
@@ -7286,7 +7287,7 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="76"/>
+      <c r="B99" s="83"/>
       <c r="C99" s="51" t="s">
         <v>333</v>
       </c>
@@ -7295,7 +7296,7 @@
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="76"/>
+      <c r="B100" s="83"/>
       <c r="C100" s="51" t="s">
         <v>334</v>
       </c>
@@ -7304,7 +7305,7 @@
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B101" s="76"/>
+      <c r="B101" s="83"/>
       <c r="C101" s="51" t="s">
         <v>335</v>
       </c>
@@ -7316,65 +7317,40 @@
       <c r="B102" s="53" t="s">
         <v>310</v>
       </c>
-      <c r="C102" s="69" t="s">
+      <c r="C102" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="D102" s="69"/>
+      <c r="D102" s="84"/>
     </row>
     <row r="103" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B103" s="53" t="s">
         <v>311</v>
       </c>
-      <c r="C103" s="69" t="s">
+      <c r="C103" s="84" t="s">
         <v>343</v>
       </c>
-      <c r="D103" s="69"/>
+      <c r="D103" s="84"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="53" t="s">
         <v>312</v>
       </c>
-      <c r="C104" s="69" t="s">
+      <c r="C104" s="84" t="s">
         <v>344</v>
       </c>
-      <c r="D104" s="69"/>
+      <c r="D104" s="84"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="C105" s="69" t="s">
+      <c r="C105" s="84" t="s">
         <v>345</v>
       </c>
-      <c r="D105" s="69"/>
+      <c r="D105" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="B79:B92"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="B95:B101"/>
-    <mergeCell ref="C95:D95"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
@@ -7391,6 +7367,31 @@
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="B95:B101"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="B79:B92"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: handle fu and fix indent
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2954448D-E85A-4A00-B8E1-93BA2CAD2648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3881959B-19D3-4678-89E0-7F52164AEDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="1" activeTab="3" xr2:uid="{812734FB-07EB-41F2-BC3F-FD4E85E7589A}"/>
   </bookViews>
@@ -213,8 +213,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -340,9 +338,6 @@
     <t>DED CHARGE</t>
   </si>
   <si>
-    <t>Performance Bond (%)</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -886,66 +881,6 @@
   </si>
   <si>
     <t>fd_Effluent Consideration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ch_mg/L </t>
-  </si>
-  <si>
-    <t>fm_Max. TDS</t>
-  </si>
-  <si>
-    <t>fm_Operation Time Day</t>
-  </si>
-  <si>
-    <t>fm_COD</t>
-  </si>
-  <si>
-    <t>fm_BOD</t>
-  </si>
-  <si>
-    <t>fm_TSS</t>
-  </si>
-  <si>
-    <t>fm_FOG</t>
-  </si>
-  <si>
-    <t>fm_Max. NH3</t>
-  </si>
-  <si>
-    <t>fm_Max. Sulfur</t>
-  </si>
-  <si>
-    <t>fm_TKN</t>
-  </si>
-  <si>
-    <t>fm_TP</t>
-  </si>
-  <si>
-    <t>fm_Max. Color Index</t>
-  </si>
-  <si>
-    <t>fm_Max. Turbidity</t>
-  </si>
-  <si>
-    <t>fm_Flow</t>
-  </si>
-  <si>
-    <t>ch_h/day</t>
-  </si>
-  <si>
-    <t>ch_PtCo</t>
-  </si>
-  <si>
-    <t>ch_NTU</t>
-  </si>
-  <si>
-    <t>ch_CMD</t>
-  </si>
-  <si>
-    <t>ch_w/w</t>
-  </si>
-  <si>
-    <t>fdfm_Expected Discharge Cake MC</t>
   </si>
   <si>
     <t>ch_Client</t>
@@ -1309,6 +1244,69 @@
   </si>
   <si>
     <t>fh_VI. TERMS AND CONDITIONS</t>
+  </si>
+  <si>
+    <t>f_Max. TDS</t>
+  </si>
+  <si>
+    <t>f_Operation Time Day</t>
+  </si>
+  <si>
+    <t>f_COD</t>
+  </si>
+  <si>
+    <t>f_BOD</t>
+  </si>
+  <si>
+    <t>f_TSS</t>
+  </si>
+  <si>
+    <t>f_FOG</t>
+  </si>
+  <si>
+    <t>f_Max. NH3</t>
+  </si>
+  <si>
+    <t>f_Max. Sulfur</t>
+  </si>
+  <si>
+    <t>f_TKN</t>
+  </si>
+  <si>
+    <t>f_TP</t>
+  </si>
+  <si>
+    <t>f_Max. Color Index</t>
+  </si>
+  <si>
+    <t>f_Max. Turbidity</t>
+  </si>
+  <si>
+    <t>f_Flow</t>
+  </si>
+  <si>
+    <t>fd_Expected Discharge Cake MC</t>
+  </si>
+  <si>
+    <t>f_Performance Bond (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fu_mg/L </t>
+  </si>
+  <si>
+    <t>fu_h/day</t>
+  </si>
+  <si>
+    <t>fu_PtCo</t>
+  </si>
+  <si>
+    <t>fu_NTU</t>
+  </si>
+  <si>
+    <t>fu_CMD</t>
+  </si>
+  <si>
+    <t>fu_w/w</t>
   </si>
 </sst>
 </file>
@@ -2061,7 +2059,7 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2107,9 +2105,6 @@
     </xf>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2213,6 +2208,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2240,11 +2241,11 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="19" fillId="35" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="35" borderId="13" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2255,6 +2256,33 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2264,38 +2292,41 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="35" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="35" borderId="13" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="35" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="35" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -4175,275 +4206,275 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.109375" style="25" customWidth="1"/>
-    <col min="4" max="5" width="28.5546875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="25" customWidth="1"/>
-    <col min="8" max="16384" width="8.44140625" style="25"/>
+    <col min="1" max="3" width="30.109375" style="24" customWidth="1"/>
+    <col min="4" max="5" width="28.5546875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="24" customWidth="1"/>
+    <col min="8" max="16384" width="8.44140625" style="24"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="24" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="31" t="s">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="31" t="s">
+      <c r="C22" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="31" t="s">
+      <c r="C24" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="31" t="s">
+      <c r="C29" s="30" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="31" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="31" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="32" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4468,8 +4499,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="A2:C24"/>
+    <sheetView topLeftCell="A4" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4485,21 +4516,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
+      <c r="A1" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4509,14 +4540,14 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -4527,10 +4558,10 @@
     </row>
     <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
+        <v>41</v>
+      </c>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -4544,12 +4575,12 @@
     </row>
     <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="87" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="88"/>
+        <v>169</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="72"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -4563,12 +4594,12 @@
     </row>
     <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="87" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="88"/>
+        <v>170</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="72"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -4581,11 +4612,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -4599,10 +4630,10 @@
     </row>
     <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
+        <v>44</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4613,10 +4644,10 @@
     </row>
     <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
+        <v>45</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4627,10 +4658,10 @@
     </row>
     <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
+        <v>43</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -4641,10 +4672,10 @@
     </row>
     <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
+        <v>145</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -4658,10 +4689,10 @@
     </row>
     <row r="12" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
+        <v>46</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -4675,10 +4706,10 @@
     </row>
     <row r="13" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
+        <v>47</v>
+      </c>
+      <c r="B13" s="60"/>
+      <c r="C13" s="61"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -4688,11 +4719,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="63"/>
+      <c r="A14" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -4703,17 +4734,17 @@
     </row>
     <row r="15" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -4724,13 +4755,13 @@
     </row>
     <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -4741,7 +4772,7 @@
     </row>
     <row r="17" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="6"/>
@@ -4755,7 +4786,7 @@
     </row>
     <row r="18" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="6"/>
@@ -4769,7 +4800,7 @@
     </row>
     <row r="19" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -4786,7 +4817,7 @@
     </row>
     <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -4803,7 +4834,7 @@
     </row>
     <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -4820,7 +4851,7 @@
     </row>
     <row r="22" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="6"/>
@@ -4834,7 +4865,7 @@
     </row>
     <row r="23" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="6"/>
@@ -4848,10 +4879,10 @@
     </row>
     <row r="24" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
+        <v>50</v>
+      </c>
+      <c r="B24" s="60"/>
+      <c r="C24" s="61"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -4861,14 +4892,14 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="61" t="s">
-        <v>182</v>
-      </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="A25" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -4879,10 +4910,10 @@
     </row>
     <row r="26" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="B26" s="69"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -4895,11 +4926,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
+      <c r="A27" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -4913,10 +4944,10 @@
     </row>
     <row r="28" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -4927,10 +4958,10 @@
     </row>
     <row r="29" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -4941,10 +4972,10 @@
     </row>
     <row r="30" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="B30" s="60"/>
+      <c r="C30" s="61"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -4955,10 +4986,10 @@
     </row>
     <row r="31" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+        <v>145</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -4972,10 +5003,10 @@
     </row>
     <row r="32" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="B32" s="60"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -4989,10 +5020,10 @@
     </row>
     <row r="33" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -5001,36 +5032,29 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="17" t="s">
+    <row r="34" spans="1:14" s="89" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="88"/>
     </row>
     <row r="35" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -5041,7 +5065,7 @@
     </row>
     <row r="36" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5055,7 +5079,7 @@
     </row>
     <row r="37" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5069,7 +5093,7 @@
     </row>
     <row r="38" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -5086,7 +5110,7 @@
     </row>
     <row r="39" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -5103,7 +5127,7 @@
     </row>
     <row r="40" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -5120,7 +5144,7 @@
     </row>
     <row r="41" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5134,10 +5158,10 @@
     </row>
     <row r="42" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="B42" s="60"/>
+      <c r="C42" s="61"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -5228,7 +5252,7 @@
       <c r="N51" s="1"/>
     </row>
     <row r="52" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
+      <c r="A52" s="18"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -5266,7 +5290,16 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="17">
+  <mergeCells count="25">
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A7:C7"/>
@@ -5283,7 +5316,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5313,8 +5345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1819EE-D6ED-4D4B-AE5F-26864AB818A8}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A12" zoomScale="81" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5328,53 +5360,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
+      <c r="A1" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
       <c r="X1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="D2" s="16"/>
       <c r="X2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>169</v>
+        <v>183</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>168</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2"/>
       <c r="X3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="4"/>
@@ -5384,13 +5416,13 @@
     </row>
     <row r="5" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>41</v>
+        <v>184</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="15"/>
       <c r="X5" t="s">
@@ -5399,11 +5431,11 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="B6" s="16"/>
       <c r="C6" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2"/>
       <c r="X6" t="s">
@@ -5412,26 +5444,26 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D7" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>2</v>
       </c>
       <c r="X7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="8"/>
       <c r="X8" t="s">
@@ -5440,11 +5472,11 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2"/>
       <c r="X9" t="s">
@@ -5453,11 +5485,11 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="13"/>
       <c r="X10" t="s">
@@ -5466,69 +5498,69 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="15"/>
       <c r="X11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2"/>
       <c r="X12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="B13" s="16"/>
       <c r="C13" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="37" t="s">
         <v>2</v>
       </c>
       <c r="X13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="B14" s="17"/>
       <c r="C14" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="8"/>
       <c r="X14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2"/>
       <c r="X15" t="s">
@@ -5537,11 +5569,11 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="13"/>
       <c r="X16" t="s">
@@ -5550,43 +5582,43 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="15"/>
       <c r="X17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B18" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2"/>
       <c r="X18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="B19" s="16"/>
       <c r="C19" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="37" t="s">
         <v>2</v>
       </c>
       <c r="X19" t="s">
@@ -5595,13 +5627,13 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" s="8"/>
       <c r="X20" t="s">
@@ -5610,13 +5642,13 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="8"/>
       <c r="X21" t="s">
@@ -5625,84 +5657,84 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="17"/>
+        <v>55</v>
+      </c>
+      <c r="B22" s="16"/>
       <c r="C22" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="21"/>
+        <v>92</v>
+      </c>
+      <c r="D22" s="20"/>
       <c r="X22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B23" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="21"/>
+      <c r="C23" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="20"/>
       <c r="X23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B24" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="21"/>
+      <c r="C24" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="20"/>
       <c r="X24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="14"/>
-      <c r="C25" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="21"/>
+      <c r="C25" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="20"/>
       <c r="X25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="17"/>
+        <v>62</v>
+      </c>
+      <c r="D26" s="16"/>
       <c r="X26" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="D27" s="36" t="s">
+      <c r="C27" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="35" t="s">
         <v>31</v>
       </c>
       <c r="X27" t="s">
@@ -5711,14 +5743,14 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="14"/>
-      <c r="C28" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" s="41" t="s">
-        <v>69</v>
+      <c r="C28" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>68</v>
       </c>
       <c r="X28" t="s">
         <v>28</v>
@@ -5726,13 +5758,13 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="14"/>
-      <c r="C29" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="36" t="s">
+      <c r="C29" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="35" t="s">
         <v>8</v>
       </c>
       <c r="X29" t="s">
@@ -5741,137 +5773,137 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="40" t="s">
-        <v>96</v>
+      <c r="C30" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="39" t="s">
-        <v>97</v>
+      <c r="C31" s="38" t="s">
+        <v>96</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="39" t="s">
-        <v>32</v>
+      <c r="C32" s="38" t="s">
+        <v>341</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34" s="42" t="s">
+      <c r="C34" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="D35" s="42" t="s">
+      <c r="C35" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" s="41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="8"/>
-      <c r="C36" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="D36" s="42" t="s">
+      <c r="C36" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="41" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="D38" s="42" t="s">
+      <c r="C38" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D39" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="41" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D40" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="41" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B41" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D41" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="41" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5953,8 +5985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811D0212-0F7E-4B31-B4FD-59C950AC3207}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5966,325 +5998,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>212</v>
+        <v>327</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="60" t="s">
-        <v>211</v>
+      <c r="C3" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>213</v>
+        <v>328</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="34" t="s">
-        <v>225</v>
+      <c r="C4" s="33" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="9"/>
+        <v>206</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="91"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>207</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="91"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="9"/>
+        <v>150</v>
+      </c>
+      <c r="B7" s="94"/>
+      <c r="C7" s="95"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B8" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="93"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="35"/>
+        <v>151</v>
+      </c>
+      <c r="B9" s="94"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>214</v>
+        <v>329</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="35" t="s">
-        <v>211</v>
+      <c r="C10" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>215</v>
+        <v>330</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="35" t="s">
-        <v>211</v>
+      <c r="C11" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>216</v>
+        <v>331</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="35" t="s">
-        <v>211</v>
+      <c r="C12" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>217</v>
+        <v>332</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="35" t="s">
-        <v>211</v>
+      <c r="C13" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>218</v>
+        <v>333</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="35" t="s">
-        <v>211</v>
+      <c r="C14" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>219</v>
+        <v>334</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="35" t="s">
-        <v>211</v>
+      <c r="C15" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>220</v>
+        <v>335</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="35" t="s">
-        <v>211</v>
+      <c r="C16" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>221</v>
+        <v>336</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="35" t="s">
-        <v>211</v>
+      <c r="C17" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>222</v>
+        <v>337</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="35" t="s">
-        <v>226</v>
+      <c r="C18" s="34" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>223</v>
+        <v>338</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="35" t="s">
-        <v>227</v>
+      <c r="C19" s="34" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="35"/>
+        <v>152</v>
+      </c>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>224</v>
+        <v>339</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="35" t="s">
-        <v>228</v>
+      <c r="C21" s="34" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" s="9"/>
+        <v>209</v>
+      </c>
+      <c r="B23" s="90" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="91"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="35"/>
+        <v>151</v>
+      </c>
+      <c r="B24" s="98"/>
+      <c r="C24" s="99"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="35" t="s">
-        <v>211</v>
+        <v>329</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="35" t="s">
-        <v>211</v>
+        <v>330</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="35" t="s">
-        <v>211</v>
+        <v>331</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="35" t="s">
-        <v>211</v>
+        <v>332</v>
+      </c>
+      <c r="B28" s="36"/>
+      <c r="C28" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="35" t="s">
-        <v>211</v>
+        <v>333</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="35" t="s">
-        <v>211</v>
+        <v>334</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="35" t="s">
-        <v>211</v>
+        <v>335</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="35" t="s">
-        <v>211</v>
+        <v>336</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="59" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="35" t="s">
-        <v>226</v>
+        <v>337</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="34" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="35" t="s">
-        <v>227</v>
+        <v>338</v>
+      </c>
+      <c r="B34" s="36"/>
+      <c r="C34" s="34" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="9"/>
+        <v>152</v>
+      </c>
+      <c r="B35" s="98"/>
+      <c r="C35" s="99"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" s="63"/>
+      <c r="C36" s="64"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>229</v>
+        <v>340</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="13">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B20" xr:uid="{FA192426-A47F-4375-83D6-14EC0F0BD2BD}">
@@ -6330,1027 +6374,1052 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="50" t="s">
-        <v>346</v>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
-      <c r="C3" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" s="85" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="77"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="55"/>
+      <c r="C5" s="85" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="56"/>
+      <c r="C6" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="56"/>
+      <c r="C7" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="56"/>
+      <c r="C8" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+    </row>
+    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="56"/>
+      <c r="C9" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="56"/>
+      <c r="C10" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="87"/>
+      <c r="C11" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="87"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="56"/>
+      <c r="C13" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="56"/>
+      <c r="C14" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="56"/>
+      <c r="C15" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="56"/>
+      <c r="C16" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="45"/>
+      <c r="E16" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="46"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="56"/>
+      <c r="C17" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="56"/>
+      <c r="C18" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="45"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="56"/>
+      <c r="C19" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="56"/>
+      <c r="C20" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="D20" s="45"/>
+      <c r="E20" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" s="45"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="56"/>
+      <c r="C21" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="56"/>
+      <c r="C22" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="47"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="55"/>
+      <c r="C23" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="56"/>
+      <c r="C24" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="D24" s="45"/>
+      <c r="E24" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" s="45"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="56"/>
+      <c r="C25" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="45"/>
+      <c r="E25" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="45"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="56"/>
+      <c r="C26" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="56"/>
+      <c r="C27" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="56"/>
+      <c r="C28" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="56"/>
+      <c r="C29" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" s="45"/>
+      <c r="E29" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="46"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="56"/>
+      <c r="C30" s="46" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="45"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="56"/>
+      <c r="C31" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="56"/>
+      <c r="C32" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="55"/>
+      <c r="C33" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="56"/>
+      <c r="C34" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="D34" s="45"/>
+      <c r="E34" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="45"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="56"/>
+      <c r="C35" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="45"/>
+      <c r="E35" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="45"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="56"/>
+      <c r="C36" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="D36" s="45"/>
+      <c r="E36" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="46"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="56"/>
+      <c r="C37" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="56"/>
+      <c r="C38" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="D38" s="45"/>
+      <c r="E38" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="46"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="56"/>
+      <c r="C39" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39" s="45"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="56"/>
+      <c r="C40" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" s="45"/>
+      <c r="E40" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F40" s="45"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="55"/>
+      <c r="C41" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="44"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="56"/>
+      <c r="C42" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D42" s="45"/>
+      <c r="E42" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="55"/>
+      <c r="C43" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
+    </row>
+    <row r="44" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="56"/>
+      <c r="C44" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="45"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="56"/>
+      <c r="C45" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" s="45"/>
+      <c r="F45" s="46"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="56"/>
+      <c r="C46" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="48"/>
+      <c r="E46" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" s="46"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="56"/>
+      <c r="C47" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+    </row>
+    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="56"/>
+      <c r="C48" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="D48" s="48"/>
+      <c r="E48" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F48" s="45"/>
+    </row>
+    <row r="49" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="56"/>
+      <c r="C49" s="46" t="s">
+        <v>256</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="55"/>
+      <c r="C50" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="44"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="56"/>
+      <c r="C51" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="45"/>
+      <c r="E51" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="46"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="56"/>
+      <c r="C52" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="D52" s="45"/>
+      <c r="E52" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F52" s="45"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="56"/>
+      <c r="C53" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="D53" s="45"/>
+      <c r="E53" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F53" s="46"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="56"/>
+      <c r="C54" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="D54" s="45"/>
+      <c r="E54" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="46"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="57"/>
+      <c r="C55" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="44"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="56"/>
+      <c r="C56" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="45"/>
+      <c r="E56" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F56" s="46"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="56"/>
+      <c r="C57" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="D57" s="45"/>
+      <c r="E57" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F57" s="46"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="56"/>
+      <c r="C58" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="D58" s="45"/>
+      <c r="E58" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F58" s="46"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="56"/>
+      <c r="C59" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D59" s="45"/>
+      <c r="E59" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F59" s="46"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="56"/>
+      <c r="C60" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D60" s="45"/>
+      <c r="E60" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" s="46"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="56"/>
+      <c r="C61" s="46" t="s">
+        <v>268</v>
+      </c>
+      <c r="D61" s="45"/>
+      <c r="E61" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F61" s="46"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="56"/>
+      <c r="C62" s="46" t="s">
+        <v>269</v>
+      </c>
+      <c r="D62" s="45"/>
+      <c r="E62" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F62" s="46"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="56"/>
+      <c r="C63" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="D63" s="45"/>
+      <c r="E63" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F63" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="86" t="s">
+        <v>271</v>
+      </c>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="58"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69" s="49"/>
+      <c r="C69" s="49" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B71" s="52" t="s">
+        <v>272</v>
+      </c>
+      <c r="C71" s="81" t="s">
+        <v>273</v>
+      </c>
+      <c r="D71" s="81"/>
+      <c r="E71" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="53"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B72" s="84" t="s">
+        <v>274</v>
+      </c>
+      <c r="C72" s="81" t="s">
+        <v>275</v>
+      </c>
+      <c r="D72" s="81"/>
+      <c r="E72" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="85"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="56"/>
-      <c r="C5" s="75" t="s">
-        <v>235</v>
-      </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="57"/>
-      <c r="C6" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="57"/>
-      <c r="C7" s="47" t="s">
-        <v>237</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="57"/>
-      <c r="C8" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
-      <c r="C11" s="75" t="s">
-        <v>241</v>
-      </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="77"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="47" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
-      <c r="C16" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F16" s="47"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="57"/>
-      <c r="C17" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="D17" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F18" s="46"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="57"/>
-      <c r="C19" s="47" t="s">
-        <v>248</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F19" s="46"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="57"/>
-      <c r="C20" s="47" t="s">
-        <v>249</v>
-      </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F20" s="46"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="57"/>
-      <c r="C21" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F21" s="46"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="57"/>
-      <c r="C22" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="48"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="56"/>
-      <c r="C23" s="45" t="s">
-        <v>252</v>
-      </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="45"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="57"/>
-      <c r="C24" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F24" s="46"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="57"/>
-      <c r="C25" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F25" s="46"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="57"/>
-      <c r="C26" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="57"/>
-      <c r="C27" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="57"/>
-      <c r="C28" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="57"/>
-      <c r="C29" s="47" t="s">
-        <v>258</v>
-      </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="47"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="57"/>
-      <c r="C30" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="D30" s="46"/>
-      <c r="E30" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="46"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="57"/>
-      <c r="C31" s="47" t="s">
-        <v>260</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="57"/>
-      <c r="C32" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="D32" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="56"/>
-      <c r="C33" s="45" t="s">
-        <v>261</v>
-      </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="57"/>
-      <c r="C34" s="47" t="s">
-        <v>262</v>
-      </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" s="46"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="57"/>
-      <c r="C35" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="46"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="57"/>
-      <c r="C36" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" s="47"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="57"/>
-      <c r="C37" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="D37" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E37" s="46"/>
-      <c r="F37" s="47"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="57"/>
-      <c r="C38" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="D38" s="46"/>
-      <c r="E38" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F38" s="47"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="57"/>
-      <c r="C39" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D39" s="46"/>
-      <c r="E39" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" s="46"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="57"/>
-      <c r="C40" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F40" s="46"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="56"/>
-      <c r="C41" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="45"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="57"/>
-      <c r="C42" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F42" s="47"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="56"/>
-      <c r="C43" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="45"/>
-    </row>
-    <row r="44" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="57"/>
-      <c r="C44" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="D44" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F44" s="46"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="57"/>
-      <c r="C45" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="D45" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E45" s="46"/>
-      <c r="F45" s="47"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="57"/>
-      <c r="C46" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" s="47"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="57"/>
-      <c r="C47" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="D47" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-    </row>
-    <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="57"/>
-      <c r="C48" s="47" t="s">
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B73" s="84"/>
+      <c r="C73" s="81" t="s">
         <v>276</v>
       </c>
-      <c r="D48" s="49"/>
-      <c r="E48" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="46"/>
-    </row>
-    <row r="49" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="57"/>
-      <c r="C49" s="47" t="s">
+      <c r="D73" s="81"/>
+      <c r="E73" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
+      <c r="H73" s="53"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="53"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B74" s="84"/>
+      <c r="C74" s="81" t="s">
         <v>277</v>
       </c>
-      <c r="D49" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="56"/>
-      <c r="C50" s="45" t="s">
+      <c r="D74" s="81"/>
+      <c r="E74" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="F74" s="53"/>
+      <c r="G74" s="53"/>
+      <c r="H74" s="53"/>
+      <c r="I74" s="53"/>
+      <c r="J74" s="53"/>
+      <c r="K74" s="53"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B75" s="84"/>
+      <c r="C75" s="81" t="s">
         <v>278</v>
       </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="45"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="57"/>
-      <c r="C51" s="47" t="s">
+      <c r="D75" s="81"/>
+      <c r="E75" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B76" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="C76" s="81" t="s">
         <v>279</v>
       </c>
-      <c r="D51" s="46"/>
-      <c r="E51" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F51" s="47"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="57"/>
-      <c r="C52" s="47" t="s">
+      <c r="D76" s="81"/>
+      <c r="E76" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B77" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="C77" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="D52" s="46"/>
-      <c r="E52" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F52" s="46"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="57"/>
-      <c r="C53" s="47" t="s">
+      <c r="D77" s="76"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B78" s="52" t="s">
+        <v>284</v>
+      </c>
+      <c r="C78" s="76" t="s">
         <v>281</v>
       </c>
-      <c r="D53" s="46"/>
-      <c r="E53" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F53" s="47"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="57"/>
-      <c r="C54" s="47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D54" s="46"/>
-      <c r="E54" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F54" s="47"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="58"/>
-      <c r="C55" s="45" t="s">
-        <v>283</v>
-      </c>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="45"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="57"/>
-      <c r="C56" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="D56" s="46"/>
-      <c r="E56" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F56" s="47"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B57" s="57"/>
-      <c r="C57" s="47" t="s">
+      <c r="D78" s="76"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B79" s="82" t="s">
         <v>285</v>
       </c>
-      <c r="D57" s="46"/>
-      <c r="E57" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F57" s="47"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="57"/>
-      <c r="C58" s="47" t="s">
+      <c r="C79" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="D58" s="46"/>
-      <c r="E58" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F58" s="47"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="57"/>
-      <c r="C59" s="47" t="s">
+      <c r="D79" s="78"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B80" s="82"/>
+      <c r="C80" s="80" t="s">
+        <v>293</v>
+      </c>
+      <c r="D80" s="78"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" s="82"/>
+      <c r="C81" s="80" t="s">
+        <v>294</v>
+      </c>
+      <c r="D81" s="78"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82" s="82"/>
+      <c r="C82" s="80" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="78"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" s="82"/>
+      <c r="C83" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D83" s="78"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84" s="82"/>
+      <c r="C84" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="D84" s="78"/>
+    </row>
+    <row r="85" spans="2:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="82"/>
+      <c r="C85" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="D85" s="79"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="82"/>
+      <c r="C86" s="78" t="s">
+        <v>299</v>
+      </c>
+      <c r="D86" s="78"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87" s="82"/>
+      <c r="C87" s="80" t="s">
+        <v>300</v>
+      </c>
+      <c r="D87" s="78"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88" s="82"/>
+      <c r="C88" s="80" t="s">
+        <v>301</v>
+      </c>
+      <c r="D88" s="78"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B89" s="82"/>
+      <c r="C89" s="80" t="s">
+        <v>302</v>
+      </c>
+      <c r="D89" s="78"/>
+    </row>
+    <row r="90" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="82"/>
+      <c r="C90" s="80" t="s">
+        <v>303</v>
+      </c>
+      <c r="D90" s="78"/>
+    </row>
+    <row r="91" spans="2:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="82"/>
+      <c r="C91" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="D91" s="78"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92" s="82"/>
+      <c r="C92" s="78" t="s">
+        <v>305</v>
+      </c>
+      <c r="D92" s="78"/>
+    </row>
+    <row r="93" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="82" t="s">
         <v>287</v>
       </c>
-      <c r="D59" s="46"/>
-      <c r="E59" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F59" s="47"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="57"/>
-      <c r="C60" s="47" t="s">
-        <v>288</v>
-      </c>
-      <c r="D60" s="46"/>
-      <c r="E60" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F60" s="47"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="57"/>
-      <c r="C61" s="47" t="s">
-        <v>289</v>
-      </c>
-      <c r="D61" s="46"/>
-      <c r="E61" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F61" s="47"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="57"/>
-      <c r="C62" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="D62" s="46"/>
-      <c r="E62" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F62" s="47"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="57"/>
-      <c r="C63" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="D63" s="46"/>
-      <c r="E63" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="F63" s="47" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="76" t="s">
-        <v>292</v>
-      </c>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B65" s="59"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="59"/>
-      <c r="F65" s="59"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B69" s="50"/>
-      <c r="C69" s="50" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B71" s="53" t="s">
-        <v>293</v>
-      </c>
-      <c r="C71" s="78" t="s">
-        <v>294</v>
-      </c>
-      <c r="D71" s="78"/>
-      <c r="E71" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="54"/>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B72" s="79" t="s">
-        <v>295</v>
-      </c>
-      <c r="C72" s="78" t="s">
-        <v>296</v>
-      </c>
-      <c r="D72" s="78"/>
-      <c r="E72" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="54"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B73" s="79"/>
-      <c r="C73" s="78" t="s">
-        <v>297</v>
-      </c>
-      <c r="D73" s="78"/>
-      <c r="E73" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="54"/>
-      <c r="K73" s="54"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B74" s="79"/>
-      <c r="C74" s="78" t="s">
-        <v>298</v>
-      </c>
-      <c r="D74" s="78"/>
-      <c r="E74" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="54"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B75" s="79"/>
-      <c r="C75" s="78" t="s">
-        <v>299</v>
-      </c>
-      <c r="D75" s="78"/>
-      <c r="E75" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="54"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B76" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="C76" s="78" t="s">
-        <v>300</v>
-      </c>
-      <c r="D76" s="78"/>
-      <c r="E76" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
-      <c r="J76" s="54"/>
-      <c r="K76" s="54"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B77" s="53" t="s">
-        <v>304</v>
-      </c>
-      <c r="C77" s="84" t="s">
-        <v>301</v>
-      </c>
-      <c r="D77" s="84"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B78" s="53" t="s">
-        <v>305</v>
-      </c>
-      <c r="C78" s="84" t="s">
-        <v>302</v>
-      </c>
-      <c r="D78" s="84"/>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B79" s="80" t="s">
+      <c r="C93" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="C79" s="81" t="s">
+      <c r="D93" s="78"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="82"/>
+      <c r="C94" s="78" t="s">
         <v>307</v>
       </c>
-      <c r="D79" s="81"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B80" s="80"/>
-      <c r="C80" s="82" t="s">
-        <v>314</v>
-      </c>
-      <c r="D80" s="81"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="80"/>
-      <c r="C81" s="82" t="s">
-        <v>315</v>
-      </c>
-      <c r="D81" s="81"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="80"/>
-      <c r="C82" s="82" t="s">
-        <v>316</v>
-      </c>
-      <c r="D82" s="81"/>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="80"/>
-      <c r="C83" s="82" t="s">
-        <v>317</v>
-      </c>
-      <c r="D83" s="81"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="80"/>
-      <c r="C84" s="81" t="s">
-        <v>318</v>
-      </c>
-      <c r="D84" s="81"/>
-    </row>
-    <row r="85" spans="2:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="80"/>
-      <c r="C85" s="86" t="s">
-        <v>319</v>
-      </c>
-      <c r="D85" s="86"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="80"/>
-      <c r="C86" s="81" t="s">
-        <v>320</v>
-      </c>
-      <c r="D86" s="81"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="80"/>
-      <c r="C87" s="82" t="s">
-        <v>321</v>
-      </c>
-      <c r="D87" s="81"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B88" s="80"/>
-      <c r="C88" s="82" t="s">
-        <v>322</v>
-      </c>
-      <c r="D88" s="81"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="80"/>
-      <c r="C89" s="82" t="s">
-        <v>323</v>
-      </c>
-      <c r="D89" s="81"/>
-    </row>
-    <row r="90" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="80"/>
-      <c r="C90" s="82" t="s">
-        <v>324</v>
-      </c>
-      <c r="D90" s="81"/>
-    </row>
-    <row r="91" spans="2:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="80"/>
-      <c r="C91" s="81" t="s">
-        <v>325</v>
-      </c>
-      <c r="D91" s="81"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="80"/>
-      <c r="C92" s="81" t="s">
-        <v>326</v>
-      </c>
-      <c r="D92" s="81"/>
-    </row>
-    <row r="93" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="80" t="s">
-        <v>308</v>
-      </c>
-      <c r="C93" s="81" t="s">
-        <v>327</v>
-      </c>
-      <c r="D93" s="81"/>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="80"/>
-      <c r="C94" s="81" t="s">
-        <v>328</v>
-      </c>
-      <c r="D94" s="81"/>
+      <c r="D94" s="78"/>
     </row>
     <row r="95" spans="2:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="83" t="s">
-        <v>309</v>
-      </c>
-      <c r="C95" s="84" t="s">
-        <v>329</v>
-      </c>
-      <c r="D95" s="84"/>
+        <v>288</v>
+      </c>
+      <c r="C95" s="76" t="s">
+        <v>308</v>
+      </c>
+      <c r="D95" s="76"/>
     </row>
     <row r="96" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B96" s="83"/>
-      <c r="C96" s="51" t="s">
-        <v>330</v>
-      </c>
-      <c r="D96" s="51" t="s">
-        <v>336</v>
+      <c r="C96" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="D96" s="50" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="83"/>
-      <c r="C97" s="51" t="s">
-        <v>331</v>
-      </c>
-      <c r="D97" s="52" t="s">
-        <v>337</v>
+      <c r="C97" s="50" t="s">
+        <v>310</v>
+      </c>
+      <c r="D97" s="51" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="83"/>
-      <c r="C98" s="51" t="s">
-        <v>332</v>
-      </c>
-      <c r="D98" s="52" t="s">
-        <v>338</v>
+      <c r="C98" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="D98" s="51" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="83"/>
-      <c r="C99" s="51" t="s">
-        <v>333</v>
-      </c>
-      <c r="D99" s="52" t="s">
-        <v>339</v>
+      <c r="C99" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="D99" s="51" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="83"/>
-      <c r="C100" s="51" t="s">
-        <v>334</v>
-      </c>
-      <c r="D100" s="52" t="s">
-        <v>340</v>
+      <c r="C100" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="D100" s="51" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="83"/>
-      <c r="C101" s="51" t="s">
-        <v>335</v>
-      </c>
-      <c r="D101" s="52" t="s">
-        <v>341</v>
+      <c r="C101" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="D101" s="51" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B102" s="53" t="s">
-        <v>310</v>
-      </c>
-      <c r="C102" s="84" t="s">
-        <v>342</v>
-      </c>
-      <c r="D102" s="84"/>
+      <c r="B102" s="52" t="s">
+        <v>289</v>
+      </c>
+      <c r="C102" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="D102" s="76"/>
     </row>
     <row r="103" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="53" t="s">
-        <v>311</v>
-      </c>
-      <c r="C103" s="84" t="s">
-        <v>343</v>
-      </c>
-      <c r="D103" s="84"/>
+      <c r="B103" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="C103" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="D103" s="76"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B104" s="53" t="s">
-        <v>312</v>
-      </c>
-      <c r="C104" s="84" t="s">
-        <v>344</v>
-      </c>
-      <c r="D104" s="84"/>
+      <c r="B104" s="52" t="s">
+        <v>291</v>
+      </c>
+      <c r="C104" s="76" t="s">
+        <v>323</v>
+      </c>
+      <c r="D104" s="76"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B105" s="53" t="s">
-        <v>313</v>
-      </c>
-      <c r="C105" s="84" t="s">
-        <v>345</v>
-      </c>
-      <c r="D105" s="84"/>
+      <c r="B105" s="52" t="s">
+        <v>292</v>
+      </c>
+      <c r="C105" s="76" t="s">
+        <v>324</v>
+      </c>
+      <c r="D105" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="B79:B92"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="B95:B101"/>
+    <mergeCell ref="C95:D95"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
@@ -7367,31 +7436,6 @@
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C78:D78"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="B95:B101"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="B79:B92"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7460,27 +7504,27 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: table data input
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,27 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAB6306-F196-41F5-BE23-AD5847BEAABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F251FC3F-BC66-493B-9C94-B1E7A199DED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="687" firstSheet="3" activeTab="4" xr2:uid="{812734FB-07EB-41F2-BC3F-FD4E85E7589A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="3" activeTab="4" xr2:uid="{812734FB-07EB-41F2-BC3F-FD4E85E7589A}"/>
   </bookViews>
   <sheets>
     <sheet name="LIBRARY INDUSTRY CLASSIFICATION" sheetId="27" state="hidden" r:id="rId1"/>
     <sheet name="DIP_Customer Information" sheetId="18" r:id="rId2"/>
     <sheet name="DIP_Project Information" sheetId="30" r:id="rId3"/>
     <sheet name="DIP_Technical Information" sheetId="29" r:id="rId4"/>
-    <sheet name="DIP_Data Input (2)" sheetId="34" r:id="rId5"/>
-    <sheet name="DIP_Data Input" sheetId="33" r:id="rId6"/>
-    <sheet name="DATA_PROPOSAL" sheetId="23" r:id="rId7"/>
-    <sheet name="DATA_OPEX" sheetId="24" r:id="rId8"/>
-    <sheet name="DATA_BOQ" sheetId="25" r:id="rId9"/>
-    <sheet name="DATA_ELI" sheetId="26" r:id="rId10"/>
+    <sheet name="DIP_Data Input" sheetId="34" r:id="rId5"/>
+    <sheet name="DATA_PROPOSAL" sheetId="23" r:id="rId6"/>
+    <sheet name="DATA_OPEX" sheetId="24" r:id="rId7"/>
+    <sheet name="DATA_BOQ" sheetId="25" r:id="rId8"/>
+    <sheet name="DATA_ELI" sheetId="26" r:id="rId9"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="_12.ABUTHMEN" localSheetId="0">#REF!</definedName>
@@ -204,7 +203,7 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId15"/>
+        <x14:slicerCache r:id="rId14"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -241,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="311">
   <si>
     <t>NEW PROJECT</t>
   </si>
@@ -653,9 +652,6 @@
     <t>User's option</t>
   </si>
   <si>
-    <t>Default Percentage, but user can change</t>
-  </si>
-  <si>
     <t>default: fourteen (14) days, but user can change based on Invoicing Term in DIP_Project Information</t>
   </si>
   <si>
@@ -1001,159 +997,18 @@
     <t>ftn_Notes: Whichever scope not stated but required for the successful commissioning of WWTP system shall be discussed</t>
   </si>
   <si>
-    <t>All items suitably packed for overland transport by trucking</t>
-  </si>
-  <si>
-    <t>To be determined after confirmation by PO/SPK and down payment</t>
-  </si>
-  <si>
-    <t>1.     The system will produce the effluent as refers to the Government’s permit, but the warranty has given with conditions below:</t>
-  </si>
-  <si>
-    <t>- The system operated as the basic design and follows the limit of the inlet flow</t>
-  </si>
-  <si>
-    <t>-  The system operated as its SOP</t>
-  </si>
-  <si>
-    <t>-  The raw water temperature is within the operational value of the basic design</t>
-  </si>
-  <si>
-    <t>-  All equipment/system equipment works properly and is operated properly</t>
-  </si>
-  <si>
-    <t>2.     The warranty is valid if all the system installed by GRINVIRO.</t>
-  </si>
-  <si>
-    <t>3.     The default warranty is valid for 365 calendar days since the system has been commissioned or after the system has reach the parameters quality as standard parameters. If the installed product/equipment/material is defective during fabrication (manufacturing defect)/delivery/installation or during commissioning, GRINVIRO will immediately repair or replace the product/equipment/material.</t>
-  </si>
-  <si>
-    <t>4.     If there is damage to the system which is an operational negligence during the warranty period:</t>
-  </si>
-  <si>
-    <t>-  GRINVIRO will provide support in the form of free repair services</t>
-  </si>
-  <si>
-    <t>-  If there is a replacement of material/equipment parts, it will be entirely the burden of the buyer</t>
-  </si>
-  <si>
-    <t>-  In this case, all accommodation costs (transportation, food and housing costs) are borne by the buyer</t>
-  </si>
-  <si>
-    <t>-  When the warranty period has been over, the buyer will be charged for repairs and or replacement costs for equipment parts/materials (if any)</t>
-  </si>
-  <si>
-    <t>5.     In this case, the buyer is fully aware of the responsibility for the correct operation and according to the SOP and masters the basics of Waste Water Treatment system science for good system operation and maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.     GRINVIRO will provide the certificate of warranty  </t>
-  </si>
-  <si>
-    <t>1.     Equipment outside the manufacture of Grinviro will be given a warranty following a supplier warranty. </t>
-  </si>
-  <si>
-    <t>2.     GRINVIRO will provide the certificate of warranty for equipment by principle.</t>
-  </si>
-  <si>
-    <t>In case the Buyer seeks Termination for convenience of this Contract, such termination shall be effective upon Seller’s receipt of Buyer’s written notice of termination and payment of termination charges in accordance with the Termination Schedule. If Buyer terminates this Contract for convenience, title to the Equipment shall remain with the Seller. Seller may suspend performance upon receipt of Buyer’s termination notice, without incurring any liability to</t>
-  </si>
-  <si>
-    <t>Receipt of Termination Notice by Seller</t>
-  </si>
-  <si>
-    <t>Total Termination Charges, Percent of Total Contract Price</t>
-  </si>
-  <si>
-    <t>1 – 30 days (after DP received)</t>
-  </si>
-  <si>
-    <t>31 – 60 days</t>
-  </si>
-  <si>
-    <t>61 – 90 days</t>
-  </si>
-  <si>
-    <t>91 days – Date of RTS</t>
-  </si>
-  <si>
-    <t>After Date of RTS</t>
-  </si>
-  <si>
-    <t>The technical specifications may vary between equivalent suppliers and/ or technical details</t>
-  </si>
-  <si>
-    <t>This proposal is based on an exchange rate of IDR 16,500 to USD. If the rate exceeds this value, it will impact the project/equipment cost</t>
-  </si>
-  <si>
-    <t>1 month from date of quotation issuance</t>
-  </si>
-  <si>
-    <t>Exclude PPN 11 % and other taxes</t>
-  </si>
-  <si>
     <t>14 days</t>
   </si>
   <si>
     <t>sub_VI. TERMS AND CONDITIONS</t>
   </si>
   <si>
-    <t>-        $P1$% Down Payment payable immediately after signing of the Order Confirmation against presentation of Commercial Invoice</t>
-  </si>
-  <si>
-    <t>-        $P3$% Balance Payment immediately after commissioning</t>
-  </si>
-  <si>
-    <t>-        $P4$% Balance Payment immediately after retention time or 90 days after commissioning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All invoices are due and payable at the specified payment date or </t>
-  </si>
-  <si>
     <t>days after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</t>
   </si>
   <si>
     <t>Helper:</t>
   </si>
   <si>
-    <t>-        $P2$% Balance Payment immediately after material on site or by progressive (75% Material on site &amp; 25% Installation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terms </t>
-  </si>
-  <si>
-    <t>Due Dates</t>
-  </si>
-  <si>
-    <t>Packing</t>
-  </si>
-  <si>
-    <t>Delivery</t>
-  </si>
-  <si>
-    <t>Equipment Warranty</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>exchange Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validity </t>
-  </si>
-  <si>
-    <t>Taxes</t>
-  </si>
-  <si>
-    <t>Payments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Warranty </t>
-  </si>
-  <si>
-    <t>Termination for Convenience</t>
-  </si>
-  <si>
     <t>WRP</t>
   </si>
   <si>
@@ -1172,9 +1027,6 @@
     <t>tdi_-        $P3$% Balance Payment immediately after commissioning</t>
   </si>
   <si>
-    <t>tdi_'-        $P4$% Balance Payment immediately after retention time or 90 days after commissioning</t>
-  </si>
-  <si>
     <t>thr_Payments</t>
   </si>
   <si>
@@ -1317,6 +1169,21 @@
   </si>
   <si>
     <t>LEVEL-1</t>
+  </si>
+  <si>
+    <t>tdi_-        $P4$% Balance Payment immediately after retention time or 90 days after commissioning</t>
+  </si>
+  <si>
+    <t>Default Percentage: 30%, but user can change</t>
+  </si>
+  <si>
+    <t>Default Percentage: 50%, but user can change</t>
+  </si>
+  <si>
+    <t>Default Percentage: 15%, but user can change</t>
+  </si>
+  <si>
+    <t>Default Percentage: 5%, but user can change</t>
   </si>
 </sst>
 </file>
@@ -2232,6 +2099,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2241,15 +2129,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2266,26 +2145,26 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="19" fillId="35" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2298,56 +2177,44 @@
     <xf numFmtId="9" fontId="19" fillId="35" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -4515,46 +4382,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4B5FA4-65EE-45F5-B4AD-337850B5CC81}">
-  <dimension ref="B2:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064A824E-56CC-4807-BE57-7CD799BC0894}">
   <sheetPr codeName="Sheet10"/>
@@ -4577,18 +4404,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="71"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -4601,11 +4428,11 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -4621,8 +4448,8 @@
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="73"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -4636,12 +4463,12 @@
     </row>
     <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -4655,12 +4482,12 @@
     </row>
     <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="75"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -4673,11 +4500,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -4693,8 +4520,8 @@
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4707,8 +4534,8 @@
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4721,8 +4548,8 @@
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="77"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -4735,8 +4562,8 @@
       <c r="A11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="77"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -4752,8 +4579,8 @@
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -4769,8 +4596,8 @@
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="77"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -4780,11 +4607,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="71"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -4798,10 +4625,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -4816,7 +4643,7 @@
     </row>
     <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="11"/>
@@ -4833,7 +4660,7 @@
     </row>
     <row r="17" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4847,7 +4674,7 @@
     </row>
     <row r="18" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -4861,7 +4688,7 @@
     </row>
     <row r="19" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -4878,7 +4705,7 @@
     </row>
     <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -4895,7 +4722,7 @@
     </row>
     <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -4912,7 +4739,7 @@
     </row>
     <row r="22" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -4926,7 +4753,7 @@
     </row>
     <row r="23" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4942,8 +4769,8 @@
       <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -4953,11 +4780,11 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="68" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="70"/>
+      <c r="A25" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
@@ -4973,8 +4800,8 @@
       <c r="A26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -4987,11 +4814,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="69"/>
-      <c r="C27" s="70"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -5007,8 +4834,8 @@
       <c r="A28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="77"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="66"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -5021,8 +4848,8 @@
       <c r="A29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="77"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="66"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -5035,8 +4862,8 @@
       <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="66"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -5049,8 +4876,8 @@
       <c r="A31" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="66"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -5066,8 +4893,8 @@
       <c r="A32" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="77"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -5083,8 +4910,8 @@
       <c r="A33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="77"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="66"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -5098,10 +4925,10 @@
         <v>22</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="D34" s="56"/>
       <c r="E34" s="56"/>
@@ -5109,7 +4936,7 @@
     </row>
     <row r="35" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="11"/>
@@ -5126,7 +4953,7 @@
     </row>
     <row r="36" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -5140,7 +4967,7 @@
     </row>
     <row r="37" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -5154,7 +4981,7 @@
     </row>
     <row r="38" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -5171,7 +4998,7 @@
     </row>
     <row r="39" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -5188,7 +5015,7 @@
     </row>
     <row r="40" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -5205,7 +5032,7 @@
     </row>
     <row r="41" spans="1:14" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -5221,8 +5048,8 @@
       <c r="A42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="77"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="66"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -5352,17 +5179,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="25">
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A27:C27"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A1:C1"/>
@@ -5377,6 +5193,17 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5430,7 +5257,7 @@
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>0</v>
@@ -5443,10 +5270,10 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>37</v>
@@ -5467,7 +5294,7 @@
     </row>
     <row r="5" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>11</v>
@@ -5494,7 +5321,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>2</v>
@@ -5532,7 +5359,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>3</v>
@@ -5544,10 +5371,10 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>60</v>
@@ -5560,7 +5387,7 @@
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>2</v>
@@ -5598,7 +5425,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>4</v>
@@ -5610,7 +5437,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>5</v>
@@ -5626,7 +5453,7 @@
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="37" t="s">
         <v>2</v>
@@ -5634,7 +5461,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>5</v>
@@ -5646,7 +5473,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="35" t="s">
         <v>5</v>
@@ -5668,7 +5495,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>5</v>
@@ -5680,7 +5507,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>7</v>
@@ -5702,7 +5529,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>5</v>
@@ -5718,7 +5545,7 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>10</v>
@@ -5730,10 +5557,10 @@
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -5742,7 +5569,7 @@
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D29" s="35" t="s">
         <v>6</v>
@@ -5774,7 +5601,7 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D32" s="2"/>
     </row>
@@ -5794,7 +5621,7 @@
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D34" s="41" t="s">
         <v>8</v>
@@ -5806,7 +5633,7 @@
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D35" s="41" t="s">
         <v>8</v>
@@ -5818,7 +5645,7 @@
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D36" s="41" t="s">
         <v>1</v>
@@ -5840,7 +5667,7 @@
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D38" s="41" t="s">
         <v>8</v>
@@ -5852,7 +5679,7 @@
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D39" s="41" t="s">
         <v>1</v>
@@ -5864,7 +5691,7 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D40" s="41" t="s">
         <v>1</v>
@@ -5872,13 +5699,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D41" s="41" t="s">
         <v>1</v>
@@ -5888,7 +5715,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <dataValidations count="21">
+  <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28" xr:uid="{12F6FA4A-63A5-4CB5-8A8E-9786EFBCAD13}">
       <formula1>"14 days,30 days,45 days"</formula1>
     </dataValidation>
@@ -5923,7 +5750,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{FC4642AD-5BCE-4079-8C0A-C8352F93C120}">
       <formula1>"TURNKEY,DBB,BOO,BOT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 B20 B21 B23" xr:uid="{8CAC2A28-BA35-4E11-8AA7-6BD3F533C491}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 B20:B21 B23 B26" xr:uid="{8CAC2A28-BA35-4E11-8AA7-6BD3F533C491}">
       <formula1>"GRADE-A,GRADE-B,GRADE-C,GRADE-E"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{CD0A02A6-1365-423F-B7A5-D9C17828AE16}">
@@ -5937,9 +5764,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{C8081261-9B16-4DBC-AC0D-D9172317541C}">
       <formula1>"NO CHALLENGE,NORMAL,DIFFICULT"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26" xr:uid="{B54A9DAA-3985-4EB0-B11F-B60CA49B6AD1}">
-      <formula1>"GRADE-A,GRADE-B,GRADE-C,GRADE-E"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27:B29" xr:uid="{B15FEE10-11C2-4F68-A603-95731D9C520C}">
       <formula1>"BY VALUE,BY GRADE"</formula1>
@@ -5982,317 +5806,322 @@
       <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="71"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="83" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="87" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="88"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="84"/>
+      <c r="C6" s="88"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="86"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="90"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="71"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B23" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="84"/>
+      <c r="C23" s="88"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="84"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="36"/>
       <c r="C31" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B33" s="36"/>
       <c r="C33" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B34" s="36"/>
       <c r="C34" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="90"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="69"/>
-      <c r="C36" s="70"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="71"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>125</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="A36:C36"/>
@@ -6301,11 +6130,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{FA192426-A47F-4375-83D6-14EC0F0BD2BD}">
@@ -6338,8 +6162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAC1C9E-F228-4693-A589-4056EE764A51}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="66" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:C102"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="66" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6351,13 +6175,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>132</v>
@@ -6366,21 +6190,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="43" t="s">
         <v>178</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -6388,7 +6212,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>129</v>
@@ -6398,7 +6222,7 @@
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>129</v>
@@ -6419,7 +6243,7 @@
     </row>
     <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="42" t="s">
         <v>129</v>
@@ -6429,7 +6253,7 @@
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="42" t="s">
         <v>129</v>
@@ -6448,7 +6272,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="42" t="s">
         <v>129</v>
@@ -6458,7 +6282,7 @@
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B12" s="42" t="s">
         <v>129</v>
@@ -6468,7 +6292,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="42" t="s">
         <v>129</v>
@@ -6478,7 +6302,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="42" t="s">
@@ -6488,7 +6312,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>129</v>
@@ -6498,7 +6322,7 @@
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="42" t="s">
@@ -6530,7 +6354,7 @@
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="42" t="s">
@@ -6540,7 +6364,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B20" s="61"/>
       <c r="C20" s="61"/>
@@ -6579,7 +6403,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>129</v>
@@ -6611,7 +6435,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B27" s="45"/>
       <c r="C27" s="42" t="s">
@@ -6621,7 +6445,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B28" s="45"/>
       <c r="C28" s="42" t="s">
@@ -6631,7 +6455,7 @@
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>129</v>
@@ -6641,7 +6465,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>129</v>
@@ -6651,7 +6475,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B31" s="43"/>
       <c r="C31" s="43"/>
@@ -6659,7 +6483,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="42" t="s">
@@ -6669,7 +6493,7 @@
     </row>
     <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B33" s="45"/>
       <c r="C33" s="42" t="s">
@@ -6679,7 +6503,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="42" t="s">
@@ -6689,7 +6513,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>129</v>
@@ -6699,7 +6523,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="42" t="s">
@@ -6709,7 +6533,7 @@
     </row>
     <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" s="45"/>
       <c r="C37" s="42" t="s">
@@ -6719,7 +6543,7 @@
     </row>
     <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="42" t="s">
@@ -6729,7 +6553,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
@@ -6737,7 +6561,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B40" s="45"/>
       <c r="C40" s="42" t="s">
@@ -6747,7 +6571,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" s="43"/>
       <c r="C41" s="43"/>
@@ -6755,7 +6579,7 @@
     </row>
     <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="42" t="s">
@@ -6767,7 +6591,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B43" s="42" t="s">
         <v>129</v>
@@ -6777,7 +6601,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B44" s="47"/>
       <c r="C44" s="42" t="s">
@@ -6787,7 +6611,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B45" s="42" t="s">
         <v>129</v>
@@ -6819,7 +6643,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -6827,7 +6651,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B49" s="45"/>
       <c r="C49" s="42" t="s">
@@ -6848,7 +6672,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B51" s="45"/>
       <c r="C51" s="42" t="s">
@@ -6858,7 +6682,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B52" s="45"/>
       <c r="C52" s="42" t="s">
@@ -6868,7 +6692,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -6876,7 +6700,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B54" s="45"/>
       <c r="C54" s="42" t="s">
@@ -6886,7 +6710,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B55" s="45"/>
       <c r="C55" s="42" t="s">
@@ -6896,7 +6720,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B56" s="45"/>
       <c r="C56" s="42" t="s">
@@ -6906,7 +6730,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B57" s="45"/>
       <c r="C57" s="42" t="s">
@@ -6916,7 +6740,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B58" s="45"/>
       <c r="C58" s="42" t="s">
@@ -6926,7 +6750,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B59" s="45"/>
       <c r="C59" s="42" t="s">
@@ -6936,7 +6760,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B60" s="45"/>
       <c r="C60" s="42" t="s">
@@ -6946,7 +6770,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B61" s="45"/>
       <c r="C61" s="42" t="s">
@@ -6958,7 +6782,7 @@
     </row>
     <row r="62" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B62" s="58"/>
       <c r="C62" s="58"/>
@@ -6973,22 +6797,22 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="63" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="B67" s="63"/>
       <c r="C67" s="63"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="51" t="s">
-        <v>302</v>
-      </c>
-      <c r="B68" s="100" t="str">
+        <v>254</v>
+      </c>
+      <c r="B68" s="91" t="str">
         <f>"td_Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
         <v xml:space="preserve">td_Cost And Freight (CFR) , , </v>
       </c>
-      <c r="C68" s="100"/>
+      <c r="C68" s="91"/>
       <c r="D68" s="53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E68" s="52"/>
       <c r="F68" s="52"/>
@@ -6997,15 +6821,15 @@
       <c r="I68" s="52"/>
     </row>
     <row r="69" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="101" t="s">
+      <c r="A69" s="92" t="s">
+        <v>258</v>
+      </c>
+      <c r="B69" s="93" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="93"/>
+      <c r="D69" s="52" t="s">
         <v>307</v>
-      </c>
-      <c r="B69" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="C69" s="102"/>
-      <c r="D69" s="52" t="s">
-        <v>133</v>
       </c>
       <c r="E69" s="52"/>
       <c r="F69" s="52"/>
@@ -7014,13 +6838,13 @@
       <c r="I69" s="52"/>
     </row>
     <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="101"/>
-      <c r="B70" s="103" t="s">
-        <v>304</v>
-      </c>
-      <c r="C70" s="103"/>
+      <c r="A70" s="92"/>
+      <c r="B70" s="94" t="s">
+        <v>256</v>
+      </c>
+      <c r="C70" s="94"/>
       <c r="D70" s="52" t="s">
-        <v>133</v>
+        <v>308</v>
       </c>
       <c r="E70" s="52"/>
       <c r="F70" s="52"/>
@@ -7029,13 +6853,13 @@
       <c r="I70" s="52"/>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="101"/>
-      <c r="B71" s="103" t="s">
-        <v>305</v>
-      </c>
-      <c r="C71" s="103"/>
+      <c r="A71" s="92"/>
+      <c r="B71" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="C71" s="94"/>
       <c r="D71" s="52" t="s">
-        <v>133</v>
+        <v>309</v>
       </c>
       <c r="E71" s="52"/>
       <c r="F71" s="52"/>
@@ -7044,13 +6868,13 @@
       <c r="I71" s="52"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="101"/>
-      <c r="B72" s="103" t="s">
+      <c r="A72" s="92"/>
+      <c r="B72" s="94" t="s">
         <v>306</v>
       </c>
-      <c r="C72" s="103"/>
+      <c r="C72" s="94"/>
       <c r="D72" s="52" t="s">
-        <v>133</v>
+        <v>310</v>
       </c>
       <c r="E72" s="52"/>
       <c r="F72" s="52"/>
@@ -7060,275 +6884,280 @@
     </row>
     <row r="73" spans="1:12" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="51" t="s">
-        <v>308</v>
-      </c>
-      <c r="B73" s="98" t="str">
+        <v>259</v>
+      </c>
+      <c r="B73" s="96" t="str">
         <f>J73&amp;K73&amp;L73</f>
         <v>td_All invoices are due and payable at the specified payment date or fourteen (14) daysdays after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
       </c>
-      <c r="C73" s="99"/>
+      <c r="C73" s="97"/>
       <c r="D73" s="53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E73" s="52"/>
       <c r="F73" s="52"/>
       <c r="G73" s="52"/>
       <c r="H73" s="52"/>
       <c r="I73" s="52" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="J73" s="64" t="s">
-        <v>309</v>
+        <v>260</v>
       </c>
       <c r="K73" s="64" t="str">
         <f>IF('DIP_Project Information'!D28="14 Days","fourteen (14) days",IF('DIP_Project Information'!D28="30 Days","thirty (30) days",IF('DIP_Project Information'!D28="45 Days","forty-five (45) days","[invalid payment term]")))</f>
         <v>fourteen (14) days</v>
       </c>
       <c r="L73" s="64" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="51" t="s">
-        <v>310</v>
-      </c>
-      <c r="B74" s="91" t="s">
-        <v>312</v>
-      </c>
-      <c r="C74" s="91"/>
+        <v>261</v>
+      </c>
+      <c r="B74" s="98" t="s">
+        <v>263</v>
+      </c>
+      <c r="C74" s="98"/>
     </row>
     <row r="75" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="51" t="s">
-        <v>311</v>
-      </c>
-      <c r="B75" s="91" t="s">
-        <v>313</v>
-      </c>
-      <c r="C75" s="91"/>
+        <v>262</v>
+      </c>
+      <c r="B75" s="98" t="s">
+        <v>264</v>
+      </c>
+      <c r="C75" s="98"/>
     </row>
     <row r="76" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="94" t="s">
-        <v>315</v>
-      </c>
-      <c r="B76" s="93" t="s">
-        <v>314</v>
-      </c>
-      <c r="C76" s="93"/>
+      <c r="A76" s="99" t="s">
+        <v>266</v>
+      </c>
+      <c r="B76" s="100" t="s">
+        <v>265</v>
+      </c>
+      <c r="C76" s="100"/>
     </row>
     <row r="77" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="94"/>
-      <c r="B77" s="97" t="s">
-        <v>316</v>
-      </c>
-      <c r="C77" s="97"/>
+      <c r="A77" s="99"/>
+      <c r="B77" s="95" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" s="95"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="94"/>
-      <c r="B78" s="97" t="s">
-        <v>317</v>
-      </c>
-      <c r="C78" s="97"/>
+      <c r="A78" s="99"/>
+      <c r="B78" s="95" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" s="95"/>
     </row>
     <row r="79" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="94"/>
-      <c r="B79" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="C79" s="97"/>
+      <c r="A79" s="99"/>
+      <c r="B79" s="95" t="s">
+        <v>269</v>
+      </c>
+      <c r="C79" s="95"/>
     </row>
     <row r="80" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="94"/>
-      <c r="B80" s="97" t="s">
-        <v>319</v>
-      </c>
-      <c r="C80" s="97"/>
+      <c r="A80" s="99"/>
+      <c r="B80" s="95" t="s">
+        <v>270</v>
+      </c>
+      <c r="C80" s="95"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="94"/>
-      <c r="B81" s="93" t="s">
-        <v>320</v>
-      </c>
-      <c r="C81" s="93"/>
+      <c r="A81" s="99"/>
+      <c r="B81" s="100" t="s">
+        <v>271</v>
+      </c>
+      <c r="C81" s="100"/>
     </row>
     <row r="82" spans="1:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="94"/>
-      <c r="B82" s="96" t="s">
-        <v>321</v>
-      </c>
-      <c r="C82" s="96"/>
+      <c r="A82" s="99"/>
+      <c r="B82" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" s="101"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="94"/>
-      <c r="B83" s="93" t="s">
-        <v>322</v>
-      </c>
-      <c r="C83" s="93"/>
+      <c r="A83" s="99"/>
+      <c r="B83" s="100" t="s">
+        <v>273</v>
+      </c>
+      <c r="C83" s="100"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="94"/>
-      <c r="B84" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="C84" s="97"/>
+      <c r="A84" s="99"/>
+      <c r="B84" s="95" t="s">
+        <v>274</v>
+      </c>
+      <c r="C84" s="95"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="94"/>
-      <c r="B85" s="97" t="s">
-        <v>324</v>
-      </c>
-      <c r="C85" s="97"/>
+      <c r="A85" s="99"/>
+      <c r="B85" s="95" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="95"/>
     </row>
     <row r="86" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="94"/>
-      <c r="B86" s="97" t="s">
-        <v>325</v>
-      </c>
-      <c r="C86" s="97"/>
+      <c r="A86" s="99"/>
+      <c r="B86" s="95" t="s">
+        <v>276</v>
+      </c>
+      <c r="C86" s="95"/>
     </row>
     <row r="87" spans="1:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="94"/>
-      <c r="B87" s="97" t="s">
-        <v>326</v>
-      </c>
-      <c r="C87" s="97"/>
+      <c r="A87" s="99"/>
+      <c r="B87" s="95" t="s">
+        <v>277</v>
+      </c>
+      <c r="C87" s="95"/>
     </row>
     <row r="88" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="94"/>
-      <c r="B88" s="93" t="s">
-        <v>327</v>
-      </c>
-      <c r="C88" s="93"/>
+      <c r="A88" s="99"/>
+      <c r="B88" s="100" t="s">
+        <v>278</v>
+      </c>
+      <c r="C88" s="100"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="94"/>
-      <c r="B89" s="93" t="s">
-        <v>328</v>
-      </c>
-      <c r="C89" s="93"/>
+      <c r="A89" s="99"/>
+      <c r="B89" s="100" t="s">
+        <v>279</v>
+      </c>
+      <c r="C89" s="100"/>
     </row>
     <row r="90" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="94" t="s">
-        <v>331</v>
-      </c>
-      <c r="B90" s="93" t="s">
-        <v>329</v>
-      </c>
-      <c r="C90" s="93"/>
+      <c r="A90" s="99" t="s">
+        <v>282</v>
+      </c>
+      <c r="B90" s="100" t="s">
+        <v>280</v>
+      </c>
+      <c r="C90" s="100"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="94"/>
-      <c r="B91" s="93" t="s">
-        <v>330</v>
-      </c>
-      <c r="C91" s="93"/>
+      <c r="A91" s="99"/>
+      <c r="B91" s="100" t="s">
+        <v>281</v>
+      </c>
+      <c r="C91" s="100"/>
     </row>
     <row r="92" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="95" t="s">
-        <v>332</v>
-      </c>
-      <c r="B92" s="91" t="s">
-        <v>333</v>
-      </c>
-      <c r="C92" s="91"/>
+      <c r="A92" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="B92" s="98" t="s">
+        <v>284</v>
+      </c>
+      <c r="C92" s="98"/>
     </row>
     <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="95"/>
+      <c r="A93" s="102"/>
       <c r="B93" s="49" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="C93" s="49" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="95"/>
+      <c r="A94" s="102"/>
       <c r="B94" s="49" t="s">
-        <v>344</v>
+        <v>295</v>
       </c>
       <c r="C94" s="50" t="s">
-        <v>349</v>
+        <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="95"/>
+      <c r="A95" s="102"/>
       <c r="B95" s="49" t="s">
-        <v>345</v>
+        <v>296</v>
       </c>
       <c r="C95" s="50" t="s">
-        <v>350</v>
+        <v>301</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="95"/>
+      <c r="A96" s="102"/>
       <c r="B96" s="49" t="s">
-        <v>346</v>
+        <v>297</v>
       </c>
       <c r="C96" s="50" t="s">
-        <v>351</v>
+        <v>302</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="95"/>
+      <c r="A97" s="102"/>
       <c r="B97" s="49" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="C97" s="50" t="s">
-        <v>352</v>
+        <v>303</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="95"/>
+      <c r="A98" s="102"/>
       <c r="B98" s="49" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="C98" s="50" t="s">
-        <v>353</v>
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="51" t="s">
-        <v>335</v>
-      </c>
-      <c r="B99" s="91" t="s">
-        <v>334</v>
-      </c>
-      <c r="C99" s="91"/>
+        <v>286</v>
+      </c>
+      <c r="B99" s="98" t="s">
+        <v>285</v>
+      </c>
+      <c r="C99" s="98"/>
     </row>
     <row r="100" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="51" t="s">
-        <v>336</v>
-      </c>
-      <c r="B100" s="92" t="s">
-        <v>337</v>
-      </c>
-      <c r="C100" s="92"/>
+        <v>287</v>
+      </c>
+      <c r="B100" s="103" t="s">
+        <v>288</v>
+      </c>
+      <c r="C100" s="103"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="51" t="s">
-        <v>338</v>
-      </c>
-      <c r="B101" s="91" t="s">
-        <v>339</v>
-      </c>
-      <c r="C101" s="91"/>
+        <v>289</v>
+      </c>
+      <c r="B101" s="98" t="s">
+        <v>290</v>
+      </c>
+      <c r="C101" s="98"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="51" t="s">
-        <v>340</v>
-      </c>
-      <c r="B102" s="91" t="s">
-        <v>341</v>
-      </c>
-      <c r="C102" s="91"/>
+        <v>291</v>
+      </c>
+      <c r="B102" s="98" t="s">
+        <v>292</v>
+      </c>
+      <c r="C102" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="A92:A98"/>
+    <mergeCell ref="B92:C92"/>
     <mergeCell ref="B87:C87"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
@@ -7345,1050 +7174,18 @@
     <mergeCell ref="B84:C84"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="B86:C86"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A92:A98"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CD6C03-D229-4FF5-A957-B2C9090C939C}">
-  <dimension ref="A1:L102"/>
-  <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
-    <col min="2" max="4" width="40.77734375" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="48"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="59"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
-        <v>205</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="str">
-        <f>"ft_To obtain license to operate " &amp; 'DIP_Project Information'!B3 &amp; " such as SLF (Sertifikat Laik Fungsi)"</f>
-        <v>ft_To obtain license to operate WRP such as SLF (Sertifikat Laik Fungsi)</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-    </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="str">
-        <f>"ftg_Civil and Structural Works – " &amp; 'DIP_Project Information'!B3 &amp; " System"</f>
-        <v>ftg_Civil and Structural Works – WRP System</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
-        <v>209</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
-        <v>210</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="46"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
-        <v>213</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="45"/>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="str">
-        <f>"ft_Design and drawing for " &amp; 'DIP_Project Information'!B3 &amp; " concrete tank, pump/blower room, control room, chemical room "</f>
-        <v xml:space="preserve">ft_Design and drawing for WRP concrete tank, pump/blower room, control room, chemical room </v>
-      </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="45"/>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="str">
-        <f>"ft_Foundation for " &amp; 'DIP_Project Information'!B3 &amp; " containerized tank, pump/blower room, control room, chemical room"</f>
-        <v>ft_Foundation for WRP containerized tank, pump/blower room, control room, chemical room</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="45"/>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="45"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="60" t="s">
-        <v>247</v>
-      </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="str">
-        <f>"ftg_Mechanical and Piping – "&amp;'DIP_Project Information'!B3&amp; " System"</f>
-        <v>ftg_Mechanical and Piping – WRP System</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="str">
-        <f>"ft_Supply and installation of all mechanical material for " &amp; 'DIP_Project Information'!B3 &amp; " system"</f>
-        <v>ft_Supply and installation of all mechanical material for WRP system</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="45"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="str">
-        <f>"ft_Design, testing and commissioning of "&amp;'DIP_Project Information'!B3&amp;"  system"</f>
-        <v>ft_Design, testing and commissioning of WRP  system</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="45"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="46" t="str">
-        <f>"ft_Inlet wastewater transfer piping to " &amp; 'DIP_Project Information'!B3 &amp; " System"</f>
-        <v>ft_Inlet wastewater transfer piping to WRP System</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="46" t="str">
-        <f>"ft_Piping &amp; final system for effluent "&amp;'DIP_Project Information'!B3&amp;" to discharge"</f>
-        <v>ft_Piping &amp; final system for effluent WRP to discharge</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="46"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="45"/>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="45"/>
-    </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" s="45"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="46"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="46"/>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="45"/>
-    </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="45"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="44"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="46"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="44" t="s">
-        <v>244</v>
-      </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="44"/>
-    </row>
-    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="46" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="46"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D44" s="46"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="B45" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-    </row>
-    <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="46" t="str">
-        <f>"ft_Analyze the parameters (for " &amp; 'DIP_Project Information'!B3 &amp; " system) as per regulation during the commissioning by the internal laboratory (the contractor)"</f>
-        <v>ft_Analyze the parameters (for WRP system) as per regulation during the commissioning by the internal laboratory (the contractor)</v>
-      </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D46" s="45"/>
-    </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="46" t="str">
-        <f>"ft_Analyze the parameters (for " &amp; 'DIP_Project Information'!B3 &amp; " system) as per regulation at the end of the commissioning by the external laboratory"</f>
-        <v>ft_Analyze the parameters (for WRP system) as per regulation at the end of the commissioning by the external laboratory</v>
-      </c>
-      <c r="B47" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="44"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="46" t="s">
-        <v>231</v>
-      </c>
-      <c r="B49" s="45"/>
-      <c r="C49" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D49" s="46"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="46" t="str">
-        <f>"ft_Classroom/ Virtual training for " &amp; 'DIP_Project Information'!B3 &amp; " operation"</f>
-        <v>ft_Classroom/ Virtual training for WRP operation</v>
-      </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D50" s="45"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="46"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="46"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="44" t="s">
-        <v>246</v>
-      </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="44"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D54" s="46"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D55" s="46"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D56" s="46"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="B57" s="45"/>
-      <c r="C57" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D57" s="46"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="46" t="s">
-        <v>238</v>
-      </c>
-      <c r="B58" s="45"/>
-      <c r="C58" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D58" s="46"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="B59" s="45"/>
-      <c r="C59" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="46"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="B60" s="45"/>
-      <c r="C60" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D60" s="46"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="B61" s="45"/>
-      <c r="C61" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="58" t="s">
-        <v>248</v>
-      </c>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="63" t="s">
-        <v>280</v>
-      </c>
-      <c r="B67" s="63"/>
-      <c r="C67" s="63"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="B68" s="100" t="str">
-        <f>"Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
-        <v xml:space="preserve">Cost And Freight (CFR) , , </v>
-      </c>
-      <c r="C68" s="100"/>
-      <c r="D68" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="52"/>
-      <c r="H68" s="52"/>
-      <c r="I68" s="52"/>
-    </row>
-    <row r="69" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="101" t="s">
-        <v>297</v>
-      </c>
-      <c r="B69" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="C69" s="102"/>
-      <c r="D69" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E69" s="52"/>
-      <c r="F69" s="52"/>
-      <c r="G69" s="52"/>
-      <c r="H69" s="52"/>
-      <c r="I69" s="52"/>
-    </row>
-    <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="101"/>
-      <c r="B70" s="103" t="s">
-        <v>287</v>
-      </c>
-      <c r="C70" s="103"/>
-      <c r="D70" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E70" s="52"/>
-      <c r="F70" s="52"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
-      <c r="I70" s="52"/>
-    </row>
-    <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="101"/>
-      <c r="B71" s="103" t="s">
-        <v>282</v>
-      </c>
-      <c r="C71" s="103"/>
-      <c r="D71" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E71" s="52"/>
-      <c r="F71" s="52"/>
-      <c r="G71" s="52"/>
-      <c r="H71" s="52"/>
-      <c r="I71" s="52"/>
-    </row>
-    <row r="72" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="101"/>
-      <c r="B72" s="103" t="s">
-        <v>283</v>
-      </c>
-      <c r="C72" s="103"/>
-      <c r="D72" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E72" s="52"/>
-      <c r="F72" s="52"/>
-      <c r="G72" s="52"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="52"/>
-    </row>
-    <row r="73" spans="1:12" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="51" t="s">
-        <v>289</v>
-      </c>
-      <c r="B73" s="98" t="str">
-        <f>J73&amp;K73&amp;L73</f>
-        <v>All invoices are due and payable at the specified payment date or fourteen (14) daysdays after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
-      </c>
-      <c r="C73" s="99"/>
-      <c r="D73" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="52" t="s">
-        <v>286</v>
-      </c>
-      <c r="J73" s="64" t="s">
-        <v>284</v>
-      </c>
-      <c r="K73" s="64" t="str">
-        <f>IF('DIP_Project Information'!D28="14 Days","fourteen (14) days",IF('DIP_Project Information'!D28="30 Days","thirty (30) days",IF('DIP_Project Information'!D28="45 Days","forty-five (45) days","[invalid payment term]")))</f>
-        <v>fourteen (14) days</v>
-      </c>
-      <c r="L73" s="64" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="51" t="s">
-        <v>290</v>
-      </c>
-      <c r="B74" s="91" t="s">
-        <v>249</v>
-      </c>
-      <c r="C74" s="91"/>
-    </row>
-    <row r="75" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="51" t="s">
-        <v>291</v>
-      </c>
-      <c r="B75" s="91" t="s">
-        <v>250</v>
-      </c>
-      <c r="C75" s="91"/>
-    </row>
-    <row r="76" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="94" t="s">
-        <v>298</v>
-      </c>
-      <c r="B76" s="93" t="s">
-        <v>251</v>
-      </c>
-      <c r="C76" s="93"/>
-    </row>
-    <row r="77" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="94"/>
-      <c r="B77" s="97" t="s">
-        <v>252</v>
-      </c>
-      <c r="C77" s="97"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="94"/>
-      <c r="B78" s="97" t="s">
-        <v>253</v>
-      </c>
-      <c r="C78" s="97"/>
-    </row>
-    <row r="79" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="94"/>
-      <c r="B79" s="97" t="s">
-        <v>254</v>
-      </c>
-      <c r="C79" s="97"/>
-    </row>
-    <row r="80" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="94"/>
-      <c r="B80" s="97" t="s">
-        <v>255</v>
-      </c>
-      <c r="C80" s="97"/>
-    </row>
-    <row r="81" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="94"/>
-      <c r="B81" s="93" t="s">
-        <v>256</v>
-      </c>
-      <c r="C81" s="93"/>
-    </row>
-    <row r="82" spans="1:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="94"/>
-      <c r="B82" s="96" t="s">
-        <v>257</v>
-      </c>
-      <c r="C82" s="96"/>
-    </row>
-    <row r="83" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="94"/>
-      <c r="B83" s="93" t="s">
-        <v>258</v>
-      </c>
-      <c r="C83" s="93"/>
-    </row>
-    <row r="84" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="94"/>
-      <c r="B84" s="97" t="s">
-        <v>259</v>
-      </c>
-      <c r="C84" s="97"/>
-    </row>
-    <row r="85" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="94"/>
-      <c r="B85" s="97" t="s">
-        <v>260</v>
-      </c>
-      <c r="C85" s="97"/>
-    </row>
-    <row r="86" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="94"/>
-      <c r="B86" s="97" t="s">
-        <v>261</v>
-      </c>
-      <c r="C86" s="97"/>
-    </row>
-    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="94"/>
-      <c r="B87" s="97" t="s">
-        <v>262</v>
-      </c>
-      <c r="C87" s="97"/>
-    </row>
-    <row r="88" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="94"/>
-      <c r="B88" s="93" t="s">
-        <v>263</v>
-      </c>
-      <c r="C88" s="93"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="94"/>
-      <c r="B89" s="93" t="s">
-        <v>264</v>
-      </c>
-      <c r="C89" s="93"/>
-    </row>
-    <row r="90" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="94" t="s">
-        <v>292</v>
-      </c>
-      <c r="B90" s="93" t="s">
-        <v>265</v>
-      </c>
-      <c r="C90" s="93"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="94"/>
-      <c r="B91" s="93" t="s">
-        <v>266</v>
-      </c>
-      <c r="C91" s="93"/>
-    </row>
-    <row r="92" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="95" t="s">
-        <v>299</v>
-      </c>
-      <c r="B92" s="91" t="s">
-        <v>267</v>
-      </c>
-      <c r="C92" s="91"/>
-    </row>
-    <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="95"/>
-      <c r="B93" s="49" t="s">
-        <v>268</v>
-      </c>
-      <c r="C93" s="49" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="95"/>
-      <c r="B94" s="49" t="s">
-        <v>270</v>
-      </c>
-      <c r="C94" s="50">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="95"/>
-      <c r="B95" s="49" t="s">
-        <v>271</v>
-      </c>
-      <c r="C95" s="50">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="95"/>
-      <c r="B96" s="49" t="s">
-        <v>272</v>
-      </c>
-      <c r="C96" s="50">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="95"/>
-      <c r="B97" s="49" t="s">
-        <v>273</v>
-      </c>
-      <c r="C97" s="50">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="95"/>
-      <c r="B98" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="C98" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="51" t="s">
-        <v>293</v>
-      </c>
-      <c r="B99" s="91" t="s">
-        <v>275</v>
-      </c>
-      <c r="C99" s="91"/>
-    </row>
-    <row r="100" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="51" t="s">
-        <v>294</v>
-      </c>
-      <c r="B100" s="91" t="s">
-        <v>276</v>
-      </c>
-      <c r="C100" s="91"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="51" t="s">
-        <v>295</v>
-      </c>
-      <c r="B101" s="91" t="s">
-        <v>277</v>
-      </c>
-      <c r="C101" s="91"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="51" t="s">
-        <v>296</v>
-      </c>
-      <c r="B102" s="91" t="s">
-        <v>278</v>
-      </c>
-      <c r="C102" s="91"/>
-    </row>
-  </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="A92:A98"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A76:A89"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1305BB-68D9-4D6E-9874-0A1B1E944B39}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -8405,7 +7202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B9172C-440A-42C4-9985-52EF90EECB70}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -8422,7 +7219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE1A81-9577-4E45-8F93-A27BE321C913}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -8437,4 +7234,44 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4B5FA4-65EE-45F5-B4AD-337850B5CC81}">
+  <dimension ref="B2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: save data unique
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -1802,7 +1802,11 @@
           <t>f_Company Name</t>
         </is>
       </c>
-      <c r="B4" s="62" t="inlineStr"/>
+      <c r="B4" s="62" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
       <c r="C4" s="55" t="n"/>
       <c r="D4" s="4" t="n"/>
       <c r="E4" s="4" t="n"/>
@@ -1823,7 +1827,7 @@
       </c>
       <c r="B5" s="59" t="inlineStr">
         <is>
-          <t>Non Food Industry-B</t>
+          <t>Mining</t>
         </is>
       </c>
       <c r="C5" s="55" t="n"/>
@@ -1846,7 +1850,7 @@
       </c>
       <c r="B6" s="59" t="inlineStr">
         <is>
-          <t>Tourism &amp; Hospitality</t>
+          <t>Nickel Mining</t>
         </is>
       </c>
       <c r="C6" s="55" t="n"/>
@@ -1886,7 +1890,11 @@
           <t>f_1Country</t>
         </is>
       </c>
-      <c r="B8" s="56" t="n"/>
+      <c r="B8" s="56" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
       <c r="C8" s="55" t="n"/>
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
@@ -1902,7 +1910,11 @@
           <t>f_1Province</t>
         </is>
       </c>
-      <c r="B9" s="56" t="n"/>
+      <c r="B9" s="56" t="inlineStr">
+        <is>
+          <t>Test3</t>
+        </is>
+      </c>
       <c r="C9" s="55" t="n"/>
       <c r="H9" s="1" t="n"/>
       <c r="I9" s="1" t="n"/>
@@ -1918,7 +1930,11 @@
           <t xml:space="preserve">f_1City </t>
         </is>
       </c>
-      <c r="B10" s="56" t="n"/>
+      <c r="B10" s="56" t="inlineStr">
+        <is>
+          <t>Test4</t>
+        </is>
+      </c>
       <c r="C10" s="55" t="n"/>
       <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n"/>
@@ -1934,7 +1950,11 @@
           <t>f_1Site Address</t>
         </is>
       </c>
-      <c r="B11" s="56" t="n"/>
+      <c r="B11" s="56" t="inlineStr">
+        <is>
+          <t>Test5</t>
+        </is>
+      </c>
       <c r="C11" s="55" t="n"/>
       <c r="D11" s="4" t="n"/>
       <c r="E11" s="4" t="n"/>
@@ -1953,7 +1973,11 @@
           <t>f_1Correspondence Address</t>
         </is>
       </c>
-      <c r="B12" s="57" t="n"/>
+      <c r="B12" s="57" t="inlineStr">
+        <is>
+          <t>Test6</t>
+        </is>
+      </c>
       <c r="C12" s="55" t="n"/>
       <c r="D12" s="4" t="n"/>
       <c r="E12" s="4" t="n"/>
@@ -1972,7 +1996,11 @@
           <t xml:space="preserve">f_1Postal Code </t>
         </is>
       </c>
-      <c r="B13" s="56" t="n"/>
+      <c r="B13" s="56" t="inlineStr">
+        <is>
+          <t>Test7</t>
+        </is>
+      </c>
       <c r="C13" s="55" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
@@ -2033,12 +2061,12 @@
       </c>
       <c r="B16" s="56" t="inlineStr">
         <is>
-          <t>PIC1</t>
+          <t>Test8</t>
         </is>
       </c>
       <c r="C16" s="56" t="inlineStr">
         <is>
-          <t>PIC2</t>
+          <t>Test9</t>
         </is>
       </c>
       <c r="D16" s="19" t="n"/>
@@ -2058,8 +2086,16 @@
           <t xml:space="preserve">fm_1Decision Maker </t>
         </is>
       </c>
-      <c r="B17" s="56" t="inlineStr"/>
-      <c r="C17" s="56" t="inlineStr"/>
+      <c r="B17" s="56" t="inlineStr">
+        <is>
+          <t>Test10</t>
+        </is>
+      </c>
+      <c r="C17" s="56" t="inlineStr">
+        <is>
+          <t>Test11</t>
+        </is>
+      </c>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
@@ -2074,8 +2110,16 @@
           <t>fm_1Influencer</t>
         </is>
       </c>
-      <c r="B18" s="56" t="inlineStr"/>
-      <c r="C18" s="56" t="inlineStr"/>
+      <c r="B18" s="56" t="inlineStr">
+        <is>
+          <t>Test12</t>
+        </is>
+      </c>
+      <c r="C18" s="56" t="inlineStr">
+        <is>
+          <t>Test13</t>
+        </is>
+      </c>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
       <c r="J18" s="1" t="n"/>
@@ -2090,8 +2134,16 @@
           <t xml:space="preserve">fm_1#1 Engineering Person </t>
         </is>
       </c>
-      <c r="B19" s="56" t="inlineStr"/>
-      <c r="C19" s="56" t="inlineStr"/>
+      <c r="B19" s="56" t="inlineStr">
+        <is>
+          <t>Test14</t>
+        </is>
+      </c>
+      <c r="C19" s="56" t="inlineStr">
+        <is>
+          <t>Test15</t>
+        </is>
+      </c>
       <c r="D19" s="4" t="n"/>
       <c r="E19" s="4" t="n"/>
       <c r="F19" s="4" t="n"/>
@@ -2109,8 +2161,16 @@
           <t>fm_1#2 Enginering Person</t>
         </is>
       </c>
-      <c r="B20" s="56" t="inlineStr"/>
-      <c r="C20" s="56" t="inlineStr"/>
+      <c r="B20" s="56" t="inlineStr">
+        <is>
+          <t>Test16</t>
+        </is>
+      </c>
+      <c r="C20" s="56" t="inlineStr">
+        <is>
+          <t>Test17</t>
+        </is>
+      </c>
       <c r="D20" s="4" t="n"/>
       <c r="E20" s="4" t="n"/>
       <c r="F20" s="4" t="n"/>
@@ -2128,8 +2188,16 @@
           <t>fm_1#3 Commercial Person</t>
         </is>
       </c>
-      <c r="B21" s="56" t="inlineStr"/>
-      <c r="C21" s="56" t="inlineStr"/>
+      <c r="B21" s="56" t="inlineStr">
+        <is>
+          <t>Test18</t>
+        </is>
+      </c>
+      <c r="C21" s="56" t="inlineStr">
+        <is>
+          <t>Test19</t>
+        </is>
+      </c>
       <c r="D21" s="4" t="n"/>
       <c r="E21" s="4" t="n"/>
       <c r="F21" s="4" t="n"/>
@@ -2147,8 +2215,16 @@
           <t>fm_1#4 Commercial Person</t>
         </is>
       </c>
-      <c r="B22" s="56" t="inlineStr"/>
-      <c r="C22" s="56" t="inlineStr"/>
+      <c r="B22" s="56" t="inlineStr">
+        <is>
+          <t>Test20</t>
+        </is>
+      </c>
+      <c r="C22" s="56" t="inlineStr">
+        <is>
+          <t>Test21</t>
+        </is>
+      </c>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
       <c r="J22" s="1" t="n"/>
@@ -2163,8 +2239,16 @@
           <t>fm_Company Correspondence (Admin)</t>
         </is>
       </c>
-      <c r="B23" s="56" t="inlineStr"/>
-      <c r="C23" s="56" t="inlineStr"/>
+      <c r="B23" s="56" t="inlineStr">
+        <is>
+          <t>Test22</t>
+        </is>
+      </c>
+      <c r="C23" s="56" t="inlineStr">
+        <is>
+          <t>Test23</t>
+        </is>
+      </c>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
       <c r="J23" s="1" t="n"/>
@@ -2179,7 +2263,11 @@
           <t>f_1Company Email</t>
         </is>
       </c>
-      <c r="B24" s="58" t="n"/>
+      <c r="B24" s="58" t="inlineStr">
+        <is>
+          <t>Test24</t>
+        </is>
+      </c>
       <c r="C24" s="55" t="n"/>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
@@ -2214,7 +2302,11 @@
           <t>f_Project Owner</t>
         </is>
       </c>
-      <c r="B26" s="62" t="inlineStr"/>
+      <c r="B26" s="62" t="inlineStr">
+        <is>
+          <t>Test25</t>
+        </is>
+      </c>
       <c r="C26" s="55" t="n"/>
       <c r="D26" s="4" t="n"/>
       <c r="E26" s="4" t="n"/>
@@ -2252,7 +2344,11 @@
           <t xml:space="preserve">f_2Country </t>
         </is>
       </c>
-      <c r="B28" s="56" t="n"/>
+      <c r="B28" s="56" t="inlineStr">
+        <is>
+          <t>Test26</t>
+        </is>
+      </c>
       <c r="C28" s="55" t="n"/>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
@@ -2268,7 +2364,11 @@
           <t>f_2Province</t>
         </is>
       </c>
-      <c r="B29" s="56" t="n"/>
+      <c r="B29" s="56" t="inlineStr">
+        <is>
+          <t>Test27</t>
+        </is>
+      </c>
       <c r="C29" s="55" t="n"/>
       <c r="H29" s="1" t="n"/>
       <c r="I29" s="1" t="n"/>
@@ -2284,7 +2384,11 @@
           <t xml:space="preserve">f_2City </t>
         </is>
       </c>
-      <c r="B30" s="56" t="n"/>
+      <c r="B30" s="56" t="inlineStr">
+        <is>
+          <t>Test28</t>
+        </is>
+      </c>
       <c r="C30" s="55" t="n"/>
       <c r="H30" s="1" t="n"/>
       <c r="I30" s="1" t="n"/>
@@ -2300,7 +2404,11 @@
           <t>f_2Site Address</t>
         </is>
       </c>
-      <c r="B31" s="56" t="n"/>
+      <c r="B31" s="56" t="inlineStr">
+        <is>
+          <t>Test29</t>
+        </is>
+      </c>
       <c r="C31" s="55" t="n"/>
       <c r="D31" s="4" t="n"/>
       <c r="E31" s="4" t="n"/>
@@ -2319,7 +2427,11 @@
           <t>f_2Correspondence Address</t>
         </is>
       </c>
-      <c r="B32" s="57" t="n"/>
+      <c r="B32" s="57" t="inlineStr">
+        <is>
+          <t>Test30</t>
+        </is>
+      </c>
       <c r="C32" s="55" t="n"/>
       <c r="D32" s="4" t="n"/>
       <c r="E32" s="4" t="n"/>
@@ -2338,7 +2450,11 @@
           <t xml:space="preserve">f_2Postal Code </t>
         </is>
       </c>
-      <c r="B33" s="56" t="n"/>
+      <c r="B33" s="56" t="inlineStr">
+        <is>
+          <t>Test31</t>
+        </is>
+      </c>
       <c r="C33" s="55" t="n"/>
       <c r="H33" s="1" t="n"/>
       <c r="I33" s="1" t="n"/>
@@ -2376,12 +2492,12 @@
       </c>
       <c r="B35" s="56" t="inlineStr">
         <is>
-          <t>PIC3</t>
+          <t>Test32</t>
         </is>
       </c>
       <c r="C35" s="56" t="inlineStr">
         <is>
-          <t>PIC4</t>
+          <t>Test33</t>
         </is>
       </c>
       <c r="D35" s="19" t="n"/>
@@ -2401,8 +2517,16 @@
           <t xml:space="preserve">fm_2Decision Maker </t>
         </is>
       </c>
-      <c r="B36" s="56" t="inlineStr"/>
-      <c r="C36" s="56" t="inlineStr"/>
+      <c r="B36" s="56" t="inlineStr">
+        <is>
+          <t>Test34</t>
+        </is>
+      </c>
+      <c r="C36" s="56" t="inlineStr">
+        <is>
+          <t>Test35</t>
+        </is>
+      </c>
       <c r="H36" s="1" t="n"/>
       <c r="I36" s="1" t="n"/>
       <c r="J36" s="1" t="n"/>
@@ -2417,8 +2541,16 @@
           <t>fm_2Influencer</t>
         </is>
       </c>
-      <c r="B37" s="56" t="inlineStr"/>
-      <c r="C37" s="56" t="inlineStr"/>
+      <c r="B37" s="56" t="inlineStr">
+        <is>
+          <t>Test36</t>
+        </is>
+      </c>
+      <c r="C37" s="56" t="inlineStr">
+        <is>
+          <t>Test37</t>
+        </is>
+      </c>
       <c r="H37" s="1" t="n"/>
       <c r="I37" s="1" t="n"/>
       <c r="J37" s="1" t="n"/>
@@ -2433,8 +2565,16 @@
           <t xml:space="preserve">fm_2#1 Engineering Person </t>
         </is>
       </c>
-      <c r="B38" s="56" t="inlineStr"/>
-      <c r="C38" s="56" t="inlineStr"/>
+      <c r="B38" s="56" t="inlineStr">
+        <is>
+          <t>Test38</t>
+        </is>
+      </c>
+      <c r="C38" s="56" t="inlineStr">
+        <is>
+          <t>Test39</t>
+        </is>
+      </c>
       <c r="D38" s="4" t="n"/>
       <c r="E38" s="4" t="n"/>
       <c r="F38" s="4" t="n"/>
@@ -2452,8 +2592,16 @@
           <t>fm_2#2 Enginering Person</t>
         </is>
       </c>
-      <c r="B39" s="56" t="inlineStr"/>
-      <c r="C39" s="56" t="inlineStr"/>
+      <c r="B39" s="56" t="inlineStr">
+        <is>
+          <t>Test40</t>
+        </is>
+      </c>
+      <c r="C39" s="56" t="inlineStr">
+        <is>
+          <t>Test41</t>
+        </is>
+      </c>
       <c r="D39" s="4" t="n"/>
       <c r="E39" s="4" t="n"/>
       <c r="F39" s="4" t="n"/>
@@ -2471,8 +2619,16 @@
           <t>fm_2#3 Commercial Person</t>
         </is>
       </c>
-      <c r="B40" s="56" t="inlineStr"/>
-      <c r="C40" s="56" t="inlineStr"/>
+      <c r="B40" s="56" t="inlineStr">
+        <is>
+          <t>Test42</t>
+        </is>
+      </c>
+      <c r="C40" s="56" t="inlineStr">
+        <is>
+          <t>Test43</t>
+        </is>
+      </c>
       <c r="D40" s="4" t="n"/>
       <c r="E40" s="4" t="n"/>
       <c r="F40" s="4" t="n"/>
@@ -2490,8 +2646,16 @@
           <t>fm_2#4 Commercial Person</t>
         </is>
       </c>
-      <c r="B41" s="56" t="inlineStr"/>
-      <c r="C41" s="56" t="inlineStr"/>
+      <c r="B41" s="56" t="inlineStr">
+        <is>
+          <t>Test44</t>
+        </is>
+      </c>
+      <c r="C41" s="56" t="inlineStr">
+        <is>
+          <t>Test45</t>
+        </is>
+      </c>
       <c r="H41" s="1" t="n"/>
       <c r="I41" s="1" t="n"/>
       <c r="J41" s="1" t="n"/>
@@ -2506,7 +2670,11 @@
           <t>f_2Company Email</t>
         </is>
       </c>
-      <c r="B42" s="58" t="n"/>
+      <c r="B42" s="58" t="inlineStr">
+        <is>
+          <t>Test46</t>
+        </is>
+      </c>
       <c r="C42" s="55" t="n"/>
       <c r="H42" s="1" t="n"/>
       <c r="I42" s="1" t="n"/>

</xml_diff>

<commit_message>
fix: quotation and user code
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C126A1E-FBFC-448F-9E95-8BC28036865F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4E9A7A-EC80-4D0F-B8F7-D13803A88C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" tabRatio="687" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP_Customer Information" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="Technical Information" sheetId="3" r:id="rId3"/>
     <sheet name="DIP_Data Input" sheetId="4" r:id="rId4"/>
     <sheet name="User Code" sheetId="10" r:id="rId5"/>
-    <sheet name="DATA_PROPOSAL" sheetId="5" r:id="rId6"/>
-    <sheet name="DATA_OPEX" sheetId="6" r:id="rId7"/>
-    <sheet name="DATA_BOQ" sheetId="7" r:id="rId8"/>
-    <sheet name="DATA_TEMP" sheetId="8" r:id="rId9"/>
-    <sheet name="DATA_ELI" sheetId="9" r:id="rId10"/>
+    <sheet name="No of Quotation" sheetId="11" r:id="rId6"/>
+    <sheet name="DATA_PROPOSAL" sheetId="5" r:id="rId7"/>
+    <sheet name="DATA_OPEX" sheetId="6" r:id="rId8"/>
+    <sheet name="DATA_BOQ" sheetId="7" r:id="rId9"/>
+    <sheet name="DATA_TEMP" sheetId="8" r:id="rId10"/>
+    <sheet name="DATA_ELI" sheetId="9" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="_12.ABUTHMEN">#REF!</definedName>
@@ -188,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="389">
   <si>
     <t>sub_CUSTOMER INFORMATION</t>
   </si>
@@ -1281,6 +1282,99 @@
   <si>
     <t xml:space="preserve"> after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</t>
   </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Initial Company Name</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>Document Type</t>
+  </si>
+  <si>
+    <t>Release Date</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Quotation No.</t>
+  </si>
+  <si>
+    <t>PT SD Guthrie International Sei Mangkei Refinery</t>
+  </si>
+  <si>
+    <t>SDGI</t>
+  </si>
+  <si>
+    <t>WWTP</t>
+  </si>
+  <si>
+    <t>CTP</t>
+  </si>
+  <si>
+    <t>001/09/CTP/WWTP/SDGI/2024</t>
+  </si>
+  <si>
+    <t>PT Perfetti Van Melle Indonesia</t>
+  </si>
+  <si>
+    <t>PVMI</t>
+  </si>
+  <si>
+    <t>001/11/CTP/WWTP/PVMI/2024</t>
+  </si>
+  <si>
+    <t>PT Bumi Menara Internusa</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>WRP-BOO</t>
+  </si>
+  <si>
+    <t>001/10/CTP/WRP-BOO/BMI/2024</t>
+  </si>
+  <si>
+    <t>PT Mulia Boga Raya</t>
+  </si>
+  <si>
+    <t>MBR</t>
+  </si>
+  <si>
+    <t>001/01/CTP/WWTP/MBR/2025</t>
+  </si>
+  <si>
+    <t>PT Leighton Contractors Indonesia</t>
+  </si>
+  <si>
+    <t>LCI</t>
+  </si>
+  <si>
+    <t>Cr6+</t>
+  </si>
+  <si>
+    <t>001/02/CTP/Cr6+/LCI/2025</t>
+  </si>
+  <si>
+    <t>PT Coba Jaya</t>
+  </si>
+  <si>
+    <t>PCJ</t>
+  </si>
+  <si>
+    <t>001/02/CTP/Cr6+/PCJ/2025</t>
+  </si>
 </sst>
 </file>
 
@@ -1293,7 +1387,7 @@
     <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1409,6 +1503,17 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1596,7 +1701,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1767,6 +1872,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2966,18 +3086,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -2990,11 +3110,11 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="65"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
@@ -3010,8 +3130,8 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="65"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3027,8 +3147,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -3044,8 +3164,8 @@
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3058,11 +3178,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="65"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3078,8 +3198,8 @@
       <c r="A8" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="65"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3092,8 +3212,8 @@
       <c r="A9" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3106,8 +3226,8 @@
       <c r="A10" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="65"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3120,8 +3240,8 @@
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="65"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3137,8 +3257,8 @@
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="65"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3154,8 +3274,8 @@
       <c r="A13" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="65"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="70"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3165,11 +3285,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="70"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3327,8 +3447,8 @@
       <c r="A24" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="70"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3338,11 +3458,11 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="65"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -3358,8 +3478,8 @@
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="65"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="70"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -3372,11 +3492,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="65"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="70"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3392,8 +3512,8 @@
       <c r="A28" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="65"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="70"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3406,8 +3526,8 @@
       <c r="A29" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="65"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3420,8 +3540,8 @@
       <c r="A30" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="65"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3434,8 +3554,8 @@
       <c r="A31" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="65"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="70"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -3451,8 +3571,8 @@
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="65"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="70"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3468,8 +3588,8 @@
       <c r="A33" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="65"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="70"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -3606,8 +3726,8 @@
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="65"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="70"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3617,11 +3737,11 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="71" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="67"/>
-      <c r="C43" s="65"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="70"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3634,8 +3754,8 @@
       <c r="A44" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="70"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3648,8 +3768,8 @@
       <c r="A45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="64"/>
-      <c r="C45" s="65"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="70"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -3662,15 +3782,15 @@
       <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="64"/>
-      <c r="C46" s="65"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="70"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="64"/>
-      <c r="C47" s="65"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="70"/>
     </row>
     <row r="48" spans="1:14" ht="13.2" customHeight="1">
       <c r="H48" s="1"/>
@@ -3728,6 +3848,165 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="63" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="62"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="100" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="70"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="100" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="72"/>
+      <c r="C10" s="70"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="99" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="53"/>
+      <c r="C14" s="52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="52" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -3786,12 +4065,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -4175,18 +4454,18 @@
       <c r="D39" s="27"/>
     </row>
     <row r="40" spans="1:4" ht="15.6">
-      <c r="A40" s="79" t="s">
+      <c r="A40" s="84" t="s">
         <v>268</v>
       </c>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="65"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="70"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="6" t="s">
@@ -4210,39 +4489,39 @@
       <c r="A44" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="70"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="65"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="70"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="77" t="e">
+      <c r="B46" s="82" t="e">
         <f>B50/B49</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C46" s="65"/>
+      <c r="C46" s="70"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="78"/>
-      <c r="C47" s="65"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="70"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="65"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="70"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
@@ -4338,8 +4617,8 @@
       <c r="A59" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B59" s="77"/>
-      <c r="C59" s="65"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="70"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="6" t="s">
@@ -4351,25 +4630,25 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="67"/>
-      <c r="C61" s="65"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="70"/>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="65"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="70"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="76"/>
-      <c r="C63" s="65"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="70"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="6" t="s">
@@ -4465,15 +4744,15 @@
       <c r="A74" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="77"/>
-      <c r="C74" s="65"/>
+      <c r="B74" s="82"/>
+      <c r="C74" s="70"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="66" t="s">
+      <c r="A75" s="71" t="s">
         <v>309</v>
       </c>
-      <c r="B75" s="67"/>
-      <c r="C75" s="65"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="70"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
@@ -4485,74 +4764,74 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="66" t="s">
+      <c r="A77" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="67"/>
-      <c r="C77" s="65"/>
+      <c r="B77" s="72"/>
+      <c r="C77" s="70"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B78" s="75"/>
-      <c r="C78" s="65"/>
+      <c r="B78" s="80"/>
+      <c r="C78" s="70"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B79" s="75"/>
-      <c r="C79" s="65"/>
+      <c r="B79" s="80"/>
+      <c r="C79" s="70"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B80" s="75"/>
-      <c r="C80" s="65"/>
+      <c r="B80" s="80"/>
+      <c r="C80" s="70"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B81" s="75"/>
-      <c r="C81" s="65"/>
+      <c r="B81" s="80"/>
+      <c r="C81" s="70"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B82" s="75"/>
-      <c r="C82" s="65"/>
+      <c r="B82" s="80"/>
+      <c r="C82" s="70"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B83" s="75"/>
-      <c r="C83" s="65"/>
+      <c r="B83" s="80"/>
+      <c r="C83" s="70"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B84" s="75"/>
-      <c r="C84" s="65"/>
+      <c r="B84" s="80"/>
+      <c r="C84" s="70"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B85" s="75"/>
-      <c r="C85" s="65"/>
+      <c r="B85" s="80"/>
+      <c r="C85" s="70"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B86" s="75"/>
-      <c r="C86" s="65"/>
+      <c r="B86" s="80"/>
+      <c r="C86" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -4680,18 +4959,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
@@ -4715,36 +4994,36 @@
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="65"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="70"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="70"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="65"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="70"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="65"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="70"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="65"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="70"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
@@ -4849,8 +5128,8 @@
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="65"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="70"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
@@ -4862,25 +5141,25 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="65"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="70"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="70"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="65"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
@@ -4994,15 +5273,15 @@
       <c r="A38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="65"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="70"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="65"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="70"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
@@ -5014,74 +5293,74 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="65"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="70"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="65"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="70"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="65"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="70"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="70"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="65"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="70"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="75"/>
-      <c r="C46" s="65"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="70"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="65"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="70"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="65"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="70"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="65"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="70"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="65"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -5137,7 +5416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="66" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScale="66" workbookViewId="0">
       <selection activeCell="Q70" sqref="Q70"/>
     </sheetView>
   </sheetViews>
@@ -5780,11 +6059,11 @@
       <c r="A68" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B68" s="80" t="str">
+      <c r="B68" s="85" t="str">
         <f>"td_Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
         <v xml:space="preserve">td_Cost And Freight (CFR) , , </v>
       </c>
-      <c r="C68" s="65"/>
+      <c r="C68" s="70"/>
       <c r="D68" s="38" t="s">
         <v>178</v>
       </c>
@@ -5795,13 +6074,13 @@
       <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:12" ht="34.200000000000003" customHeight="1">
-      <c r="A69" s="84" t="s">
+      <c r="A69" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="91" t="s">
+      <c r="B69" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="65"/>
+      <c r="C69" s="70"/>
       <c r="D69" s="37" t="s">
         <v>181</v>
       </c>
@@ -5812,11 +6091,11 @@
       <c r="I69" s="37"/>
     </row>
     <row r="70" spans="1:12" ht="30" customHeight="1">
-      <c r="A70" s="85"/>
-      <c r="B70" s="88" t="s">
+      <c r="A70" s="90"/>
+      <c r="B70" s="93" t="s">
         <v>182</v>
       </c>
-      <c r="C70" s="65"/>
+      <c r="C70" s="70"/>
       <c r="D70" s="37" t="s">
         <v>183</v>
       </c>
@@ -5827,11 +6106,11 @@
       <c r="I70" s="37"/>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A71" s="85"/>
-      <c r="B71" s="88" t="s">
+      <c r="A71" s="90"/>
+      <c r="B71" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="65"/>
+      <c r="C71" s="70"/>
       <c r="D71" s="37" t="s">
         <v>185</v>
       </c>
@@ -5842,11 +6121,11 @@
       <c r="I71" s="37"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A72" s="86"/>
-      <c r="B72" s="88" t="s">
+      <c r="A72" s="91"/>
+      <c r="B72" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="65"/>
+      <c r="C72" s="70"/>
       <c r="D72" s="37" t="s">
         <v>187</v>
       </c>
@@ -5860,11 +6139,11 @@
       <c r="A73" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="90" t="str">
+      <c r="B73" s="95" t="str">
         <f>J73&amp;K73&amp;L73</f>
         <v>td_All invoices are due and payable at the specified payment date or [invalid payment term] after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
       </c>
-      <c r="C73" s="65"/>
+      <c r="C73" s="70"/>
       <c r="D73" s="38" t="s">
         <v>189</v>
       </c>
@@ -5890,147 +6169,147 @@
       <c r="A74" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B74" s="83" t="s">
+      <c r="B74" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="C74" s="65"/>
+      <c r="C74" s="70"/>
     </row>
     <row r="75" spans="1:12" ht="14.4" customHeight="1">
       <c r="A75" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B75" s="83" t="s">
+      <c r="B75" s="88" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="65"/>
+      <c r="C75" s="70"/>
     </row>
     <row r="76" spans="1:12" ht="28.2" customHeight="1">
-      <c r="A76" s="87" t="s">
+      <c r="A76" s="92" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="82" t="s">
+      <c r="B76" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C76" s="65"/>
+      <c r="C76" s="70"/>
     </row>
     <row r="77" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A77" s="85"/>
-      <c r="B77" s="81" t="s">
+      <c r="A77" s="90"/>
+      <c r="B77" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="C77" s="65"/>
+      <c r="C77" s="70"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="85"/>
-      <c r="B78" s="81" t="s">
+      <c r="A78" s="90"/>
+      <c r="B78" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="C78" s="65"/>
+      <c r="C78" s="70"/>
     </row>
     <row r="79" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A79" s="85"/>
-      <c r="B79" s="81" t="s">
+      <c r="A79" s="90"/>
+      <c r="B79" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="65"/>
+      <c r="C79" s="70"/>
     </row>
     <row r="80" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A80" s="85"/>
-      <c r="B80" s="81" t="s">
+      <c r="A80" s="90"/>
+      <c r="B80" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="C80" s="65"/>
+      <c r="C80" s="70"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A81" s="85"/>
-      <c r="B81" s="82" t="s">
+      <c r="A81" s="90"/>
+      <c r="B81" s="87" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="65"/>
+      <c r="C81" s="70"/>
     </row>
     <row r="82" spans="1:3" ht="41.4" customHeight="1">
-      <c r="A82" s="85"/>
-      <c r="B82" s="89" t="s">
+      <c r="A82" s="90"/>
+      <c r="B82" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="C82" s="65"/>
+      <c r="C82" s="70"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A83" s="85"/>
-      <c r="B83" s="82" t="s">
+      <c r="A83" s="90"/>
+      <c r="B83" s="87" t="s">
         <v>204</v>
       </c>
-      <c r="C83" s="65"/>
+      <c r="C83" s="70"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A84" s="85"/>
-      <c r="B84" s="81" t="s">
+      <c r="A84" s="90"/>
+      <c r="B84" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="C84" s="65"/>
+      <c r="C84" s="70"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="85"/>
-      <c r="B85" s="81" t="s">
+      <c r="A85" s="90"/>
+      <c r="B85" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="C85" s="65"/>
+      <c r="C85" s="70"/>
     </row>
     <row r="86" spans="1:3" ht="33.6" customHeight="1">
-      <c r="A86" s="85"/>
-      <c r="B86" s="81" t="s">
+      <c r="A86" s="90"/>
+      <c r="B86" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="65"/>
+      <c r="C86" s="70"/>
     </row>
     <row r="87" spans="1:3" ht="31.2" customHeight="1">
-      <c r="A87" s="85"/>
-      <c r="B87" s="81" t="s">
+      <c r="A87" s="90"/>
+      <c r="B87" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="65"/>
+      <c r="C87" s="70"/>
     </row>
     <row r="88" spans="1:3" ht="48.6" customHeight="1">
-      <c r="A88" s="85"/>
-      <c r="B88" s="82" t="s">
+      <c r="A88" s="90"/>
+      <c r="B88" s="87" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="65"/>
+      <c r="C88" s="70"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="86"/>
-      <c r="B89" s="82" t="s">
+      <c r="A89" s="91"/>
+      <c r="B89" s="87" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="65"/>
+      <c r="C89" s="70"/>
     </row>
     <row r="90" spans="1:3" ht="30.6" customHeight="1">
-      <c r="A90" s="87" t="s">
+      <c r="A90" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="82" t="s">
+      <c r="B90" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="65"/>
+      <c r="C90" s="70"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="86"/>
-      <c r="B91" s="82" t="s">
+      <c r="A91" s="91"/>
+      <c r="B91" s="87" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="65"/>
+      <c r="C91" s="70"/>
     </row>
     <row r="92" spans="1:3" ht="55.2" customHeight="1">
-      <c r="A92" s="92" t="s">
+      <c r="A92" s="97" t="s">
         <v>214</v>
       </c>
-      <c r="B92" s="83" t="s">
+      <c r="B92" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="65"/>
+      <c r="C92" s="70"/>
     </row>
     <row r="93" spans="1:3" ht="28.8" customHeight="1">
-      <c r="A93" s="85"/>
+      <c r="A93" s="90"/>
       <c r="B93" s="34" t="s">
         <v>216</v>
       </c>
@@ -6039,7 +6318,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="85"/>
+      <c r="A94" s="90"/>
       <c r="B94" s="34" t="s">
         <v>218</v>
       </c>
@@ -6048,7 +6327,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="85"/>
+      <c r="A95" s="90"/>
       <c r="B95" s="34" t="s">
         <v>220</v>
       </c>
@@ -6057,7 +6336,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="85"/>
+      <c r="A96" s="90"/>
       <c r="B96" s="34" t="s">
         <v>222</v>
       </c>
@@ -6066,7 +6345,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="85"/>
+      <c r="A97" s="90"/>
       <c r="B97" s="34" t="s">
         <v>224</v>
       </c>
@@ -6075,7 +6354,7 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="86"/>
+      <c r="A98" s="91"/>
       <c r="B98" s="34" t="s">
         <v>226</v>
       </c>
@@ -6087,37 +6366,37 @@
       <c r="A99" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B99" s="83" t="s">
+      <c r="B99" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="65"/>
+      <c r="C99" s="70"/>
     </row>
     <row r="100" spans="1:3" ht="30" customHeight="1">
       <c r="A100" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="93" t="s">
+      <c r="B100" s="98" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="65"/>
+      <c r="C100" s="70"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="83" t="s">
+      <c r="B101" s="88" t="s">
         <v>233</v>
       </c>
-      <c r="C101" s="65"/>
+      <c r="C101" s="70"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="83" t="s">
+      <c r="B102" s="88" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="65"/>
+      <c r="C102" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -6320,6 +6599,236 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EC56CC-78DA-4128-861F-2870B8FE444B}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="32.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1">
+      <c r="A1" s="64" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="64" t="s">
+        <v>364</v>
+      </c>
+      <c r="H1" s="64" t="s">
+        <v>365</v>
+      </c>
+      <c r="I1" s="64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="31.8" thickBot="1">
+      <c r="A2" s="68" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F2" s="66">
+        <v>45635</v>
+      </c>
+      <c r="G2" s="65">
+        <v>9</v>
+      </c>
+      <c r="H2" s="67">
+        <v>2024</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.8" thickBot="1">
+      <c r="A3" s="68" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>373</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>369</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F3" s="66">
+        <v>45605</v>
+      </c>
+      <c r="G3" s="65">
+        <v>11</v>
+      </c>
+      <c r="H3" s="67">
+        <v>2024</v>
+      </c>
+      <c r="I3" s="65" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.8" thickBot="1">
+      <c r="A4" s="68" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>376</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>377</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F4" s="66">
+        <v>45574</v>
+      </c>
+      <c r="G4" s="65">
+        <v>10</v>
+      </c>
+      <c r="H4" s="67">
+        <v>2024</v>
+      </c>
+      <c r="I4" s="65" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.2" thickBot="1">
+      <c r="A5" s="68" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>369</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F5" s="66">
+        <v>45666</v>
+      </c>
+      <c r="G5" s="65">
+        <v>1</v>
+      </c>
+      <c r="H5" s="67">
+        <v>2025</v>
+      </c>
+      <c r="I5" s="65" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.2" thickBot="1">
+      <c r="A6" s="68" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>384</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="66">
+        <v>45697</v>
+      </c>
+      <c r="G6" s="65">
+        <v>2</v>
+      </c>
+      <c r="H6" s="67">
+        <v>2025</v>
+      </c>
+      <c r="I6" s="65" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.2" thickBot="1">
+      <c r="A7" s="68" t="s">
+        <v>352</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>387</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>384</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F7" s="66">
+        <v>45697</v>
+      </c>
+      <c r="G7" s="65">
+        <v>2</v>
+      </c>
+      <c r="H7" s="67">
+        <v>2025</v>
+      </c>
+      <c r="I7" s="65" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -6337,7 +6846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -6354,7 +6863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -6367,163 +6876,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
-        <v>356</v>
-      </c>
-      <c r="B1" s="62"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="94" t="s">
-        <v>236</v>
-      </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="95" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="65"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="52" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="54" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="53" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="55" t="s">
-        <v>248</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="95" t="s">
-        <v>249</v>
-      </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="65"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="52" t="s">
-        <v>250</v>
-      </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="52" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="52" t="s">
-        <v>252</v>
-      </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="52" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="94" t="s">
-        <v>253</v>
-      </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="52" t="s">
-        <v>254</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="52" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="52" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="52" t="s">
-        <v>258</v>
-      </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="52" t="s">
-        <v>259</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A13:C13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add effluent options
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4E9A7A-EC80-4D0F-B8F7-D13803A88C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ECD96B-657C-498B-80DB-A48EBC0EFC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="687" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP_Customer Information" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="435">
   <si>
     <t>sub_CUSTOMER INFORMATION</t>
   </si>
@@ -1367,13 +1367,151 @@
     <t>001/02/CTP/Cr6+/LCI/2025</t>
   </si>
   <si>
-    <t>PT Coba Jaya</t>
-  </si>
-  <si>
-    <t>PCJ</t>
-  </si>
-  <si>
-    <t>001/02/CTP/Cr6+/PCJ/2025</t>
+    <t>fd_Effluent Warranty</t>
+  </si>
+  <si>
+    <t>PERMENKES No. 2 Tahun 2023 (Parameter Air untuk Keperluan Higiene dan Sanitasi)</t>
+  </si>
+  <si>
+    <t>PERMENKES No. 2 Tahun 2023 (Parameter Wajib Air Minum)</t>
+  </si>
+  <si>
+    <t>PERMENLHK RI No. P.68 Tahun 2016 (Baku Mutu Air Limbah Domestik)</t>
+  </si>
+  <si>
+    <t>PP RI No. 22 Tahun 2021 (Baku Mutu Air Sungai Kelas 1 dan Sejenisnya)</t>
+  </si>
+  <si>
+    <t>PP RI No. 22 Tahun 2021 (Baku Mutu Air Sungai Kelas 2 dan Sejenisnya)</t>
+  </si>
+  <si>
+    <t>PP RI No. 22 Tahun 2021 (Baku Mutu Air Sungai Kelas 3 dan Sejenisnya)</t>
+  </si>
+  <si>
+    <t>PP RI No. 22 Tahun 2021 (Baku Mutu Air Sungai Kelas 4 dan Sejenisnya)</t>
+  </si>
+  <si>
+    <t>fd_Grade Customer Selection</t>
+  </si>
+  <si>
+    <t>fh_Grade and Brand Customer Preferences</t>
+  </si>
+  <si>
+    <t>fd_Pump Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Dosing Pump Selection</t>
+  </si>
+  <si>
+    <t>fd_Blower Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_APP Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Agitator Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Mixer Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_MPS Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Aerator Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Screening System Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Motor Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Diffuser Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_PLC Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_HMI Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Instrument Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Cable Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Cable Signal Brand Selection</t>
+  </si>
+  <si>
+    <t>fd_Chemical Tank Brand Selection</t>
+  </si>
+  <si>
+    <t>GRUNDFOS</t>
+  </si>
+  <si>
+    <t>fd_Type</t>
+  </si>
+  <si>
+    <t>End Suction Centrifugal Pump</t>
+  </si>
+  <si>
+    <t>fd_Model</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>NKG</t>
+  </si>
+  <si>
+    <t>EBARA</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
+    <t>FSSC</t>
+  </si>
+  <si>
+    <t>CNP</t>
+  </si>
+  <si>
+    <t>CDMF</t>
+  </si>
+  <si>
+    <t>Vertical Multistage Centrifugal Pump</t>
+  </si>
+  <si>
+    <t>Horizontal Multistage Centrifugal Pump</t>
+  </si>
+  <si>
+    <t>CHL</t>
+  </si>
+  <si>
+    <t>Submersible Pump</t>
+  </si>
+  <si>
+    <t>WQ</t>
+  </si>
+  <si>
+    <t>LEO</t>
+  </si>
+  <si>
+    <t>LVRS</t>
+  </si>
+  <si>
+    <t>LEP</t>
+  </si>
+  <si>
+    <t>SWE</t>
+  </si>
+  <si>
+    <t>XSP</t>
   </si>
 </sst>
 </file>
@@ -1381,13 +1519,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0\ &quot;m2&quot;"/>
-    <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;Rp&quot;* #,##0.00_);_(&quot;Rp&quot;* \(#,##0.00\);_(&quot;Rp&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0\ &quot;m2&quot;"/>
+    <numFmt numFmtId="167" formatCode="d/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1514,6 +1652,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1698,10 +1842,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1742,13 +1886,13 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1757,7 +1901,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1856,7 +2000,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1887,58 +2031,73 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1949,9 +2108,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,7 +2120,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2748,6 +2904,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3071,7 +3231,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:C42"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4"/>
@@ -3086,18 +3246,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="74"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -3110,11 +3270,11 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
@@ -3130,8 +3290,8 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3147,8 +3307,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -3164,8 +3324,8 @@
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3178,11 +3338,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3198,8 +3358,8 @@
       <c r="A8" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="74"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3212,8 +3372,8 @@
       <c r="A9" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="74"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3226,8 +3386,8 @@
       <c r="A10" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="74"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3240,8 +3400,8 @@
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3257,8 +3417,8 @@
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="70"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3274,8 +3434,8 @@
       <c r="A13" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="74"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3285,11 +3445,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="70"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="74"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3447,8 +3607,8 @@
       <c r="A24" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="74"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3458,11 +3618,11 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -3478,8 +3638,8 @@
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="70"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -3492,11 +3652,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="70"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="74"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3512,8 +3672,8 @@
       <c r="A28" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="74"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3526,8 +3686,8 @@
       <c r="A29" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="70"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="74"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3540,8 +3700,8 @@
       <c r="A30" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="70"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="74"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3554,8 +3714,8 @@
       <c r="A31" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="79"/>
-      <c r="C31" s="70"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -3571,8 +3731,8 @@
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="70"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3588,8 +3748,8 @@
       <c r="A33" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="70"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="74"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -3726,8 +3886,8 @@
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="70"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="74"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3737,11 +3897,11 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="77" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="72"/>
-      <c r="C43" s="70"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="74"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3754,8 +3914,8 @@
       <c r="A44" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="B44" s="69"/>
-      <c r="C44" s="70"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="74"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3768,8 +3928,8 @@
       <c r="A45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="69"/>
-      <c r="C45" s="70"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="74"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -3782,15 +3942,15 @@
       <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="69"/>
-      <c r="C46" s="70"/>
+      <c r="B46" s="75"/>
+      <c r="C46" s="74"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="69"/>
-      <c r="C47" s="70"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="74"/>
     </row>
     <row r="48" spans="1:14" ht="13.2" customHeight="1">
       <c r="H48" s="1"/>
@@ -3803,6 +3963,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B13:C13"/>
@@ -3819,20 +3993,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:C47" xr:uid="{C62B14A6-8605-4A3A-B7E8-6D0D25B30037}">
@@ -3852,7 +4012,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3869,18 +4029,18 @@
       <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="104" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="74"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="52" t="s">
@@ -3937,11 +4097,11 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="104" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="74"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
@@ -3962,11 +4122,11 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
@@ -4047,11 +4207,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="76" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="69" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4060,6 +4220,8 @@
     <col min="2" max="2" width="36.77734375" style="4" customWidth="1"/>
     <col min="3" max="3" width="42.109375" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.33203125" customWidth="1"/>
     <col min="24" max="24" width="8.77734375" customWidth="1"/>
   </cols>
@@ -4068,9 +4230,9 @@
       <c r="A1" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -4383,7 +4545,7 @@
       </c>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:9">
       <c r="A33" s="6" t="s">
         <v>57</v>
       </c>
@@ -4393,7 +4555,7 @@
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:9">
       <c r="A34" s="6" t="s">
         <v>270</v>
       </c>
@@ -4403,7 +4565,7 @@
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:9">
       <c r="A35" s="7" t="s">
         <v>306</v>
       </c>
@@ -4413,7 +4575,7 @@
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:9">
       <c r="A36" s="6" t="s">
         <v>60</v>
       </c>
@@ -4423,7 +4585,7 @@
       </c>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:9">
       <c r="A37" s="6" t="s">
         <v>61</v>
       </c>
@@ -4433,7 +4595,7 @@
       </c>
       <c r="D37" s="27"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:9">
       <c r="A38" s="6" t="s">
         <v>63</v>
       </c>
@@ -4443,7 +4605,7 @@
       </c>
       <c r="D38" s="27"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:9">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -4453,251 +4615,351 @@
       </c>
       <c r="D39" s="27"/>
     </row>
-    <row r="40" spans="1:4" ht="15.6">
-      <c r="A40" s="84" t="s">
+    <row r="40" spans="1:9">
+      <c r="A40" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="70"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="69" t="s">
+        <v>394</v>
+      </c>
+      <c r="B41" s="71"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="B42" s="71"/>
+      <c r="C42" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D42" s="71"/>
+      <c r="G42" t="s">
+        <v>413</v>
+      </c>
+      <c r="H42" t="s">
+        <v>425</v>
+      </c>
+      <c r="I42" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="69"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="D43" s="72"/>
+      <c r="G43" t="s">
+        <v>413</v>
+      </c>
+      <c r="H43" t="s">
+        <v>425</v>
+      </c>
+      <c r="I43" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="69" t="s">
+        <v>397</v>
+      </c>
+      <c r="B44" s="71"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="G44" t="s">
+        <v>413</v>
+      </c>
+      <c r="H44" t="s">
+        <v>415</v>
+      </c>
+      <c r="I44" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="69" t="s">
+        <v>398</v>
+      </c>
+      <c r="B45" s="71"/>
+      <c r="C45" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D45" s="71"/>
+      <c r="G45" t="s">
+        <v>420</v>
+      </c>
+      <c r="H45" t="s">
+        <v>425</v>
+      </c>
+      <c r="I45" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="69" t="s">
+        <v>399</v>
+      </c>
+      <c r="B46" s="71"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="G46" t="s">
+        <v>420</v>
+      </c>
+      <c r="H46" t="s">
+        <v>415</v>
+      </c>
+      <c r="I46" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="69" t="s">
+        <v>400</v>
+      </c>
+      <c r="B47" s="71"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="G47" t="s">
+        <v>423</v>
+      </c>
+      <c r="H47" t="s">
+        <v>425</v>
+      </c>
+      <c r="I47" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="69" t="s">
+        <v>401</v>
+      </c>
+      <c r="B48" s="71"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="G48" t="s">
+        <v>423</v>
+      </c>
+      <c r="H48" t="s">
+        <v>426</v>
+      </c>
+      <c r="I48" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="69" t="s">
+        <v>412</v>
+      </c>
+      <c r="B49" s="71"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="G49" t="s">
+        <v>423</v>
+      </c>
+      <c r="H49" t="s">
+        <v>428</v>
+      </c>
+      <c r="I49" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="69" t="s">
+        <v>402</v>
+      </c>
+      <c r="B50" s="71"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="G50" t="s">
+        <v>430</v>
+      </c>
+      <c r="H50" t="s">
+        <v>425</v>
+      </c>
+      <c r="I50" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="69" t="s">
+        <v>403</v>
+      </c>
+      <c r="B51" s="71"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="G51" t="s">
+        <v>430</v>
+      </c>
+      <c r="H51" t="s">
+        <v>415</v>
+      </c>
+      <c r="I51" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="69" t="s">
+        <v>404</v>
+      </c>
+      <c r="B52" s="71"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="G52" t="s">
+        <v>430</v>
+      </c>
+      <c r="H52" t="s">
+        <v>428</v>
+      </c>
+      <c r="I52" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B53" s="71"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="G53" t="s">
+        <v>430</v>
+      </c>
+      <c r="H53" t="s">
+        <v>428</v>
+      </c>
+      <c r="I53" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B54" s="71"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B55" s="71"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B56" s="71"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="B57" s="71"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B58" s="71"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B59" s="71"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.6">
+      <c r="A60" s="84" t="s">
         <v>268</v>
       </c>
-      <c r="B40" s="74"/>
-      <c r="C40" s="74"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="71" t="s">
+      <c r="B60" s="81"/>
+      <c r="C60" s="81"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="70"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6" t="s">
+      <c r="B61" s="78"/>
+      <c r="C61" s="74"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="40" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="6" t="s">
+    <row r="63" spans="1:9">
+      <c r="A63" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="20" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="6" t="s">
+    <row r="64" spans="1:9">
+      <c r="A64" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="80"/>
-      <c r="C44" s="70"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="80"/>
-      <c r="C45" s="70"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="82" t="e">
-        <f>B50/B49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C46" s="70"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="83"/>
-      <c r="C47" s="70"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="70"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="82"/>
-      <c r="C59" s="70"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="B61" s="72"/>
-      <c r="C61" s="70"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="80"/>
-      <c r="C62" s="70"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B63" s="81"/>
-      <c r="C63" s="70"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="40" t="s">
-        <v>70</v>
-      </c>
+      <c r="B64" s="85"/>
+      <c r="C64" s="74"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B65" s="85"/>
+      <c r="C65" s="74"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B66" s="86" t="e">
+        <f>B70/B69</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C66" s="74"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B67" s="87"/>
+      <c r="C67" s="74"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B68" s="88"/>
+      <c r="C68" s="74"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="40" t="s">
@@ -4706,7 +4968,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="40" t="s">
@@ -4715,7 +4977,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="40" t="s">
@@ -4724,144 +4986,239 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="6" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B72" s="3"/>
-      <c r="C72" s="49" t="s">
-        <v>87</v>
+      <c r="C72" s="40" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="6" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="49" t="s">
-        <v>89</v>
+      <c r="C73" s="40" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B74" s="82"/>
-      <c r="C74" s="70"/>
+        <v>83</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="40" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="71" t="s">
-        <v>309</v>
-      </c>
-      <c r="B75" s="72"/>
-      <c r="C75" s="70"/>
+      <c r="A75" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="40" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="21" t="s">
-        <v>109</v>
+        <v>85</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="40" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B77" s="72"/>
-      <c r="C77" s="70"/>
+      <c r="A77" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="49" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B78" s="80"/>
-      <c r="C78" s="70"/>
+        <v>88</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="49" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="B79" s="80"/>
-      <c r="C79" s="70"/>
+        <v>90</v>
+      </c>
+      <c r="B79" s="86"/>
+      <c r="C79" s="74"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="78"/>
+      <c r="C81" s="74"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="85"/>
+      <c r="C82" s="74"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B83" s="85"/>
+      <c r="C83" s="74"/>
+      <c r="E83" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="77" t="s">
+        <v>309</v>
+      </c>
+      <c r="B84" s="78"/>
+      <c r="C84" s="74"/>
+      <c r="E84" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="22"/>
+      <c r="C85" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E85" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="B86" s="78"/>
+      <c r="C86" s="74"/>
+      <c r="E86" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B87" s="85"/>
+      <c r="C87" s="74"/>
+      <c r="E87" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B88" s="85"/>
+      <c r="C88" s="74"/>
+      <c r="E88" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B80" s="80"/>
-      <c r="C80" s="70"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="6" t="s">
+      <c r="B89" s="85"/>
+      <c r="C89" s="74"/>
+      <c r="E89" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B81" s="80"/>
-      <c r="C81" s="70"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="6" t="s">
+      <c r="B90" s="85"/>
+      <c r="C90" s="74"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B82" s="80"/>
-      <c r="C82" s="70"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="6" t="s">
+      <c r="B91" s="85"/>
+      <c r="C91" s="74"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B83" s="80"/>
-      <c r="C83" s="70"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="6" t="s">
+      <c r="B92" s="85"/>
+      <c r="C92" s="74"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B84" s="80"/>
-      <c r="C84" s="70"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="6" t="s">
+      <c r="B93" s="85"/>
+      <c r="C93" s="74"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B85" s="80"/>
-      <c r="C85" s="70"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="6" t="s">
+      <c r="B94" s="85"/>
+      <c r="C94" s="74"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B86" s="80"/>
-      <c r="C86" s="70"/>
+      <c r="B95" s="85"/>
+      <c r="C95" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="23">
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="A81:C81"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A60:C60"/>
     <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <dataValidations count="24">
+  <dataValidations count="43">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"WWTP PROJECT,WRP PROJECT,WTP PROJECT,STP PROJECT,CLOSING LOOP PROJECT"</formula1>
     </dataValidation>
@@ -4913,29 +5270,87 @@
     <dataValidation type="date" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="B26:B29" xr:uid="{00000000-0002-0000-0100-000010000000}">
       <formula1>45658</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B47 D37:D39" xr:uid="{00000000-0002-0000-0100-000011000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B67 D37:D40" xr:uid="{00000000-0002-0000-0100-000011000000}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D23" xr:uid="{00000000-0002-0000-0100-000012000000}">
       <formula1>"14 days,30 days,45 days"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{0E563FC6-D334-4102-80DB-B12A49BE4535}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B64" xr:uid="{0E563FC6-D334-4102-80DB-B12A49BE4535}">
       <formula1>"MESSOPHILIC,TERMOPHILIC"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B45" xr:uid="{0AE3CB1E-D3BA-43AD-973B-95AC5034F0ED}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B65" xr:uid="{0AE3CB1E-D3BA-43AD-973B-95AC5034F0ED}">
       <formula1>"RICH FOG&amp;TSS,RICH SUGAR LOW FOG&amp;TSS,NON BGD ORGANIC,NON ORGANIC,DOMESTIC WASTE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B62" xr:uid="{3CAFC935-D919-4CAE-99B4-C39E42BBAA48}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{3CAFC935-D919-4CAE-99B4-C39E42BBAA48}">
       <formula1>"DISCHARGE ONLY,REUSE : G-3,REUSE : G-2,REUSE : G-1,REUSE : G-0"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B76" xr:uid="{722D38B0-FDF3-408F-A5A0-0137B25A2B6B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B85" xr:uid="{722D38B0-FDF3-408F-A5A0-0137B25A2B6B}">
       <formula1>"75%-85%,60%-75%,40%-50%,&lt;40%"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B78:C86" xr:uid="{986438E4-27C9-4346-92EB-B2ED90C73F27}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B87:C95" xr:uid="{986438E4-27C9-4346-92EB-B2ED90C73F27}">
       <formula1>"INLET TANK,EQUALIZING,OWS,ANAFLOAT,INTERMEDIATE TANK,ANAPAK,AERATION,SECONDARY CLARIFIER,MMF,ACF,MPS,FINAL TANK,DAF,MBR,PRIMARY CLARIFIER,BWRO,CCRO,SWRO,ANAMEM,AOP,SMF"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B83:C83" xr:uid="{9ACE7AA9-3561-4482-B5AE-1CC8193A6502}">
+      <formula1>"PERMENKES No. 2 Tahun 2023 (Parameter Wajib Air Minum), PERMENKES No. 2 Tahun 2023 (Parameter Air untuk Keperluan Higiene dan Sanitasi),"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{D5B1539D-C275-45EB-9183-7885F42584B5}">
+      <formula1>"GRUNDFOS,KSB,XYLEM,ITT GOULDS,EBARA,WILO,FLOWREX,CNP,LEO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B41" xr:uid="{6D15CE87-D514-4C0B-81EB-0E4CE7F62C0E}">
+      <formula1>"GRADE A,GRADE B,GRADE C,GRADE E"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{08B0867B-4945-4A65-BE3D-5208EFC4295B}">
+      <formula1>"PROMINENT,MILTON ROY,MLI,SEKO,FLOWREX,NEWDOSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B45" xr:uid="{97CF9C98-806A-40FD-8822-3FC73739DB15}">
+      <formula1>"ATLAS COPCO,AERZEN,ROBUSCHI,KAESER,ZGK,EURUS,CHANGHE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B46" xr:uid="{52BECC89-4D0B-4369-9F9A-553255C79538}">
+      <formula1>"BOEEP,FLOWREX"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B49" xr:uid="{E95110B2-E6A7-4E57-AFB6-751FA4B95D57}">
+      <formula1>"PENGUIN,CANATURE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B47:B48 B51:B52" xr:uid="{537E1950-1AC0-4F58-88BF-273D4E49D878}">
+      <formula1>"FLOWREX"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B50" xr:uid="{85953944-4004-4CDE-BEBC-505E1555CDB8}">
+      <formula1>"TECHASE,BOEEP,FLOWREX"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B53" xr:uid="{7550BC07-BF3B-4F31-B1E3-60BABD90CC24}">
+      <formula1>"ABB"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B54" xr:uid="{F0A0AB00-97BB-49CD-9227-DC23E45ABA85}">
+      <formula1>"JAGGER,REHAU"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B55" xr:uid="{0503AAA6-CA9D-40A3-8F21-39E4043C5C8D}">
+      <formula1>"SIEMENS,ALLEN-BRADLEY,SCHNEIDER,OMRON"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B56" xr:uid="{DEC920D3-5DEC-4C65-A781-E1E80973E12B}">
+      <formula1>"SIEMENS,ALLEN-BRADLEY,SCHNEIDER,OMRON,HAIWELL,MCGS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{A792B851-F0D0-41CA-8C0E-6E7CC343A4CA}">
+      <formula1>"DIAC-X,ENDRESS+HAUSER,WIKA,ARMATHERM,EMERSON,YOKOGAWA,VEGA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B58" xr:uid="{65773699-45FC-42E7-9DA3-133CEF3C1BA2}">
+      <formula1>"SUPREME,JJLAP,ETERNA,LOCAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{D0BD5687-B728-4D47-8D29-FCF4E690F857}">
+      <formula1>"SUPREME,JJLAP,LOCAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D45" xr:uid="{D51A701E-7350-4097-BB5C-841E8043FF45}">
+      <formula1>"TURBO BLOWER,ROOTS BLOWER,SIDE CHANNEL BLOWER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D42" xr:uid="{99A5EF61-B540-454C-B71C-2967FB1181D2}">
+      <formula1>"VERTICAL MULTISTAGE CENTRIFUGAL PUMP,END SUCTION CENTRIFUGAL PUMP,SUBMERSIBLE PUMP"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D43" xr:uid="{D1457EEC-A832-482F-B74F-3CFCBA2B89B5}">
+      <formula1>$I$42:$I$53</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4962,15 +5377,15 @@
       <c r="A1" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="74"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
@@ -4994,36 +5409,36 @@
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="74"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="74"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="74"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="74"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="74"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
@@ -5128,8 +5543,8 @@
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="70"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="74"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
@@ -5141,25 +5556,25 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="74"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="74"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="74"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
@@ -5273,15 +5688,15 @@
       <c r="A38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="82"/>
-      <c r="C38" s="70"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="74"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="70"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="74"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
@@ -5293,77 +5708,84 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="70"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="74"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="70"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="74"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="70"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="74"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="80"/>
-      <c r="C44" s="70"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="74"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="80"/>
-      <c r="C45" s="70"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="74"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="80"/>
-      <c r="C46" s="70"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="74"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="80"/>
-      <c r="C47" s="70"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="74"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="80"/>
-      <c r="C48" s="70"/>
+      <c r="B48" s="85"/>
+      <c r="C48" s="74"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="80"/>
-      <c r="C49" s="70"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="74"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="80"/>
-      <c r="C50" s="70"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B49:C49"/>
@@ -5380,13 +5802,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B40" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -6059,11 +6474,11 @@
       <c r="A68" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B68" s="85" t="str">
+      <c r="B68" s="102" t="str">
         <f>"td_Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
         <v xml:space="preserve">td_Cost And Freight (CFR) , , </v>
       </c>
-      <c r="C68" s="70"/>
+      <c r="C68" s="74"/>
       <c r="D68" s="38" t="s">
         <v>178</v>
       </c>
@@ -6074,13 +6489,13 @@
       <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:12" ht="34.200000000000003" customHeight="1">
-      <c r="A69" s="89" t="s">
+      <c r="A69" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="96" t="s">
+      <c r="B69" s="100" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="70"/>
+      <c r="C69" s="74"/>
       <c r="D69" s="37" t="s">
         <v>181</v>
       </c>
@@ -6091,11 +6506,11 @@
       <c r="I69" s="37"/>
     </row>
     <row r="70" spans="1:12" ht="30" customHeight="1">
-      <c r="A70" s="90"/>
-      <c r="B70" s="93" t="s">
+      <c r="A70" s="95"/>
+      <c r="B70" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="C70" s="70"/>
+      <c r="C70" s="74"/>
       <c r="D70" s="37" t="s">
         <v>183</v>
       </c>
@@ -6106,11 +6521,11 @@
       <c r="I70" s="37"/>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A71" s="90"/>
-      <c r="B71" s="93" t="s">
+      <c r="A71" s="95"/>
+      <c r="B71" s="91" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="70"/>
+      <c r="C71" s="74"/>
       <c r="D71" s="37" t="s">
         <v>185</v>
       </c>
@@ -6121,11 +6536,11 @@
       <c r="I71" s="37"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A72" s="91"/>
-      <c r="B72" s="93" t="s">
+      <c r="A72" s="96"/>
+      <c r="B72" s="91" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="70"/>
+      <c r="C72" s="74"/>
       <c r="D72" s="37" t="s">
         <v>187</v>
       </c>
@@ -6139,11 +6554,11 @@
       <c r="A73" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="95" t="str">
+      <c r="B73" s="99" t="str">
         <f>J73&amp;K73&amp;L73</f>
         <v>td_All invoices are due and payable at the specified payment date or [invalid payment term] after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
       </c>
-      <c r="C73" s="70"/>
+      <c r="C73" s="74"/>
       <c r="D73" s="38" t="s">
         <v>189</v>
       </c>
@@ -6169,147 +6584,147 @@
       <c r="A74" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B74" s="88" t="s">
+      <c r="B74" s="92" t="s">
         <v>193</v>
       </c>
-      <c r="C74" s="70"/>
+      <c r="C74" s="74"/>
     </row>
     <row r="75" spans="1:12" ht="14.4" customHeight="1">
       <c r="A75" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B75" s="88" t="s">
+      <c r="B75" s="92" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="70"/>
+      <c r="C75" s="74"/>
     </row>
     <row r="76" spans="1:12" ht="28.2" customHeight="1">
-      <c r="A76" s="92" t="s">
+      <c r="A76" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="87" t="s">
+      <c r="B76" s="89" t="s">
         <v>197</v>
       </c>
-      <c r="C76" s="70"/>
+      <c r="C76" s="74"/>
     </row>
     <row r="77" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A77" s="90"/>
-      <c r="B77" s="86" t="s">
+      <c r="A77" s="95"/>
+      <c r="B77" s="93" t="s">
         <v>198</v>
       </c>
-      <c r="C77" s="70"/>
+      <c r="C77" s="74"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="90"/>
-      <c r="B78" s="86" t="s">
+      <c r="A78" s="95"/>
+      <c r="B78" s="93" t="s">
         <v>199</v>
       </c>
-      <c r="C78" s="70"/>
+      <c r="C78" s="74"/>
     </row>
     <row r="79" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A79" s="90"/>
-      <c r="B79" s="86" t="s">
+      <c r="A79" s="95"/>
+      <c r="B79" s="93" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="70"/>
+      <c r="C79" s="74"/>
     </row>
     <row r="80" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A80" s="90"/>
-      <c r="B80" s="86" t="s">
+      <c r="A80" s="95"/>
+      <c r="B80" s="93" t="s">
         <v>201</v>
       </c>
-      <c r="C80" s="70"/>
+      <c r="C80" s="74"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A81" s="90"/>
-      <c r="B81" s="87" t="s">
+      <c r="A81" s="95"/>
+      <c r="B81" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="70"/>
+      <c r="C81" s="74"/>
     </row>
     <row r="82" spans="1:3" ht="41.4" customHeight="1">
-      <c r="A82" s="90"/>
-      <c r="B82" s="94" t="s">
+      <c r="A82" s="95"/>
+      <c r="B82" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="C82" s="70"/>
+      <c r="C82" s="74"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A83" s="90"/>
-      <c r="B83" s="87" t="s">
+      <c r="A83" s="95"/>
+      <c r="B83" s="89" t="s">
         <v>204</v>
       </c>
-      <c r="C83" s="70"/>
+      <c r="C83" s="74"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A84" s="90"/>
-      <c r="B84" s="86" t="s">
+      <c r="A84" s="95"/>
+      <c r="B84" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="C84" s="70"/>
+      <c r="C84" s="74"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="90"/>
-      <c r="B85" s="86" t="s">
+      <c r="A85" s="95"/>
+      <c r="B85" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="C85" s="70"/>
+      <c r="C85" s="74"/>
     </row>
     <row r="86" spans="1:3" ht="33.6" customHeight="1">
-      <c r="A86" s="90"/>
-      <c r="B86" s="86" t="s">
+      <c r="A86" s="95"/>
+      <c r="B86" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="70"/>
+      <c r="C86" s="74"/>
     </row>
     <row r="87" spans="1:3" ht="31.2" customHeight="1">
-      <c r="A87" s="90"/>
-      <c r="B87" s="86" t="s">
+      <c r="A87" s="95"/>
+      <c r="B87" s="93" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="70"/>
+      <c r="C87" s="74"/>
     </row>
     <row r="88" spans="1:3" ht="48.6" customHeight="1">
-      <c r="A88" s="90"/>
-      <c r="B88" s="87" t="s">
+      <c r="A88" s="95"/>
+      <c r="B88" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="70"/>
+      <c r="C88" s="74"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="91"/>
-      <c r="B89" s="87" t="s">
+      <c r="A89" s="96"/>
+      <c r="B89" s="89" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="70"/>
+      <c r="C89" s="74"/>
     </row>
     <row r="90" spans="1:3" ht="30.6" customHeight="1">
-      <c r="A90" s="92" t="s">
+      <c r="A90" s="97" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="87" t="s">
+      <c r="B90" s="89" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="70"/>
+      <c r="C90" s="74"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="91"/>
-      <c r="B91" s="87" t="s">
+      <c r="A91" s="96"/>
+      <c r="B91" s="89" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="70"/>
+      <c r="C91" s="74"/>
     </row>
     <row r="92" spans="1:3" ht="55.2" customHeight="1">
-      <c r="A92" s="97" t="s">
+      <c r="A92" s="101" t="s">
         <v>214</v>
       </c>
-      <c r="B92" s="88" t="s">
+      <c r="B92" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="70"/>
+      <c r="C92" s="74"/>
     </row>
     <row r="93" spans="1:3" ht="28.8" customHeight="1">
-      <c r="A93" s="90"/>
+      <c r="A93" s="95"/>
       <c r="B93" s="34" t="s">
         <v>216</v>
       </c>
@@ -6318,7 +6733,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="90"/>
+      <c r="A94" s="95"/>
       <c r="B94" s="34" t="s">
         <v>218</v>
       </c>
@@ -6327,7 +6742,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="90"/>
+      <c r="A95" s="95"/>
       <c r="B95" s="34" t="s">
         <v>220</v>
       </c>
@@ -6336,7 +6751,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="90"/>
+      <c r="A96" s="95"/>
       <c r="B96" s="34" t="s">
         <v>222</v>
       </c>
@@ -6345,7 +6760,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="90"/>
+      <c r="A97" s="95"/>
       <c r="B97" s="34" t="s">
         <v>224</v>
       </c>
@@ -6354,7 +6769,7 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="91"/>
+      <c r="A98" s="96"/>
       <c r="B98" s="34" t="s">
         <v>226</v>
       </c>
@@ -6366,50 +6781,47 @@
       <c r="A99" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B99" s="88" t="s">
+      <c r="B99" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="70"/>
+      <c r="C99" s="74"/>
     </row>
     <row r="100" spans="1:3" ht="30" customHeight="1">
       <c r="A100" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="98" t="s">
+      <c r="B100" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="70"/>
+      <c r="C100" s="74"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="88" t="s">
+      <c r="B101" s="92" t="s">
         <v>233</v>
       </c>
-      <c r="C101" s="70"/>
+      <c r="C101" s="74"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="88" t="s">
+      <c r="B102" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="70"/>
+      <c r="C102" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B75:C75"/>
     <mergeCell ref="A69:A72"/>
     <mergeCell ref="A76:A89"/>
     <mergeCell ref="B102:C102"/>
@@ -6426,13 +6838,16 @@
     <mergeCell ref="B87:C87"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="A92:A98"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B92:C92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
@@ -6443,8 +6858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDAD76A-B5C9-4A8B-B955-E4D223127E27}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6600,10 +7015,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EC56CC-78DA-4128-861F-2870B8FE444B}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6791,35 +7206,6 @@
       </c>
       <c r="I6" s="65" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="16.2" thickBot="1">
-      <c r="A7" s="68" t="s">
-        <v>352</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>386</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>387</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>384</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>370</v>
-      </c>
-      <c r="F7" s="66">
-        <v>45697</v>
-      </c>
-      <c r="G7" s="65">
-        <v>2</v>
-      </c>
-      <c r="H7" s="67">
-        <v>2025</v>
-      </c>
-      <c r="I7" s="65" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: remove uncessary print debug in generate proposal
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ECD96B-657C-498B-80DB-A48EBC0EFC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE2A19-268B-4DBB-938E-8EFE211C4422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="687" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="687" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP_Customer Information" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,16 @@
     <sheet name="DIP_Data Input" sheetId="4" r:id="rId4"/>
     <sheet name="User Code" sheetId="10" r:id="rId5"/>
     <sheet name="No of Quotation" sheetId="11" r:id="rId6"/>
-    <sheet name="DATA_PROPOSAL" sheetId="5" r:id="rId7"/>
-    <sheet name="DATA_OPEX" sheetId="6" r:id="rId8"/>
-    <sheet name="DATA_BOQ" sheetId="7" r:id="rId9"/>
-    <sheet name="DATA_TEMP" sheetId="8" r:id="rId10"/>
-    <sheet name="DATA_ELI" sheetId="9" r:id="rId11"/>
+    <sheet name="Effluent Warranty" sheetId="12" r:id="rId7"/>
+    <sheet name="DATA_PROPOSAL" sheetId="5" r:id="rId8"/>
+    <sheet name="DATA_OPEX" sheetId="6" r:id="rId9"/>
+    <sheet name="DATA_BOQ" sheetId="7" r:id="rId10"/>
+    <sheet name="DATA_TEMP" sheetId="8" r:id="rId11"/>
+    <sheet name="DATA_ELI" sheetId="9" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="_12.ABUTHMEN">#REF!</definedName>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="502">
   <si>
     <t>sub_CUSTOMER INFORMATION</t>
   </si>
@@ -1513,6 +1514,207 @@
   <si>
     <t>XSP</t>
   </si>
+  <si>
+    <t>Warranty_Type</t>
+  </si>
+  <si>
+    <t>Parameter_Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Row_Order</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>TDS</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Sisa Cl</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>Pb</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>E.Coli</t>
+  </si>
+  <si>
+    <t>Total Coliform</t>
+  </si>
+  <si>
+    <t>Odor</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>CFU/100 mL</t>
+  </si>
+  <si>
+    <t>6.5-8.5</t>
+  </si>
+  <si>
+    <t>&lt;300</t>
+  </si>
+  <si>
+    <t>&lt;3</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2-0.5</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>odorless</t>
+  </si>
+  <si>
+    <t>TDS*</t>
+  </si>
+  <si>
+    <t>Cr6+*</t>
+  </si>
+  <si>
+    <t>Fe*</t>
+  </si>
+  <si>
+    <t>Mn*</t>
+  </si>
+  <si>
+    <t>BOD</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>FOG</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>jumlah/100 mL</t>
+  </si>
+  <si>
+    <t>Pt-Co Unit</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>Total Nitrogen</t>
+  </si>
+  <si>
+    <t>Total Phospate</t>
+  </si>
+  <si>
+    <t>Fluoride*</t>
+  </si>
+  <si>
+    <t>Sulphure as H2S*</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>Cyanide*</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>Free Chlorine</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>Oil and Grease</t>
+  </si>
+  <si>
+    <t>Total Detergent</t>
+  </si>
+  <si>
+    <t>Fecal Coliform</t>
+  </si>
+  <si>
+    <t>MPN/100 mL</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>6-9</t>
+  </si>
 </sst>
 </file>
 
@@ -1525,7 +1727,7 @@
     <numFmt numFmtId="167" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,6 +1861,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1698,7 +1905,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1837,6 +2044,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1845,7 +2063,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2043,6 +2261,28 @@
     <xf numFmtId="3" fontId="20" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2129,6 +2369,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -2137,7 +2380,254 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2906,8 +3396,18 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A618CFEC-44F6-4C8B-BDE3-EA2F79B81662}" name="Table1" displayName="Table1" ref="A1:E126" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E126" xr:uid="{A618CFEC-44F6-4C8B-BDE3-EA2F79B81662}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8FF9B65A-C827-4665-A0C4-F657B5567CE1}" name="Warranty_Type" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{835507C8-9876-4B11-A685-71BD8080045C}" name="Parameter_Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{2A9AD4F8-CBA0-44C7-AF2B-5CC8CABF75A5}" name="Value" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B56B2D63-8511-4C83-BD0F-C279A53E1FF6}" name="Unit" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{81D1AD90-8006-4C83-BF91-52435EB042C6}" name="Row_Order" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3246,18 +3746,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="82"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -3270,11 +3770,11 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="74"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
@@ -3290,8 +3790,8 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3307,8 +3807,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="74"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -3324,8 +3824,8 @@
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="74"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3338,11 +3838,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3358,8 +3858,8 @@
       <c r="A8" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="74"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="82"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3372,8 +3872,8 @@
       <c r="A9" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="74"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="82"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3386,8 +3886,8 @@
       <c r="A10" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="74"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="82"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3400,8 +3900,8 @@
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="74"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3417,8 +3917,8 @@
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="74"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3434,8 +3934,8 @@
       <c r="A13" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="82"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3445,11 +3945,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="74"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="82"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3607,8 +4107,8 @@
       <c r="A24" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="82"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3618,11 +4118,11 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -3638,8 +4138,8 @@
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="82"/>
-      <c r="C26" s="74"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="82"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -3652,11 +4152,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="74"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="82"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3672,8 +4172,8 @@
       <c r="A28" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="75"/>
-      <c r="C28" s="74"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="82"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3686,8 +4186,8 @@
       <c r="A29" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="74"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="82"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3700,8 +4200,8 @@
       <c r="A30" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="74"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="82"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3714,8 +4214,8 @@
       <c r="A31" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="74"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -3731,8 +4231,8 @@
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="79"/>
-      <c r="C32" s="74"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3748,8 +4248,8 @@
       <c r="A33" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="74"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="82"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -3886,8 +4386,8 @@
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="74"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="82"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3897,11 +4397,11 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="78"/>
-      <c r="C43" s="74"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="82"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3914,8 +4414,8 @@
       <c r="A44" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="74"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="82"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3928,8 +4428,8 @@
       <c r="A45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="74"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="82"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -3942,15 +4442,15 @@
       <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="75"/>
-      <c r="C46" s="74"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="82"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="74"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="82"/>
     </row>
     <row r="48" spans="1:14" ht="13.2" customHeight="1">
       <c r="H48" s="1"/>
@@ -4008,6 +4508,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4029,18 +4544,18 @@
       <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="111" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="74"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="82"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="52" t="s">
@@ -4097,11 +4612,11 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="112" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="74"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="82"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
@@ -4122,11 +4637,11 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="111" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
@@ -4166,7 +4681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -4210,8 +4725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="69" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView topLeftCell="A66" zoomScale="69" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4227,12 +4742,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -4888,18 +5403,18 @@
       <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:9" ht="15.6">
-      <c r="A60" s="84" t="s">
+      <c r="A60" s="92" t="s">
         <v>268</v>
       </c>
-      <c r="B60" s="81"/>
-      <c r="C60" s="81"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="89"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="77" t="s">
+      <c r="A61" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="78"/>
-      <c r="C61" s="74"/>
+      <c r="B61" s="86"/>
+      <c r="C61" s="82"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="6" t="s">
@@ -4923,39 +5438,39 @@
       <c r="A64" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="85"/>
-      <c r="C64" s="74"/>
+      <c r="B64" s="93"/>
+      <c r="C64" s="82"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B65" s="85"/>
-      <c r="C65" s="74"/>
+      <c r="B65" s="93"/>
+      <c r="C65" s="82"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="86" t="e">
+      <c r="B66" s="94" t="e">
         <f>B70/B69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C66" s="74"/>
+      <c r="C66" s="82"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B67" s="87"/>
-      <c r="C67" s="74"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="82"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B68" s="88"/>
-      <c r="C68" s="74"/>
+      <c r="B68" s="96"/>
+      <c r="C68" s="82"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
@@ -5051,8 +5566,8 @@
       <c r="A79" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B79" s="86"/>
-      <c r="C79" s="74"/>
+      <c r="B79" s="94"/>
+      <c r="C79" s="82"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
@@ -5064,35 +5579,35 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="77" t="s">
+      <c r="A81" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="78"/>
-      <c r="C81" s="74"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="82"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B82" s="85"/>
-      <c r="C82" s="74"/>
+      <c r="B82" s="93"/>
+      <c r="C82" s="82"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="B83" s="85"/>
-      <c r="C83" s="74"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="82"/>
       <c r="E83" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="85" t="s">
         <v>309</v>
       </c>
-      <c r="B84" s="78"/>
-      <c r="C84" s="74"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="82"/>
       <c r="E84" t="s">
         <v>387</v>
       </c>
@@ -5110,11 +5625,11 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="77" t="s">
+      <c r="A86" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="B86" s="78"/>
-      <c r="C86" s="74"/>
+      <c r="B86" s="86"/>
+      <c r="C86" s="82"/>
       <c r="E86" t="s">
         <v>390</v>
       </c>
@@ -5123,8 +5638,8 @@
       <c r="A87" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B87" s="85"/>
-      <c r="C87" s="74"/>
+      <c r="B87" s="93"/>
+      <c r="C87" s="82"/>
       <c r="E87" t="s">
         <v>391</v>
       </c>
@@ -5133,8 +5648,8 @@
       <c r="A88" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B88" s="85"/>
-      <c r="C88" s="74"/>
+      <c r="B88" s="93"/>
+      <c r="C88" s="82"/>
       <c r="E88" t="s">
         <v>392</v>
       </c>
@@ -5143,8 +5658,8 @@
       <c r="A89" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B89" s="85"/>
-      <c r="C89" s="74"/>
+      <c r="B89" s="93"/>
+      <c r="C89" s="82"/>
       <c r="E89" t="s">
         <v>393</v>
       </c>
@@ -5153,43 +5668,43 @@
       <c r="A90" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B90" s="85"/>
-      <c r="C90" s="74"/>
+      <c r="B90" s="93"/>
+      <c r="C90" s="82"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B91" s="85"/>
-      <c r="C91" s="74"/>
+      <c r="B91" s="93"/>
+      <c r="C91" s="82"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B92" s="85"/>
-      <c r="C92" s="74"/>
+      <c r="B92" s="93"/>
+      <c r="C92" s="82"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B93" s="85"/>
-      <c r="C93" s="74"/>
+      <c r="B93" s="93"/>
+      <c r="C93" s="82"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B94" s="85"/>
-      <c r="C94" s="74"/>
+      <c r="B94" s="93"/>
+      <c r="C94" s="82"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B95" s="85"/>
-      <c r="C95" s="74"/>
+      <c r="B95" s="93"/>
+      <c r="C95" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -5374,18 +5889,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="82"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
@@ -5409,36 +5924,36 @@
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="74"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="82"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="74"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="82"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="82"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="74"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="82"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="74"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="82"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
@@ -5543,8 +6058,8 @@
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="74"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="82"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
@@ -5556,25 +6071,25 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="74"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="82"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="82"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="82"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
@@ -5688,15 +6203,15 @@
       <c r="A38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="86"/>
-      <c r="C38" s="74"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="82"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="77" t="s">
+      <c r="A39" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="78"/>
-      <c r="C39" s="74"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="82"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
@@ -5708,74 +6223,74 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="78"/>
-      <c r="C41" s="74"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="82"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="85"/>
-      <c r="C42" s="74"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="82"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="85"/>
-      <c r="C43" s="74"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="82"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="85"/>
-      <c r="C44" s="74"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="82"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="85"/>
-      <c r="C45" s="74"/>
+      <c r="B45" s="93"/>
+      <c r="C45" s="82"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="85"/>
-      <c r="C46" s="74"/>
+      <c r="B46" s="93"/>
+      <c r="C46" s="82"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="85"/>
-      <c r="C47" s="74"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="82"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="85"/>
-      <c r="C48" s="74"/>
+      <c r="B48" s="93"/>
+      <c r="C48" s="82"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="85"/>
-      <c r="C49" s="74"/>
+      <c r="B49" s="93"/>
+      <c r="C49" s="82"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="74"/>
+      <c r="B50" s="93"/>
+      <c r="C50" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -6474,11 +6989,11 @@
       <c r="A68" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B68" s="102" t="str">
+      <c r="B68" s="110" t="str">
         <f>"td_Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
         <v xml:space="preserve">td_Cost And Freight (CFR) , , </v>
       </c>
-      <c r="C68" s="74"/>
+      <c r="C68" s="82"/>
       <c r="D68" s="38" t="s">
         <v>178</v>
       </c>
@@ -6489,13 +7004,13 @@
       <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:12" ht="34.200000000000003" customHeight="1">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="100" t="s">
+      <c r="B69" s="108" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="74"/>
+      <c r="C69" s="82"/>
       <c r="D69" s="37" t="s">
         <v>181</v>
       </c>
@@ -6506,11 +7021,11 @@
       <c r="I69" s="37"/>
     </row>
     <row r="70" spans="1:12" ht="30" customHeight="1">
-      <c r="A70" s="95"/>
-      <c r="B70" s="91" t="s">
+      <c r="A70" s="103"/>
+      <c r="B70" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="C70" s="74"/>
+      <c r="C70" s="82"/>
       <c r="D70" s="37" t="s">
         <v>183</v>
       </c>
@@ -6521,11 +7036,11 @@
       <c r="I70" s="37"/>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A71" s="95"/>
-      <c r="B71" s="91" t="s">
+      <c r="A71" s="103"/>
+      <c r="B71" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="74"/>
+      <c r="C71" s="82"/>
       <c r="D71" s="37" t="s">
         <v>185</v>
       </c>
@@ -6536,11 +7051,11 @@
       <c r="I71" s="37"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A72" s="96"/>
-      <c r="B72" s="91" t="s">
+      <c r="A72" s="104"/>
+      <c r="B72" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="74"/>
+      <c r="C72" s="82"/>
       <c r="D72" s="37" t="s">
         <v>187</v>
       </c>
@@ -6554,11 +7069,11 @@
       <c r="A73" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="99" t="str">
+      <c r="B73" s="107" t="str">
         <f>J73&amp;K73&amp;L73</f>
         <v>td_All invoices are due and payable at the specified payment date or [invalid payment term] after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
       </c>
-      <c r="C73" s="74"/>
+      <c r="C73" s="82"/>
       <c r="D73" s="38" t="s">
         <v>189</v>
       </c>
@@ -6584,147 +7099,147 @@
       <c r="A74" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B74" s="92" t="s">
+      <c r="B74" s="100" t="s">
         <v>193</v>
       </c>
-      <c r="C74" s="74"/>
+      <c r="C74" s="82"/>
     </row>
     <row r="75" spans="1:12" ht="14.4" customHeight="1">
       <c r="A75" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="100" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="74"/>
+      <c r="C75" s="82"/>
     </row>
     <row r="76" spans="1:12" ht="28.2" customHeight="1">
-      <c r="A76" s="97" t="s">
+      <c r="A76" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="89" t="s">
+      <c r="B76" s="97" t="s">
         <v>197</v>
       </c>
-      <c r="C76" s="74"/>
+      <c r="C76" s="82"/>
     </row>
     <row r="77" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A77" s="95"/>
-      <c r="B77" s="93" t="s">
+      <c r="A77" s="103"/>
+      <c r="B77" s="101" t="s">
         <v>198</v>
       </c>
-      <c r="C77" s="74"/>
+      <c r="C77" s="82"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="95"/>
-      <c r="B78" s="93" t="s">
+      <c r="A78" s="103"/>
+      <c r="B78" s="101" t="s">
         <v>199</v>
       </c>
-      <c r="C78" s="74"/>
+      <c r="C78" s="82"/>
     </row>
     <row r="79" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A79" s="95"/>
-      <c r="B79" s="93" t="s">
+      <c r="A79" s="103"/>
+      <c r="B79" s="101" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="74"/>
+      <c r="C79" s="82"/>
     </row>
     <row r="80" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A80" s="95"/>
-      <c r="B80" s="93" t="s">
+      <c r="A80" s="103"/>
+      <c r="B80" s="101" t="s">
         <v>201</v>
       </c>
-      <c r="C80" s="74"/>
+      <c r="C80" s="82"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A81" s="95"/>
-      <c r="B81" s="89" t="s">
+      <c r="A81" s="103"/>
+      <c r="B81" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="74"/>
+      <c r="C81" s="82"/>
     </row>
     <row r="82" spans="1:3" ht="41.4" customHeight="1">
-      <c r="A82" s="95"/>
-      <c r="B82" s="98" t="s">
+      <c r="A82" s="103"/>
+      <c r="B82" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="C82" s="74"/>
+      <c r="C82" s="82"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A83" s="95"/>
-      <c r="B83" s="89" t="s">
+      <c r="A83" s="103"/>
+      <c r="B83" s="97" t="s">
         <v>204</v>
       </c>
-      <c r="C83" s="74"/>
+      <c r="C83" s="82"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A84" s="95"/>
-      <c r="B84" s="93" t="s">
+      <c r="A84" s="103"/>
+      <c r="B84" s="101" t="s">
         <v>205</v>
       </c>
-      <c r="C84" s="74"/>
+      <c r="C84" s="82"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="95"/>
-      <c r="B85" s="93" t="s">
+      <c r="A85" s="103"/>
+      <c r="B85" s="101" t="s">
         <v>206</v>
       </c>
-      <c r="C85" s="74"/>
+      <c r="C85" s="82"/>
     </row>
     <row r="86" spans="1:3" ht="33.6" customHeight="1">
-      <c r="A86" s="95"/>
-      <c r="B86" s="93" t="s">
+      <c r="A86" s="103"/>
+      <c r="B86" s="101" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="74"/>
+      <c r="C86" s="82"/>
     </row>
     <row r="87" spans="1:3" ht="31.2" customHeight="1">
-      <c r="A87" s="95"/>
-      <c r="B87" s="93" t="s">
+      <c r="A87" s="103"/>
+      <c r="B87" s="101" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="74"/>
+      <c r="C87" s="82"/>
     </row>
     <row r="88" spans="1:3" ht="48.6" customHeight="1">
-      <c r="A88" s="95"/>
-      <c r="B88" s="89" t="s">
+      <c r="A88" s="103"/>
+      <c r="B88" s="97" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="74"/>
+      <c r="C88" s="82"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="96"/>
-      <c r="B89" s="89" t="s">
+      <c r="A89" s="104"/>
+      <c r="B89" s="97" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="74"/>
+      <c r="C89" s="82"/>
     </row>
     <row r="90" spans="1:3" ht="30.6" customHeight="1">
-      <c r="A90" s="97" t="s">
+      <c r="A90" s="105" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="89" t="s">
+      <c r="B90" s="97" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="74"/>
+      <c r="C90" s="82"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="96"/>
-      <c r="B91" s="89" t="s">
+      <c r="A91" s="104"/>
+      <c r="B91" s="97" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="74"/>
+      <c r="C91" s="82"/>
     </row>
     <row r="92" spans="1:3" ht="55.2" customHeight="1">
-      <c r="A92" s="101" t="s">
+      <c r="A92" s="109" t="s">
         <v>214</v>
       </c>
-      <c r="B92" s="92" t="s">
+      <c r="B92" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="74"/>
+      <c r="C92" s="82"/>
     </row>
     <row r="93" spans="1:3" ht="28.8" customHeight="1">
-      <c r="A93" s="95"/>
+      <c r="A93" s="103"/>
       <c r="B93" s="34" t="s">
         <v>216</v>
       </c>
@@ -6733,7 +7248,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="95"/>
+      <c r="A94" s="103"/>
       <c r="B94" s="34" t="s">
         <v>218</v>
       </c>
@@ -6742,7 +7257,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="95"/>
+      <c r="A95" s="103"/>
       <c r="B95" s="34" t="s">
         <v>220</v>
       </c>
@@ -6751,7 +7266,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="95"/>
+      <c r="A96" s="103"/>
       <c r="B96" s="34" t="s">
         <v>222</v>
       </c>
@@ -6760,7 +7275,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="95"/>
+      <c r="A97" s="103"/>
       <c r="B97" s="34" t="s">
         <v>224</v>
       </c>
@@ -6769,7 +7284,7 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="96"/>
+      <c r="A98" s="104"/>
       <c r="B98" s="34" t="s">
         <v>226</v>
       </c>
@@ -6781,37 +7296,37 @@
       <c r="A99" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B99" s="92" t="s">
+      <c r="B99" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="74"/>
+      <c r="C99" s="82"/>
     </row>
     <row r="100" spans="1:3" ht="30" customHeight="1">
       <c r="A100" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="90" t="s">
+      <c r="B100" s="98" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="74"/>
+      <c r="C100" s="82"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="92" t="s">
+      <c r="B101" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="C101" s="74"/>
+      <c r="C101" s="82"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="92" t="s">
+      <c r="B102" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="74"/>
+      <c r="C102" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -7018,7 +7533,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7215,6 +7730,2156 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4F2126-D3AA-4FAD-B204-2AEC4B5DBC7F}">
+  <dimension ref="A1:E126"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="77.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6">
+      <c r="A1" s="77" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6">
+      <c r="A2" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2" s="76"/>
+      <c r="E2" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6">
+      <c r="A3" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>441</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E3" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6">
+      <c r="A4" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>442</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>463</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>458</v>
+      </c>
+      <c r="E4" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6">
+      <c r="A5" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C5" s="75">
+        <v>10</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>459</v>
+      </c>
+      <c r="E5" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6">
+      <c r="A6" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C6" s="75">
+        <v>20</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E6" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6">
+      <c r="A7" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C7" s="75">
+        <v>3</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E7" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6">
+      <c r="A8" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>384</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>464</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E8" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6">
+      <c r="A9" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>446</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E9" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6">
+      <c r="A10" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>447</v>
+      </c>
+      <c r="C10" s="75" t="s">
+        <v>466</v>
+      </c>
+      <c r="D10" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E10" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6">
+      <c r="A11" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>448</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>467</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E11" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6">
+      <c r="A12" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>449</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>464</v>
+      </c>
+      <c r="D12" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E12" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.6">
+      <c r="A13" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>450</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>468</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E13" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.6">
+      <c r="A14" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>451</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>464</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E14" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.6">
+      <c r="A15" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>452</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="D15" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E15" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.6">
+      <c r="A16" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>453</v>
+      </c>
+      <c r="C16" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E16" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.6">
+      <c r="A17" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>454</v>
+      </c>
+      <c r="C17" s="75">
+        <v>0</v>
+      </c>
+      <c r="D17" s="74" t="s">
+        <v>460</v>
+      </c>
+      <c r="E17" s="73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.6">
+      <c r="A18" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C18" s="75">
+        <v>0</v>
+      </c>
+      <c r="D18" s="74" t="s">
+        <v>460</v>
+      </c>
+      <c r="E18" s="73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.6">
+      <c r="A19" s="73" t="s">
+        <v>388</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>456</v>
+      </c>
+      <c r="C19" s="75" t="s">
+        <v>470</v>
+      </c>
+      <c r="D19" s="76"/>
+      <c r="E19" s="73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.6">
+      <c r="A20" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="75" t="s">
+        <v>461</v>
+      </c>
+      <c r="D20" s="80"/>
+      <c r="E20" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.6">
+      <c r="A21" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>471</v>
+      </c>
+      <c r="C21" s="75" t="s">
+        <v>462</v>
+      </c>
+      <c r="D21" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E21" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.6">
+      <c r="A22" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>442</v>
+      </c>
+      <c r="C22" s="75" t="s">
+        <v>463</v>
+      </c>
+      <c r="D22" s="74" t="s">
+        <v>458</v>
+      </c>
+      <c r="E22" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.6">
+      <c r="A23" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C23" s="75">
+        <v>10</v>
+      </c>
+      <c r="D23" s="74" t="s">
+        <v>459</v>
+      </c>
+      <c r="E23" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.6">
+      <c r="A24" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C24" s="75">
+        <v>20</v>
+      </c>
+      <c r="D24" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E24" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.6">
+      <c r="A25" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C25" s="75">
+        <v>3</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E25" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.6">
+      <c r="A26" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>472</v>
+      </c>
+      <c r="C26" s="75" t="s">
+        <v>464</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E26" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.6">
+      <c r="A27" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>473</v>
+      </c>
+      <c r="C27" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D27" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E27" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.6">
+      <c r="A28" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>474</v>
+      </c>
+      <c r="C28" s="75" t="s">
+        <v>466</v>
+      </c>
+      <c r="D28" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E28" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.6">
+      <c r="A29" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>454</v>
+      </c>
+      <c r="C29" s="75">
+        <v>0</v>
+      </c>
+      <c r="D29" s="74" t="s">
+        <v>460</v>
+      </c>
+      <c r="E29" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.6">
+      <c r="A30" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C30" s="75">
+        <v>0</v>
+      </c>
+      <c r="D30" s="74" t="s">
+        <v>460</v>
+      </c>
+      <c r="E30" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.6">
+      <c r="A31" s="73" t="s">
+        <v>387</v>
+      </c>
+      <c r="B31" s="74" t="s">
+        <v>456</v>
+      </c>
+      <c r="C31" s="75" t="s">
+        <v>470</v>
+      </c>
+      <c r="D31" s="80"/>
+      <c r="E31" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.6">
+      <c r="A32" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B32" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C32" s="113" t="s">
+        <v>501</v>
+      </c>
+      <c r="D32" s="80"/>
+      <c r="E32" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.6">
+      <c r="A33" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B33" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C33" s="75">
+        <v>30</v>
+      </c>
+      <c r="D33" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E33" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.6">
+      <c r="A34" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>476</v>
+      </c>
+      <c r="C34" s="75">
+        <v>100</v>
+      </c>
+      <c r="D34" s="74" t="s">
+        <v>458</v>
+      </c>
+      <c r="E34" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.6">
+      <c r="A35" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="C35" s="75">
+        <v>30</v>
+      </c>
+      <c r="D35" s="74" t="s">
+        <v>459</v>
+      </c>
+      <c r="E35" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.6">
+      <c r="A36" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>478</v>
+      </c>
+      <c r="C36" s="75">
+        <v>5</v>
+      </c>
+      <c r="D36" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E36" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.6">
+      <c r="A37" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B37" s="74" t="s">
+        <v>479</v>
+      </c>
+      <c r="C37" s="75">
+        <v>10</v>
+      </c>
+      <c r="D37" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E37" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.6">
+      <c r="A38" s="73" t="s">
+        <v>389</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C38" s="75">
+        <v>3000</v>
+      </c>
+      <c r="D38" s="74" t="s">
+        <v>480</v>
+      </c>
+      <c r="E38" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.6">
+      <c r="A39" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B39" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C39" s="113" t="s">
+        <v>501</v>
+      </c>
+      <c r="D39" s="80"/>
+      <c r="E39" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.6">
+      <c r="A40" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B40" s="74" t="s">
+        <v>471</v>
+      </c>
+      <c r="C40" s="75">
+        <v>1000</v>
+      </c>
+      <c r="D40" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E40" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.6">
+      <c r="A41" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B41" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="C41" s="75">
+        <v>40</v>
+      </c>
+      <c r="D41" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E41" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.6">
+      <c r="A42" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C42" s="75">
+        <v>15</v>
+      </c>
+      <c r="D42" s="74" t="s">
+        <v>481</v>
+      </c>
+      <c r="E42" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.6">
+      <c r="A43" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C43" s="75">
+        <v>2</v>
+      </c>
+      <c r="D43" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E43" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.6">
+      <c r="A44" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>476</v>
+      </c>
+      <c r="C44" s="75">
+        <v>10</v>
+      </c>
+      <c r="D44" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E44" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.6">
+      <c r="A45" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B45" s="74" t="s">
+        <v>482</v>
+      </c>
+      <c r="C45" s="75">
+        <v>6</v>
+      </c>
+      <c r="D45" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E45" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.6">
+      <c r="A46" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B46" s="74" t="s">
+        <v>483</v>
+      </c>
+      <c r="C46" s="75">
+        <v>300</v>
+      </c>
+      <c r="D46" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E46" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.6">
+      <c r="A47" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B47" s="74" t="s">
+        <v>484</v>
+      </c>
+      <c r="C47" s="75">
+        <v>300</v>
+      </c>
+      <c r="D47" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E47" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.6">
+      <c r="A48" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B48" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C48" s="75">
+        <v>10</v>
+      </c>
+      <c r="D48" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E48" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.6">
+      <c r="A49" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C49" s="75" t="s">
+        <v>485</v>
+      </c>
+      <c r="D49" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E49" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.6">
+      <c r="A50" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B50" s="74" t="s">
+        <v>479</v>
+      </c>
+      <c r="C50" s="75" t="s">
+        <v>466</v>
+      </c>
+      <c r="D50" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E50" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.6">
+      <c r="A51" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B51" s="74" t="s">
+        <v>486</v>
+      </c>
+      <c r="C51" s="75">
+        <v>15</v>
+      </c>
+      <c r="D51" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E51" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.6">
+      <c r="A52" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B52" s="74" t="s">
+        <v>487</v>
+      </c>
+      <c r="C52" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D52" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E52" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.6">
+      <c r="A53" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B53" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="C53" s="75">
+        <v>1</v>
+      </c>
+      <c r="D53" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E53" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.6">
+      <c r="A54" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B54" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="C54" s="75" t="s">
+        <v>490</v>
+      </c>
+      <c r="D54" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E54" s="73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.6">
+      <c r="A55" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B55" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C55" s="75" t="s">
+        <v>492</v>
+      </c>
+      <c r="D55" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E55" s="73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.6">
+      <c r="A56" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B56" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="C56" s="75" t="s">
+        <v>494</v>
+      </c>
+      <c r="D56" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E56" s="73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.6">
+      <c r="A57" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B57" s="74" t="s">
+        <v>495</v>
+      </c>
+      <c r="C57" s="75">
+        <v>1</v>
+      </c>
+      <c r="D57" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E57" s="73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.6">
+      <c r="A58" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B58" s="74" t="s">
+        <v>496</v>
+      </c>
+      <c r="C58" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D58" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E58" s="73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.6">
+      <c r="A59" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B59" s="74" t="s">
+        <v>497</v>
+      </c>
+      <c r="C59" s="75">
+        <v>100</v>
+      </c>
+      <c r="D59" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E59" s="73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.6">
+      <c r="A60" s="73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B60" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C60" s="75">
+        <v>1000</v>
+      </c>
+      <c r="D60" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E60" s="73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.6">
+      <c r="A61" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B61" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C61" s="113" t="s">
+        <v>501</v>
+      </c>
+      <c r="D61" s="80"/>
+      <c r="E61" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.6">
+      <c r="A62" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B62" s="74" t="s">
+        <v>441</v>
+      </c>
+      <c r="C62" s="75">
+        <v>1000</v>
+      </c>
+      <c r="D62" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E62" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.6">
+      <c r="A63" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B63" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="C63" s="75">
+        <v>50</v>
+      </c>
+      <c r="D63" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E63" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.6">
+      <c r="A64" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C64" s="75">
+        <v>50</v>
+      </c>
+      <c r="D64" s="74" t="s">
+        <v>481</v>
+      </c>
+      <c r="E64" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.6">
+      <c r="A65" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B65" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C65" s="75">
+        <v>3</v>
+      </c>
+      <c r="D65" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E65" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.6">
+      <c r="A66" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B66" s="74" t="s">
+        <v>476</v>
+      </c>
+      <c r="C66" s="75">
+        <v>25</v>
+      </c>
+      <c r="D66" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E66" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.6">
+      <c r="A67" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B67" s="74" t="s">
+        <v>482</v>
+      </c>
+      <c r="C67" s="75">
+        <v>4</v>
+      </c>
+      <c r="D67" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E67" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.6">
+      <c r="A68" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B68" s="74" t="s">
+        <v>483</v>
+      </c>
+      <c r="C68" s="75">
+        <v>300</v>
+      </c>
+      <c r="D68" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E68" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.6">
+      <c r="A69" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B69" s="74" t="s">
+        <v>484</v>
+      </c>
+      <c r="C69" s="75">
+        <v>300</v>
+      </c>
+      <c r="D69" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E69" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.6">
+      <c r="A70" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B70" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C70" s="75">
+        <v>10</v>
+      </c>
+      <c r="D70" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E70" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.6">
+      <c r="A71" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B71" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C71" s="75" t="s">
+        <v>485</v>
+      </c>
+      <c r="D71" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.6">
+      <c r="A72" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B72" s="74" t="s">
+        <v>479</v>
+      </c>
+      <c r="C72" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D72" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E72" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.6">
+      <c r="A73" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B73" s="74" t="s">
+        <v>486</v>
+      </c>
+      <c r="C73" s="75">
+        <v>15</v>
+      </c>
+      <c r="D73" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E73" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.6">
+      <c r="A74" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B74" s="74" t="s">
+        <v>487</v>
+      </c>
+      <c r="C74" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D74" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E74" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.6">
+      <c r="A75" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B75" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="C75" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="D75" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E75" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.6">
+      <c r="A76" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B76" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="C76" s="75" t="s">
+        <v>490</v>
+      </c>
+      <c r="D76" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E76" s="73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.6">
+      <c r="A77" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B77" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C77" s="75" t="s">
+        <v>492</v>
+      </c>
+      <c r="D77" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E77" s="73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.6">
+      <c r="A78" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B78" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="C78" s="75" t="s">
+        <v>494</v>
+      </c>
+      <c r="D78" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E78" s="73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.6">
+      <c r="A79" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B79" s="74" t="s">
+        <v>495</v>
+      </c>
+      <c r="C79" s="75">
+        <v>1</v>
+      </c>
+      <c r="D79" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E79" s="73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.6">
+      <c r="A80" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B80" s="74" t="s">
+        <v>496</v>
+      </c>
+      <c r="C80" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D80" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E80" s="73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.6">
+      <c r="A81" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B81" s="74" t="s">
+        <v>497</v>
+      </c>
+      <c r="C81" s="75">
+        <v>1000</v>
+      </c>
+      <c r="D81" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E81" s="73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.6">
+      <c r="A82" s="73" t="s">
+        <v>391</v>
+      </c>
+      <c r="B82" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C82" s="75">
+        <v>5000</v>
+      </c>
+      <c r="D82" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E82" s="73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.6">
+      <c r="A83" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C83" s="113" t="s">
+        <v>501</v>
+      </c>
+      <c r="D83" s="80"/>
+      <c r="E83" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.6">
+      <c r="A84" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B84" s="74" t="s">
+        <v>441</v>
+      </c>
+      <c r="C84" s="75">
+        <v>1000</v>
+      </c>
+      <c r="D84" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E84" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.6">
+      <c r="A85" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B85" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="C85" s="75">
+        <v>100</v>
+      </c>
+      <c r="D85" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E85" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.6">
+      <c r="A86" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B86" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C86" s="75">
+        <v>100</v>
+      </c>
+      <c r="D86" s="74" t="s">
+        <v>481</v>
+      </c>
+      <c r="E86" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.6">
+      <c r="A87" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B87" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C87" s="75">
+        <v>6</v>
+      </c>
+      <c r="D87" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E87" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.6">
+      <c r="A88" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B88" s="74" t="s">
+        <v>476</v>
+      </c>
+      <c r="C88" s="75">
+        <v>40</v>
+      </c>
+      <c r="D88" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E88" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.6">
+      <c r="A89" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B89" s="74" t="s">
+        <v>482</v>
+      </c>
+      <c r="C89" s="75">
+        <v>3</v>
+      </c>
+      <c r="D89" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E89" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.6">
+      <c r="A90" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B90" s="74" t="s">
+        <v>483</v>
+      </c>
+      <c r="C90" s="75">
+        <v>300</v>
+      </c>
+      <c r="D90" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E90" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.6">
+      <c r="A91" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B91" s="74" t="s">
+        <v>484</v>
+      </c>
+      <c r="C91" s="75">
+        <v>300</v>
+      </c>
+      <c r="D91" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E91" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.6">
+      <c r="A92" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B92" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C92" s="75">
+        <v>20</v>
+      </c>
+      <c r="D92" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E92" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.6">
+      <c r="A93" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B93" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C93" s="75" t="s">
+        <v>485</v>
+      </c>
+      <c r="D93" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E93" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.6">
+      <c r="A94" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B94" s="74" t="s">
+        <v>479</v>
+      </c>
+      <c r="C94" s="75" t="s">
+        <v>499</v>
+      </c>
+      <c r="D94" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E94" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.6">
+      <c r="A95" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B95" s="74" t="s">
+        <v>486</v>
+      </c>
+      <c r="C95" s="75">
+        <v>25</v>
+      </c>
+      <c r="D95" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E95" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.6">
+      <c r="A96" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B96" s="74" t="s">
+        <v>487</v>
+      </c>
+      <c r="C96" s="75">
+        <v>1</v>
+      </c>
+      <c r="D96" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E96" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15.6">
+      <c r="A97" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B97" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="C97" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="D97" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E97" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.6">
+      <c r="A98" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B98" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="C98" s="75" t="s">
+        <v>490</v>
+      </c>
+      <c r="D98" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E98" s="73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.6">
+      <c r="A99" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B99" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C99" s="75" t="s">
+        <v>492</v>
+      </c>
+      <c r="D99" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E99" s="73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15.6">
+      <c r="A100" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B100" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="C100" s="75" t="s">
+        <v>494</v>
+      </c>
+      <c r="D100" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E100" s="73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15.6">
+      <c r="A101" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B101" s="74" t="s">
+        <v>495</v>
+      </c>
+      <c r="C101" s="75">
+        <v>1</v>
+      </c>
+      <c r="D101" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E101" s="73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.6">
+      <c r="A102" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B102" s="74" t="s">
+        <v>496</v>
+      </c>
+      <c r="C102" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="D102" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E102" s="73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.6">
+      <c r="A103" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B103" s="74" t="s">
+        <v>497</v>
+      </c>
+      <c r="C103" s="75">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E103" s="73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.6">
+      <c r="A104" s="73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B104" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C104" s="75">
+        <v>10000</v>
+      </c>
+      <c r="D104" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E104" s="73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.6">
+      <c r="A105" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B105" s="74" t="s">
+        <v>440</v>
+      </c>
+      <c r="C105" s="113" t="s">
+        <v>501</v>
+      </c>
+      <c r="D105" s="80"/>
+      <c r="E105" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.6">
+      <c r="A106" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B106" s="74" t="s">
+        <v>441</v>
+      </c>
+      <c r="C106" s="75">
+        <v>2000</v>
+      </c>
+      <c r="D106" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E106" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.6">
+      <c r="A107" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B107" s="74" t="s">
+        <v>477</v>
+      </c>
+      <c r="C107" s="75">
+        <v>400</v>
+      </c>
+      <c r="D107" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E107" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.6">
+      <c r="A108" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B108" s="74" t="s">
+        <v>443</v>
+      </c>
+      <c r="C108" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D108" s="74" t="s">
+        <v>481</v>
+      </c>
+      <c r="E108" s="73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15.6">
+      <c r="A109" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B109" s="74" t="s">
+        <v>475</v>
+      </c>
+      <c r="C109" s="75">
+        <v>12</v>
+      </c>
+      <c r="D109" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E109" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15.6">
+      <c r="A110" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B110" s="74" t="s">
+        <v>476</v>
+      </c>
+      <c r="C110" s="75">
+        <v>80</v>
+      </c>
+      <c r="D110" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E110" s="73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15.6">
+      <c r="A111" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B111" s="74" t="s">
+        <v>482</v>
+      </c>
+      <c r="C111" s="75">
+        <v>1</v>
+      </c>
+      <c r="D111" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E111" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15.6">
+      <c r="A112" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B112" s="74" t="s">
+        <v>483</v>
+      </c>
+      <c r="C112" s="75">
+        <v>400</v>
+      </c>
+      <c r="D112" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E112" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15.6">
+      <c r="A113" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B113" s="74" t="s">
+        <v>484</v>
+      </c>
+      <c r="C113" s="75">
+        <v>600</v>
+      </c>
+      <c r="D113" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E113" s="73">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15.6">
+      <c r="A114" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B114" s="74" t="s">
+        <v>444</v>
+      </c>
+      <c r="C114" s="75">
+        <v>20</v>
+      </c>
+      <c r="D114" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E114" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15.6">
+      <c r="A115" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B115" s="74" t="s">
+        <v>445</v>
+      </c>
+      <c r="C115" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D115" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E115" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="15.6">
+      <c r="A116" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B116" s="74" t="s">
+        <v>479</v>
+      </c>
+      <c r="C116" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D116" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E116" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15.6">
+      <c r="A117" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B117" s="74" t="s">
+        <v>486</v>
+      </c>
+      <c r="C117" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D117" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E117" s="73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15.6">
+      <c r="A118" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B118" s="74" t="s">
+        <v>487</v>
+      </c>
+      <c r="C118" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D118" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E118" s="73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15.6">
+      <c r="A119" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B119" s="74" t="s">
+        <v>488</v>
+      </c>
+      <c r="C119" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D119" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E119" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15.6">
+      <c r="A120" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B120" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="C120" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D120" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E120" s="73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15.6">
+      <c r="A121" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B121" s="74" t="s">
+        <v>491</v>
+      </c>
+      <c r="C121" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D121" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E121" s="73">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15.6">
+      <c r="A122" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B122" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="C122" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D122" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E122" s="73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15.6">
+      <c r="A123" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B123" s="74" t="s">
+        <v>495</v>
+      </c>
+      <c r="C123" s="75">
+        <v>10</v>
+      </c>
+      <c r="D123" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E123" s="73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15.6">
+      <c r="A124" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B124" s="74" t="s">
+        <v>496</v>
+      </c>
+      <c r="C124" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="D124" s="74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E124" s="73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="15.6">
+      <c r="A125" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B125" s="74" t="s">
+        <v>497</v>
+      </c>
+      <c r="C125" s="75">
+        <v>2000</v>
+      </c>
+      <c r="D125" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E125" s="73">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15.6">
+      <c r="A126" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="B126" s="74" t="s">
+        <v>455</v>
+      </c>
+      <c r="C126" s="75">
+        <v>10000</v>
+      </c>
+      <c r="D126" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="E126" s="73">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7232,7 +9897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7247,19 +9912,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: change references cell flow
</commit_message>
<xml_diff>
--- a/data/SET_BDU.xlsx
+++ b/data/SET_BDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIAC-V\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE2A19-268B-4DBB-938E-8EFE211C4422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19393ABE-E9AE-404D-8E16-BB9123C562C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="687" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="687" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIP_Customer Information" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="503">
   <si>
     <t>sub_CUSTOMER INFORMATION</t>
   </si>
@@ -1452,15 +1452,9 @@
     <t>GRUNDFOS</t>
   </si>
   <si>
-    <t>fd_Type</t>
-  </si>
-  <si>
     <t>End Suction Centrifugal Pump</t>
   </si>
   <si>
-    <t>fd_Model</t>
-  </si>
-  <si>
     <t>CR</t>
   </si>
   <si>
@@ -1714,6 +1708,15 @@
   </si>
   <si>
     <t>6-9</t>
+  </si>
+  <si>
+    <t>fd_Pump Type</t>
+  </si>
+  <si>
+    <t>fd_Pump Model</t>
+  </si>
+  <si>
+    <t>fd_Blower Type</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2066,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2283,6 +2286,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2369,9 +2375,10 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -3746,18 +3753,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.6" customHeight="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
     </row>
     <row r="2" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="82"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -3770,11 +3777,11 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="82"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
@@ -3790,8 +3797,8 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="82"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3807,8 +3814,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -3824,8 +3831,8 @@
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="82"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -3838,11 +3845,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="82"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3858,8 +3865,8 @@
       <c r="A8" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="82"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="83"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3872,8 +3879,8 @@
       <c r="A9" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="83"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3886,8 +3893,8 @@
       <c r="A10" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="83"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3900,8 +3907,8 @@
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="82"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3917,8 +3924,8 @@
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="82"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -3934,8 +3941,8 @@
       <c r="A13" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="82"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="83"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3945,11 +3952,11 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="82"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="83"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -4107,8 +4114,8 @@
       <c r="A24" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="82"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -4118,11 +4125,11 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A25" s="85" t="s">
+      <c r="A25" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="82"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -4138,8 +4145,8 @@
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="90"/>
-      <c r="C26" s="82"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -4152,11 +4159,11 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="86"/>
-      <c r="C27" s="82"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="83"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -4172,8 +4179,8 @@
       <c r="A28" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="82"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="83"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -4186,8 +4193,8 @@
       <c r="A29" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="83"/>
-      <c r="C29" s="82"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="83"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -4200,8 +4207,8 @@
       <c r="A30" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="82"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="83"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -4214,8 +4221,8 @@
       <c r="A31" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="84"/>
-      <c r="C31" s="82"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -4231,8 +4238,8 @@
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="87"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -4248,8 +4255,8 @@
       <c r="A33" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B33" s="84"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="83"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -4386,8 +4393,8 @@
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="82"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="83"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -4397,11 +4404,11 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" ht="13.2" customHeight="1">
-      <c r="A43" s="85" t="s">
+      <c r="A43" s="86" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="86"/>
-      <c r="C43" s="82"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="83"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -4414,8 +4421,8 @@
       <c r="A44" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="B44" s="83"/>
-      <c r="C44" s="82"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="83"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -4428,8 +4435,8 @@
       <c r="A45" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="83"/>
-      <c r="C45" s="82"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="83"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -4442,15 +4449,15 @@
       <c r="A46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="83"/>
-      <c r="C46" s="82"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="83"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="83"/>
-      <c r="C47" s="82"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="83"/>
     </row>
     <row r="48" spans="1:14" ht="13.2" customHeight="1">
       <c r="H48" s="1"/>
@@ -4544,18 +4551,18 @@
       <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="112" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="113" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="82"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="83"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="52" t="s">
@@ -4612,11 +4619,11 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="113" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="83"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
@@ -4637,11 +4644,11 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="112" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
@@ -4723,16 +4730,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="69" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="69" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="48.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.109375" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -4742,12 +4749,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -5151,212 +5158,206 @@
         <v>396</v>
       </c>
       <c r="B42" s="71"/>
-      <c r="C42" s="24" t="s">
-        <v>414</v>
-      </c>
-      <c r="D42" s="71"/>
+      <c r="D42" s="6"/>
       <c r="G42" t="s">
         <v>413</v>
       </c>
       <c r="H42" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I42" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="69"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="D43" s="72"/>
+      <c r="A43" s="24" t="s">
+        <v>500</v>
+      </c>
+      <c r="B43" s="71"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="6"/>
       <c r="G43" t="s">
         <v>413</v>
       </c>
       <c r="H43" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I43" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="69" t="s">
-        <v>397</v>
-      </c>
-      <c r="B44" s="71"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="24" t="s">
+        <v>501</v>
+      </c>
+      <c r="B44" s="72"/>
       <c r="D44" s="6"/>
       <c r="G44" t="s">
         <v>413</v>
       </c>
       <c r="H44" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I44" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="69" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B45" s="71"/>
-      <c r="C45" s="24" t="s">
-        <v>414</v>
-      </c>
-      <c r="D45" s="71"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
       <c r="G45" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H45" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I45" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="69" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B46" s="71"/>
-      <c r="C46" s="6"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="6"/>
       <c r="G46" t="s">
+        <v>418</v>
+      </c>
+      <c r="H46" t="s">
+        <v>414</v>
+      </c>
+      <c r="I46" t="s">
         <v>420</v>
       </c>
-      <c r="H46" t="s">
-        <v>415</v>
-      </c>
-      <c r="I46" t="s">
-        <v>422</v>
-      </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="69" t="s">
-        <v>400</v>
+      <c r="A47" s="24" t="s">
+        <v>502</v>
       </c>
       <c r="B47" s="71"/>
-      <c r="C47" s="6"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="6"/>
       <c r="G47" t="s">
+        <v>421</v>
+      </c>
+      <c r="H47" t="s">
         <v>423</v>
       </c>
-      <c r="H47" t="s">
-        <v>425</v>
-      </c>
       <c r="I47" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="69" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B48" s="71"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="G48" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H48" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I48" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="69" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B49" s="71"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="G49" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H49" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I49" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="69" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B50" s="71"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="G50" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H50" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I50" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="69" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="B51" s="71"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="G51" t="s">
+        <v>428</v>
+      </c>
+      <c r="H51" t="s">
+        <v>414</v>
+      </c>
+      <c r="I51" t="s">
         <v>430</v>
-      </c>
-      <c r="H51" t="s">
-        <v>415</v>
-      </c>
-      <c r="I51" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="69" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B52" s="71"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="G52" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H52" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I52" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="6" t="s">
-        <v>405</v>
+      <c r="A53" s="69" t="s">
+        <v>403</v>
       </c>
       <c r="B53" s="71"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="G53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H53" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I53" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="6" t="s">
-        <v>406</v>
+      <c r="A54" s="69" t="s">
+        <v>404</v>
       </c>
       <c r="B54" s="71"/>
       <c r="C54" s="6"/>
@@ -5364,7 +5365,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B55" s="71"/>
       <c r="C55" s="6"/>
@@ -5372,7 +5373,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B56" s="71"/>
       <c r="C56" s="6"/>
@@ -5380,7 +5381,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B57" s="71"/>
       <c r="C57" s="6"/>
@@ -5388,7 +5389,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B58" s="71"/>
       <c r="C58" s="6"/>
@@ -5396,103 +5397,101 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B59" s="71"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6">
-      <c r="A60" s="92" t="s">
+    <row r="60" spans="1:9">
+      <c r="A60" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B60" s="71"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B61" s="71"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.6">
+      <c r="A62" s="114" t="s">
         <v>268</v>
       </c>
-      <c r="B60" s="89"/>
-      <c r="C60" s="89"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="85" t="s">
+      <c r="B62" s="115"/>
+      <c r="C62" s="115"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="86"/>
-      <c r="C61" s="82"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="20" t="s">
-        <v>72</v>
-      </c>
+      <c r="B63" s="87"/>
+      <c r="C63" s="83"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="93"/>
-      <c r="C64" s="82"/>
+        <v>69</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="40" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" s="93"/>
-      <c r="C65" s="82"/>
+        <v>71</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="20" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" s="94" t="e">
-        <f>B70/B69</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C66" s="82"/>
+        <v>73</v>
+      </c>
+      <c r="B66" s="94"/>
+      <c r="C66" s="83"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" s="95"/>
-      <c r="C67" s="82"/>
+        <v>74</v>
+      </c>
+      <c r="B67" s="94"/>
+      <c r="C67" s="83"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="96"/>
-      <c r="C68" s="82"/>
+        <v>75</v>
+      </c>
+      <c r="B68" s="95" t="e">
+        <f>B72/B71</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C68" s="83"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B69" s="96"/>
+      <c r="C69" s="83"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="40" t="s">
-        <v>70</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B70" s="97"/>
+      <c r="C70" s="83"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="40" t="s">
@@ -5501,7 +5500,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="40" t="s">
@@ -5510,7 +5509,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="40" t="s">
@@ -5519,7 +5518,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="40" t="s">
@@ -5528,7 +5527,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="40" t="s">
@@ -5537,7 +5536,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="40" t="s">
@@ -5546,191 +5545,188 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B77" s="3"/>
-      <c r="C77" s="49" t="s">
-        <v>87</v>
+      <c r="C77" s="40" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="49" t="s">
-        <v>89</v>
+      <c r="C78" s="40" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" s="94"/>
-      <c r="C79" s="82"/>
+        <v>86</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="49" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" s="95"/>
+      <c r="C81" s="83"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="49" t="s">
+      <c r="B82" s="8"/>
+      <c r="C82" s="49" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="85" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="86"/>
-      <c r="C81" s="82"/>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="6" t="s">
+      <c r="B83" s="87"/>
+      <c r="C83" s="83"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B82" s="93"/>
-      <c r="C82" s="82"/>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="6" t="s">
+      <c r="B84" s="94"/>
+      <c r="C84" s="83"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="B83" s="93"/>
-      <c r="C83" s="82"/>
-      <c r="E83" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="85" t="s">
+      <c r="B85" s="94"/>
+      <c r="C85" s="83"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="86" t="s">
         <v>309</v>
       </c>
-      <c r="B84" s="86"/>
-      <c r="C84" s="82"/>
-      <c r="E84" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="6" t="s">
+      <c r="B86" s="87"/>
+      <c r="C86" s="83"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="21" t="s">
+      <c r="B87" s="22"/>
+      <c r="C87" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E85" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="85" t="s">
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="B86" s="86"/>
-      <c r="C86" s="82"/>
-      <c r="E86" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="6" t="s">
+      <c r="B88" s="87"/>
+      <c r="C88" s="83"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B87" s="93"/>
-      <c r="C87" s="82"/>
-      <c r="E87" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="6" t="s">
+      <c r="B89" s="94"/>
+      <c r="C89" s="83"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B88" s="93"/>
-      <c r="C88" s="82"/>
-      <c r="E88" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="6" t="s">
+      <c r="B90" s="94"/>
+      <c r="C90" s="83"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B89" s="93"/>
-      <c r="C89" s="82"/>
-      <c r="E89" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="6" t="s">
+      <c r="B91" s="94"/>
+      <c r="C91" s="83"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B90" s="93"/>
-      <c r="C90" s="82"/>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="6" t="s">
+      <c r="B92" s="94"/>
+      <c r="C92" s="83"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B91" s="93"/>
-      <c r="C91" s="82"/>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="6" t="s">
+      <c r="B93" s="94"/>
+      <c r="C93" s="83"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B92" s="93"/>
-      <c r="C92" s="82"/>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="6" t="s">
+      <c r="B94" s="94"/>
+      <c r="C94" s="83"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B93" s="93"/>
-      <c r="C93" s="82"/>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="6" t="s">
+      <c r="B95" s="94"/>
+      <c r="C95" s="83"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B94" s="93"/>
-      <c r="C94" s="82"/>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="6" t="s">
+      <c r="B96" s="94"/>
+      <c r="C96" s="83"/>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B95" s="93"/>
-      <c r="C95" s="82"/>
+      <c r="B97" s="94"/>
+      <c r="C97" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
     <mergeCell ref="B89:C89"/>
     <mergeCell ref="B90:C90"/>
     <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B84:C84"/>
     <mergeCell ref="A86:C86"/>
-    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:C63"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="43">
@@ -5785,82 +5781,80 @@
     <dataValidation type="date" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="B26:B29" xr:uid="{00000000-0002-0000-0100-000010000000}">
       <formula1>45658</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B67 D37:D40" xr:uid="{00000000-0002-0000-0100-000011000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B69 D37:D40" xr:uid="{00000000-0002-0000-0100-000011000000}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D23" xr:uid="{00000000-0002-0000-0100-000012000000}">
       <formula1>"14 days,30 days,45 days"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B64" xr:uid="{0E563FC6-D334-4102-80DB-B12A49BE4535}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B66" xr:uid="{0E563FC6-D334-4102-80DB-B12A49BE4535}">
       <formula1>"MESSOPHILIC,TERMOPHILIC"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B65" xr:uid="{0AE3CB1E-D3BA-43AD-973B-95AC5034F0ED}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B67" xr:uid="{0AE3CB1E-D3BA-43AD-973B-95AC5034F0ED}">
       <formula1>"RICH FOG&amp;TSS,RICH SUGAR LOW FOG&amp;TSS,NON BGD ORGANIC,NON ORGANIC,DOMESTIC WASTE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B82" xr:uid="{3CAFC935-D919-4CAE-99B4-C39E42BBAA48}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B84" xr:uid="{3CAFC935-D919-4CAE-99B4-C39E42BBAA48}">
       <formula1>"DISCHARGE ONLY,REUSE : G-3,REUSE : G-2,REUSE : G-1,REUSE : G-0"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B85" xr:uid="{722D38B0-FDF3-408F-A5A0-0137B25A2B6B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{722D38B0-FDF3-408F-A5A0-0137B25A2B6B}">
       <formula1>"75%-85%,60%-75%,40%-50%,&lt;40%"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B87:C95" xr:uid="{986438E4-27C9-4346-92EB-B2ED90C73F27}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B89:C97" xr:uid="{986438E4-27C9-4346-92EB-B2ED90C73F27}">
       <formula1>"INLET TANK,EQUALIZING,OWS,ANAFLOAT,INTERMEDIATE TANK,ANAPAK,AERATION,SECONDARY CLARIFIER,MMF,ACF,MPS,FINAL TANK,DAF,MBR,PRIMARY CLARIFIER,BWRO,CCRO,SWRO,ANAMEM,AOP,SMF"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B83:C83" xr:uid="{9ACE7AA9-3561-4482-B5AE-1CC8193A6502}">
-      <formula1>"PERMENKES No. 2 Tahun 2023 (Parameter Wajib Air Minum), PERMENKES No. 2 Tahun 2023 (Parameter Air untuk Keperluan Higiene dan Sanitasi),"</formula1>
-    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B85:C85" xr:uid="{9ACE7AA9-3561-4482-B5AE-1CC8193A6502}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B42" xr:uid="{D5B1539D-C275-45EB-9183-7885F42584B5}">
       <formula1>"GRUNDFOS,KSB,XYLEM,ITT GOULDS,EBARA,WILO,FLOWREX,CNP,LEO"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B41" xr:uid="{6D15CE87-D514-4C0B-81EB-0E4CE7F62C0E}">
       <formula1>"GRADE A,GRADE B,GRADE C,GRADE E"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{08B0867B-4945-4A65-BE3D-5208EFC4295B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B45" xr:uid="{08B0867B-4945-4A65-BE3D-5208EFC4295B}">
       <formula1>"PROMINENT,MILTON ROY,MLI,SEKO,FLOWREX,NEWDOSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B45" xr:uid="{97CF9C98-806A-40FD-8822-3FC73739DB15}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B46" xr:uid="{97CF9C98-806A-40FD-8822-3FC73739DB15}">
       <formula1>"ATLAS COPCO,AERZEN,ROBUSCHI,KAESER,ZGK,EURUS,CHANGHE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B46" xr:uid="{52BECC89-4D0B-4369-9F9A-553255C79538}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B48" xr:uid="{52BECC89-4D0B-4369-9F9A-553255C79538}">
       <formula1>"BOEEP,FLOWREX"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B49" xr:uid="{E95110B2-E6A7-4E57-AFB6-751FA4B95D57}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B51" xr:uid="{E95110B2-E6A7-4E57-AFB6-751FA4B95D57}">
       <formula1>"PENGUIN,CANATURE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B47:B48 B51:B52" xr:uid="{537E1950-1AC0-4F58-88BF-273D4E49D878}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B49:B50 B53:B54" xr:uid="{537E1950-1AC0-4F58-88BF-273D4E49D878}">
       <formula1>"FLOWREX"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B50" xr:uid="{85953944-4004-4CDE-BEBC-505E1555CDB8}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B52" xr:uid="{85953944-4004-4CDE-BEBC-505E1555CDB8}">
       <formula1>"TECHASE,BOEEP,FLOWREX"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B53" xr:uid="{7550BC07-BF3B-4F31-B1E3-60BABD90CC24}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B55" xr:uid="{7550BC07-BF3B-4F31-B1E3-60BABD90CC24}">
       <formula1>"ABB"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B54" xr:uid="{F0A0AB00-97BB-49CD-9227-DC23E45ABA85}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B56" xr:uid="{F0A0AB00-97BB-49CD-9227-DC23E45ABA85}">
       <formula1>"JAGGER,REHAU"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B55" xr:uid="{0503AAA6-CA9D-40A3-8F21-39E4043C5C8D}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{0503AAA6-CA9D-40A3-8F21-39E4043C5C8D}">
       <formula1>"SIEMENS,ALLEN-BRADLEY,SCHNEIDER,OMRON"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B56" xr:uid="{DEC920D3-5DEC-4C65-A781-E1E80973E12B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B58" xr:uid="{DEC920D3-5DEC-4C65-A781-E1E80973E12B}">
       <formula1>"SIEMENS,ALLEN-BRADLEY,SCHNEIDER,OMRON,HAIWELL,MCGS"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B57" xr:uid="{A792B851-F0D0-41CA-8C0E-6E7CC343A4CA}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{A792B851-F0D0-41CA-8C0E-6E7CC343A4CA}">
       <formula1>"DIAC-X,ENDRESS+HAUSER,WIKA,ARMATHERM,EMERSON,YOKOGAWA,VEGA"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B58" xr:uid="{65773699-45FC-42E7-9DA3-133CEF3C1BA2}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B60" xr:uid="{65773699-45FC-42E7-9DA3-133CEF3C1BA2}">
       <formula1>"SUPREME,JJLAP,ETERNA,LOCAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{D0BD5687-B728-4D47-8D29-FCF4E690F857}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B61" xr:uid="{D0BD5687-B728-4D47-8D29-FCF4E690F857}">
       <formula1>"SUPREME,JJLAP,LOCAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D45" xr:uid="{D51A701E-7350-4097-BB5C-841E8043FF45}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B47" xr:uid="{D51A701E-7350-4097-BB5C-841E8043FF45}">
       <formula1>"TURBO BLOWER,ROOTS BLOWER,SIDE CHANNEL BLOWER"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D42" xr:uid="{99A5EF61-B540-454C-B71C-2967FB1181D2}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B43" xr:uid="{99A5EF61-B540-454C-B71C-2967FB1181D2}">
       <formula1>"VERTICAL MULTISTAGE CENTRIFUGAL PUMP,END SUCTION CENTRIFUGAL PUMP,SUBMERSIBLE PUMP"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D43" xr:uid="{D1457EEC-A832-482F-B74F-3CFCBA2B89B5}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{D1457EEC-A832-482F-B74F-3CFCBA2B89B5}">
       <formula1>$I$42:$I$53</formula1>
     </dataValidation>
   </dataValidations>
@@ -5889,18 +5883,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="82"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
@@ -5924,36 +5918,36 @@
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="82"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="83"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="82"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="83"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="82"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="83"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="82"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="83"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
@@ -6058,8 +6052,8 @@
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="82"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="83"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
@@ -6071,25 +6065,25 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="85" t="s">
+      <c r="A23" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="86"/>
-      <c r="C23" s="82"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="83"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="82"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="83"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="82"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="83"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
@@ -6203,15 +6197,15 @@
       <c r="A38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="82"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="83"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="85" t="s">
+      <c r="A39" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="86"/>
-      <c r="C39" s="82"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="83"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
@@ -6223,74 +6217,74 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="82"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="83"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="93"/>
-      <c r="C42" s="82"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="93"/>
-      <c r="C43" s="82"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="83"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="93"/>
-      <c r="C44" s="82"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="83"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="93"/>
-      <c r="C45" s="82"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="83"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="93"/>
-      <c r="C46" s="82"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="83"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="82"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="83"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="93"/>
-      <c r="C48" s="82"/>
+      <c r="B48" s="94"/>
+      <c r="C48" s="83"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="93"/>
-      <c r="C49" s="82"/>
+      <c r="B49" s="94"/>
+      <c r="C49" s="83"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="93"/>
-      <c r="C50" s="82"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -6989,11 +6983,11 @@
       <c r="A68" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B68" s="110" t="str">
+      <c r="B68" s="111" t="str">
         <f>"td_Cost And Freight (CFR) " &amp; 'DIP_Customer Information'!B10 &amp; ", " &amp; 'DIP_Customer Information'!B9 &amp; ", " &amp; 'DIP_Customer Information'!B8</f>
         <v xml:space="preserve">td_Cost And Freight (CFR) , , </v>
       </c>
-      <c r="C68" s="82"/>
+      <c r="C68" s="83"/>
       <c r="D68" s="38" t="s">
         <v>178</v>
       </c>
@@ -7004,13 +6998,13 @@
       <c r="I68" s="37"/>
     </row>
     <row r="69" spans="1:12" ht="34.200000000000003" customHeight="1">
-      <c r="A69" s="102" t="s">
+      <c r="A69" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="B69" s="108" t="s">
+      <c r="B69" s="109" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="82"/>
+      <c r="C69" s="83"/>
       <c r="D69" s="37" t="s">
         <v>181</v>
       </c>
@@ -7021,11 +7015,11 @@
       <c r="I69" s="37"/>
     </row>
     <row r="70" spans="1:12" ht="30" customHeight="1">
-      <c r="A70" s="103"/>
-      <c r="B70" s="99" t="s">
+      <c r="A70" s="104"/>
+      <c r="B70" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="C70" s="82"/>
+      <c r="C70" s="83"/>
       <c r="D70" s="37" t="s">
         <v>183</v>
       </c>
@@ -7036,11 +7030,11 @@
       <c r="I70" s="37"/>
     </row>
     <row r="71" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A71" s="103"/>
-      <c r="B71" s="99" t="s">
+      <c r="A71" s="104"/>
+      <c r="B71" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="C71" s="82"/>
+      <c r="C71" s="83"/>
       <c r="D71" s="37" t="s">
         <v>185</v>
       </c>
@@ -7051,11 +7045,11 @@
       <c r="I71" s="37"/>
     </row>
     <row r="72" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A72" s="104"/>
-      <c r="B72" s="99" t="s">
+      <c r="A72" s="105"/>
+      <c r="B72" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C72" s="82"/>
+      <c r="C72" s="83"/>
       <c r="D72" s="37" t="s">
         <v>187</v>
       </c>
@@ -7069,11 +7063,11 @@
       <c r="A73" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="107" t="str">
+      <c r="B73" s="108" t="str">
         <f>J73&amp;K73&amp;L73</f>
         <v>td_All invoices are due and payable at the specified payment date or [invalid payment term] after invoice date if no payment schedule has been specified in the Sales Oder Contract or in Seller's confirmation of order. In case Buyer defaults in payment, Buyer shall be subject to a default late payment penalty of 1.0% of the outstanding amounts due to Seller for every calendar week or part thereof.</v>
       </c>
-      <c r="C73" s="82"/>
+      <c r="C73" s="83"/>
       <c r="D73" s="38" t="s">
         <v>189</v>
       </c>
@@ -7099,147 +7093,147 @@
       <c r="A74" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B74" s="100" t="s">
+      <c r="B74" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="C74" s="82"/>
+      <c r="C74" s="83"/>
     </row>
     <row r="75" spans="1:12" ht="14.4" customHeight="1">
       <c r="A75" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="B75" s="100" t="s">
+      <c r="B75" s="101" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="82"/>
+      <c r="C75" s="83"/>
     </row>
     <row r="76" spans="1:12" ht="28.2" customHeight="1">
-      <c r="A76" s="105" t="s">
+      <c r="A76" s="106" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="97" t="s">
+      <c r="B76" s="98" t="s">
         <v>197</v>
       </c>
-      <c r="C76" s="82"/>
+      <c r="C76" s="83"/>
     </row>
     <row r="77" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A77" s="103"/>
-      <c r="B77" s="101" t="s">
+      <c r="A77" s="104"/>
+      <c r="B77" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="C77" s="82"/>
+      <c r="C77" s="83"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="103"/>
-      <c r="B78" s="101" t="s">
+      <c r="A78" s="104"/>
+      <c r="B78" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="C78" s="82"/>
+      <c r="C78" s="83"/>
     </row>
     <row r="79" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A79" s="103"/>
-      <c r="B79" s="101" t="s">
+      <c r="A79" s="104"/>
+      <c r="B79" s="102" t="s">
         <v>200</v>
       </c>
-      <c r="C79" s="82"/>
+      <c r="C79" s="83"/>
     </row>
     <row r="80" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A80" s="103"/>
-      <c r="B80" s="101" t="s">
+      <c r="A80" s="104"/>
+      <c r="B80" s="102" t="s">
         <v>201</v>
       </c>
-      <c r="C80" s="82"/>
+      <c r="C80" s="83"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A81" s="103"/>
-      <c r="B81" s="97" t="s">
+      <c r="A81" s="104"/>
+      <c r="B81" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="82"/>
+      <c r="C81" s="83"/>
     </row>
     <row r="82" spans="1:3" ht="41.4" customHeight="1">
-      <c r="A82" s="103"/>
-      <c r="B82" s="106" t="s">
+      <c r="A82" s="104"/>
+      <c r="B82" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="C82" s="82"/>
+      <c r="C82" s="83"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A83" s="103"/>
-      <c r="B83" s="97" t="s">
+      <c r="A83" s="104"/>
+      <c r="B83" s="98" t="s">
         <v>204</v>
       </c>
-      <c r="C83" s="82"/>
+      <c r="C83" s="83"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A84" s="103"/>
-      <c r="B84" s="101" t="s">
+      <c r="A84" s="104"/>
+      <c r="B84" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="C84" s="82"/>
+      <c r="C84" s="83"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="103"/>
-      <c r="B85" s="101" t="s">
+      <c r="A85" s="104"/>
+      <c r="B85" s="102" t="s">
         <v>206</v>
       </c>
-      <c r="C85" s="82"/>
+      <c r="C85" s="83"/>
     </row>
     <row r="86" spans="1:3" ht="33.6" customHeight="1">
-      <c r="A86" s="103"/>
-      <c r="B86" s="101" t="s">
+      <c r="A86" s="104"/>
+      <c r="B86" s="102" t="s">
         <v>207</v>
       </c>
-      <c r="C86" s="82"/>
+      <c r="C86" s="83"/>
     </row>
     <row r="87" spans="1:3" ht="31.2" customHeight="1">
-      <c r="A87" s="103"/>
-      <c r="B87" s="101" t="s">
+      <c r="A87" s="104"/>
+      <c r="B87" s="102" t="s">
         <v>208</v>
       </c>
-      <c r="C87" s="82"/>
+      <c r="C87" s="83"/>
     </row>
     <row r="88" spans="1:3" ht="48.6" customHeight="1">
-      <c r="A88" s="103"/>
-      <c r="B88" s="97" t="s">
+      <c r="A88" s="104"/>
+      <c r="B88" s="98" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="82"/>
+      <c r="C88" s="83"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="104"/>
-      <c r="B89" s="97" t="s">
+      <c r="A89" s="105"/>
+      <c r="B89" s="98" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="82"/>
+      <c r="C89" s="83"/>
     </row>
     <row r="90" spans="1:3" ht="30.6" customHeight="1">
-      <c r="A90" s="105" t="s">
+      <c r="A90" s="106" t="s">
         <v>211</v>
       </c>
-      <c r="B90" s="97" t="s">
+      <c r="B90" s="98" t="s">
         <v>212</v>
       </c>
-      <c r="C90" s="82"/>
+      <c r="C90" s="83"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="104"/>
-      <c r="B91" s="97" t="s">
+      <c r="A91" s="105"/>
+      <c r="B91" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="82"/>
+      <c r="C91" s="83"/>
     </row>
     <row r="92" spans="1:3" ht="55.2" customHeight="1">
-      <c r="A92" s="109" t="s">
+      <c r="A92" s="110" t="s">
         <v>214</v>
       </c>
-      <c r="B92" s="100" t="s">
+      <c r="B92" s="101" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="82"/>
+      <c r="C92" s="83"/>
     </row>
     <row r="93" spans="1:3" ht="28.8" customHeight="1">
-      <c r="A93" s="103"/>
+      <c r="A93" s="104"/>
       <c r="B93" s="34" t="s">
         <v>216</v>
       </c>
@@ -7248,7 +7242,7 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="103"/>
+      <c r="A94" s="104"/>
       <c r="B94" s="34" t="s">
         <v>218</v>
       </c>
@@ -7257,7 +7251,7 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="103"/>
+      <c r="A95" s="104"/>
       <c r="B95" s="34" t="s">
         <v>220</v>
       </c>
@@ -7266,7 +7260,7 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="103"/>
+      <c r="A96" s="104"/>
       <c r="B96" s="34" t="s">
         <v>222</v>
       </c>
@@ -7275,7 +7269,7 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="103"/>
+      <c r="A97" s="104"/>
       <c r="B97" s="34" t="s">
         <v>224</v>
       </c>
@@ -7284,7 +7278,7 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="104"/>
+      <c r="A98" s="105"/>
       <c r="B98" s="34" t="s">
         <v>226</v>
       </c>
@@ -7296,37 +7290,37 @@
       <c r="A99" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B99" s="100" t="s">
+      <c r="B99" s="101" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="82"/>
+      <c r="C99" s="83"/>
     </row>
     <row r="100" spans="1:3" ht="30" customHeight="1">
       <c r="A100" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="98" t="s">
+      <c r="B100" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="82"/>
+      <c r="C100" s="83"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B101" s="100" t="s">
+      <c r="B101" s="101" t="s">
         <v>233</v>
       </c>
-      <c r="C101" s="82"/>
+      <c r="C101" s="83"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="100" t="s">
+      <c r="B102" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="82"/>
+      <c r="C102" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -7733,7 +7727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD4F2126-D3AA-4FAD-B204-2AEC4B5DBC7F}">
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
@@ -7748,19 +7742,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6">
       <c r="A1" s="77" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1" s="78" t="s">
         <v>435</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="D1" s="78" t="s">
         <v>436</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="E1" s="79" t="s">
         <v>437</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>438</v>
-      </c>
-      <c r="E1" s="79" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6">
@@ -7768,10 +7762,10 @@
         <v>388</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D2" s="76"/>
       <c r="E2" s="73">
@@ -7783,13 +7777,13 @@
         <v>388</v>
       </c>
       <c r="B3" s="74" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E3" s="73">
         <v>2</v>
@@ -7800,13 +7794,13 @@
         <v>388</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D4" s="74" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E4" s="73">
         <v>3</v>
@@ -7817,13 +7811,13 @@
         <v>388</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C5" s="75">
         <v>10</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E5" s="73">
         <v>4</v>
@@ -7834,13 +7828,13 @@
         <v>388</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C6" s="75">
         <v>20</v>
       </c>
       <c r="D6" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E6" s="73">
         <v>5</v>
@@ -7851,13 +7845,13 @@
         <v>388</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C7" s="75">
         <v>3</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E7" s="73">
         <v>6</v>
@@ -7871,10 +7865,10 @@
         <v>384</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D8" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E8" s="73">
         <v>7</v>
@@ -7885,13 +7879,13 @@
         <v>388</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D9" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E9" s="73">
         <v>8</v>
@@ -7902,13 +7896,13 @@
         <v>388</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E10" s="73">
         <v>9</v>
@@ -7919,13 +7913,13 @@
         <v>388</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E11" s="73">
         <v>10</v>
@@ -7936,13 +7930,13 @@
         <v>388</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D12" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E12" s="73">
         <v>11</v>
@@ -7953,13 +7947,13 @@
         <v>388</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D13" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E13" s="73">
         <v>12</v>
@@ -7970,13 +7964,13 @@
         <v>388</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D14" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E14" s="73">
         <v>13</v>
@@ -7987,13 +7981,13 @@
         <v>388</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E15" s="73">
         <v>14</v>
@@ -8004,13 +7998,13 @@
         <v>388</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D16" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E16" s="73">
         <v>15</v>
@@ -8021,13 +8015,13 @@
         <v>388</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C17" s="75">
         <v>0</v>
       </c>
       <c r="D17" s="74" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E17" s="73">
         <v>16</v>
@@ -8038,13 +8032,13 @@
         <v>388</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C18" s="75">
         <v>0</v>
       </c>
       <c r="D18" s="74" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E18" s="73">
         <v>17</v>
@@ -8055,10 +8049,10 @@
         <v>388</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="73">
@@ -8070,10 +8064,10 @@
         <v>387</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D20" s="80"/>
       <c r="E20" s="73">
@@ -8085,13 +8079,13 @@
         <v>387</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D21" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E21" s="73">
         <v>2</v>
@@ -8102,13 +8096,13 @@
         <v>387</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D22" s="74" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E22" s="73">
         <v>3</v>
@@ -8119,13 +8113,13 @@
         <v>387</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C23" s="75">
         <v>10</v>
       </c>
       <c r="D23" s="74" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E23" s="73">
         <v>4</v>
@@ -8136,13 +8130,13 @@
         <v>387</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C24" s="75">
         <v>20</v>
       </c>
       <c r="D24" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E24" s="73">
         <v>5</v>
@@ -8153,13 +8147,13 @@
         <v>387</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C25" s="75">
         <v>3</v>
       </c>
       <c r="D25" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E25" s="73">
         <v>6</v>
@@ -8170,13 +8164,13 @@
         <v>387</v>
       </c>
       <c r="B26" s="74" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D26" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E26" s="73">
         <v>7</v>
@@ -8187,13 +8181,13 @@
         <v>387</v>
       </c>
       <c r="B27" s="74" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D27" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E27" s="73">
         <v>8</v>
@@ -8204,13 +8198,13 @@
         <v>387</v>
       </c>
       <c r="B28" s="74" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D28" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E28" s="73">
         <v>9</v>
@@ -8221,13 +8215,13 @@
         <v>387</v>
       </c>
       <c r="B29" s="74" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C29" s="75">
         <v>0</v>
       </c>
       <c r="D29" s="74" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E29" s="73">
         <v>10</v>
@@ -8238,13 +8232,13 @@
         <v>387</v>
       </c>
       <c r="B30" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C30" s="75">
         <v>0</v>
       </c>
       <c r="D30" s="74" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E30" s="73">
         <v>11</v>
@@ -8255,10 +8249,10 @@
         <v>387</v>
       </c>
       <c r="B31" s="74" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D31" s="80"/>
       <c r="E31" s="73">
@@ -8270,10 +8264,10 @@
         <v>389</v>
       </c>
       <c r="B32" s="74" t="s">
-        <v>440</v>
-      </c>
-      <c r="C32" s="113" t="s">
-        <v>501</v>
+        <v>438</v>
+      </c>
+      <c r="C32" s="81" t="s">
+        <v>499</v>
       </c>
       <c r="D32" s="80"/>
       <c r="E32" s="73">
@@ -8285,13 +8279,13 @@
         <v>389</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C33" s="75">
         <v>30</v>
       </c>
       <c r="D33" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E33" s="73">
         <v>2</v>
@@ -8302,13 +8296,13 @@
         <v>389</v>
       </c>
       <c r="B34" s="74" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C34" s="75">
         <v>100</v>
       </c>
       <c r="D34" s="74" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E34" s="73">
         <v>3</v>
@@ -8319,13 +8313,13 @@
         <v>389</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C35" s="75">
         <v>30</v>
       </c>
       <c r="D35" s="74" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E35" s="73">
         <v>4</v>
@@ -8336,13 +8330,13 @@
         <v>389</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C36" s="75">
         <v>5</v>
       </c>
       <c r="D36" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E36" s="73">
         <v>5</v>
@@ -8353,13 +8347,13 @@
         <v>389</v>
       </c>
       <c r="B37" s="74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C37" s="75">
         <v>10</v>
       </c>
       <c r="D37" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E37" s="73">
         <v>6</v>
@@ -8370,13 +8364,13 @@
         <v>389</v>
       </c>
       <c r="B38" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C38" s="75">
         <v>3000</v>
       </c>
       <c r="D38" s="74" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E38" s="73">
         <v>7</v>
@@ -8387,10 +8381,10 @@
         <v>390</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>440</v>
-      </c>
-      <c r="C39" s="113" t="s">
-        <v>501</v>
+        <v>438</v>
+      </c>
+      <c r="C39" s="81" t="s">
+        <v>499</v>
       </c>
       <c r="D39" s="80"/>
       <c r="E39" s="73">
@@ -8402,13 +8396,13 @@
         <v>390</v>
       </c>
       <c r="B40" s="74" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C40" s="75">
         <v>1000</v>
       </c>
       <c r="D40" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E40" s="73">
         <v>2</v>
@@ -8419,13 +8413,13 @@
         <v>390</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C41" s="75">
         <v>40</v>
       </c>
       <c r="D41" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E41" s="73">
         <v>3</v>
@@ -8436,13 +8430,13 @@
         <v>390</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C42" s="75">
         <v>15</v>
       </c>
       <c r="D42" s="74" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E42" s="73">
         <v>4</v>
@@ -8453,13 +8447,13 @@
         <v>390</v>
       </c>
       <c r="B43" s="74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C43" s="75">
         <v>2</v>
       </c>
       <c r="D43" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E43" s="73">
         <v>5</v>
@@ -8470,13 +8464,13 @@
         <v>390</v>
       </c>
       <c r="B44" s="74" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C44" s="75">
         <v>10</v>
       </c>
       <c r="D44" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E44" s="73">
         <v>6</v>
@@ -8487,13 +8481,13 @@
         <v>390</v>
       </c>
       <c r="B45" s="74" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C45" s="75">
         <v>6</v>
       </c>
       <c r="D45" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E45" s="73">
         <v>7</v>
@@ -8504,13 +8498,13 @@
         <v>390</v>
       </c>
       <c r="B46" s="74" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C46" s="75">
         <v>300</v>
       </c>
       <c r="D46" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E46" s="73">
         <v>8</v>
@@ -8521,13 +8515,13 @@
         <v>390</v>
       </c>
       <c r="B47" s="74" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C47" s="75">
         <v>300</v>
       </c>
       <c r="D47" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E47" s="73">
         <v>9</v>
@@ -8538,13 +8532,13 @@
         <v>390</v>
       </c>
       <c r="B48" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C48" s="75">
         <v>10</v>
       </c>
       <c r="D48" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E48" s="73">
         <v>10</v>
@@ -8555,13 +8549,13 @@
         <v>390</v>
       </c>
       <c r="B49" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C49" s="75" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D49" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E49" s="73">
         <v>11</v>
@@ -8572,13 +8566,13 @@
         <v>390</v>
       </c>
       <c r="B50" s="74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C50" s="75" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D50" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E50" s="73">
         <v>12</v>
@@ -8589,13 +8583,13 @@
         <v>390</v>
       </c>
       <c r="B51" s="74" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C51" s="75">
         <v>15</v>
       </c>
       <c r="D51" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E51" s="73">
         <v>13</v>
@@ -8606,13 +8600,13 @@
         <v>390</v>
       </c>
       <c r="B52" s="74" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C52" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D52" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E52" s="73">
         <v>14</v>
@@ -8623,13 +8617,13 @@
         <v>390</v>
       </c>
       <c r="B53" s="74" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C53" s="75">
         <v>1</v>
       </c>
       <c r="D53" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E53" s="73">
         <v>15</v>
@@ -8640,13 +8634,13 @@
         <v>390</v>
       </c>
       <c r="B54" s="74" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D54" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E54" s="73">
         <v>16</v>
@@ -8657,13 +8651,13 @@
         <v>390</v>
       </c>
       <c r="B55" s="74" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D55" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E55" s="73">
         <v>17</v>
@@ -8674,13 +8668,13 @@
         <v>390</v>
       </c>
       <c r="B56" s="74" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D56" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E56" s="73">
         <v>18</v>
@@ -8691,13 +8685,13 @@
         <v>390</v>
       </c>
       <c r="B57" s="74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C57" s="75">
         <v>1</v>
       </c>
       <c r="D57" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E57" s="73">
         <v>19</v>
@@ -8708,13 +8702,13 @@
         <v>390</v>
       </c>
       <c r="B58" s="74" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D58" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E58" s="73">
         <v>20</v>
@@ -8725,13 +8719,13 @@
         <v>390</v>
       </c>
       <c r="B59" s="74" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C59" s="75">
         <v>100</v>
       </c>
       <c r="D59" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E59" s="73">
         <v>21</v>
@@ -8742,13 +8736,13 @@
         <v>390</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C60" s="75">
         <v>1000</v>
       </c>
       <c r="D60" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E60" s="73">
         <v>22</v>
@@ -8759,10 +8753,10 @@
         <v>391</v>
       </c>
       <c r="B61" s="74" t="s">
-        <v>440</v>
-      </c>
-      <c r="C61" s="113" t="s">
-        <v>501</v>
+        <v>438</v>
+      </c>
+      <c r="C61" s="81" t="s">
+        <v>499</v>
       </c>
       <c r="D61" s="80"/>
       <c r="E61" s="73">
@@ -8774,13 +8768,13 @@
         <v>391</v>
       </c>
       <c r="B62" s="74" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C62" s="75">
         <v>1000</v>
       </c>
       <c r="D62" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E62" s="73">
         <v>2</v>
@@ -8791,13 +8785,13 @@
         <v>391</v>
       </c>
       <c r="B63" s="74" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C63" s="75">
         <v>50</v>
       </c>
       <c r="D63" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E63" s="73">
         <v>3</v>
@@ -8808,13 +8802,13 @@
         <v>391</v>
       </c>
       <c r="B64" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C64" s="75">
         <v>50</v>
       </c>
       <c r="D64" s="74" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E64" s="73">
         <v>4</v>
@@ -8825,13 +8819,13 @@
         <v>391</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C65" s="75">
         <v>3</v>
       </c>
       <c r="D65" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E65" s="73">
         <v>5</v>
@@ -8842,13 +8836,13 @@
         <v>391</v>
       </c>
       <c r="B66" s="74" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C66" s="75">
         <v>25</v>
       </c>
       <c r="D66" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E66" s="73">
         <v>6</v>
@@ -8859,13 +8853,13 @@
         <v>391</v>
       </c>
       <c r="B67" s="74" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C67" s="75">
         <v>4</v>
       </c>
       <c r="D67" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E67" s="73">
         <v>7</v>
@@ -8876,13 +8870,13 @@
         <v>391</v>
       </c>
       <c r="B68" s="74" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C68" s="75">
         <v>300</v>
       </c>
       <c r="D68" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E68" s="73">
         <v>8</v>
@@ -8893,13 +8887,13 @@
         <v>391</v>
       </c>
       <c r="B69" s="74" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C69" s="75">
         <v>300</v>
       </c>
       <c r="D69" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E69" s="73">
         <v>9</v>
@@ -8910,13 +8904,13 @@
         <v>391</v>
       </c>
       <c r="B70" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C70" s="75">
         <v>10</v>
       </c>
       <c r="D70" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E70" s="73">
         <v>10</v>
@@ -8927,13 +8921,13 @@
         <v>391</v>
       </c>
       <c r="B71" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D71" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E71" s="73">
         <v>11</v>
@@ -8944,13 +8938,13 @@
         <v>391</v>
       </c>
       <c r="B72" s="74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D72" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E72" s="73">
         <v>12</v>
@@ -8961,13 +8955,13 @@
         <v>391</v>
       </c>
       <c r="B73" s="74" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C73" s="75">
         <v>15</v>
       </c>
       <c r="D73" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E73" s="73">
         <v>13</v>
@@ -8978,13 +8972,13 @@
         <v>391</v>
       </c>
       <c r="B74" s="74" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D74" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E74" s="73">
         <v>14</v>
@@ -8995,13 +8989,13 @@
         <v>391</v>
       </c>
       <c r="B75" s="74" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D75" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E75" s="73">
         <v>15</v>
@@ -9012,13 +9006,13 @@
         <v>391</v>
       </c>
       <c r="B76" s="74" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D76" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E76" s="73">
         <v>16</v>
@@ -9029,13 +9023,13 @@
         <v>391</v>
       </c>
       <c r="B77" s="74" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C77" s="75" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D77" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E77" s="73">
         <v>17</v>
@@ -9046,13 +9040,13 @@
         <v>391</v>
       </c>
       <c r="B78" s="74" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C78" s="75" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D78" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E78" s="73">
         <v>18</v>
@@ -9063,13 +9057,13 @@
         <v>391</v>
       </c>
       <c r="B79" s="74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C79" s="75">
         <v>1</v>
       </c>
       <c r="D79" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E79" s="73">
         <v>19</v>
@@ -9080,13 +9074,13 @@
         <v>391</v>
       </c>
       <c r="B80" s="74" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C80" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D80" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E80" s="73">
         <v>20</v>
@@ -9097,13 +9091,13 @@
         <v>391</v>
       </c>
       <c r="B81" s="74" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C81" s="75">
         <v>1000</v>
       </c>
       <c r="D81" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E81" s="73">
         <v>21</v>
@@ -9114,13 +9108,13 @@
         <v>391</v>
       </c>
       <c r="B82" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C82" s="75">
         <v>5000</v>
       </c>
       <c r="D82" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E82" s="73">
         <v>22</v>
@@ -9131,10 +9125,10 @@
         <v>392</v>
       </c>
       <c r="B83" s="74" t="s">
-        <v>440</v>
-      </c>
-      <c r="C83" s="113" t="s">
-        <v>501</v>
+        <v>438</v>
+      </c>
+      <c r="C83" s="81" t="s">
+        <v>499</v>
       </c>
       <c r="D83" s="80"/>
       <c r="E83" s="73">
@@ -9146,13 +9140,13 @@
         <v>392</v>
       </c>
       <c r="B84" s="74" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C84" s="75">
         <v>1000</v>
       </c>
       <c r="D84" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E84" s="73">
         <v>2</v>
@@ -9163,13 +9157,13 @@
         <v>392</v>
       </c>
       <c r="B85" s="74" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C85" s="75">
         <v>100</v>
       </c>
       <c r="D85" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E85" s="73">
         <v>3</v>
@@ -9180,13 +9174,13 @@
         <v>392</v>
       </c>
       <c r="B86" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C86" s="75">
         <v>100</v>
       </c>
       <c r="D86" s="74" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E86" s="73">
         <v>4</v>
@@ -9197,13 +9191,13 @@
         <v>392</v>
       </c>
       <c r="B87" s="74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C87" s="75">
         <v>6</v>
       </c>
       <c r="D87" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E87" s="73">
         <v>5</v>
@@ -9214,13 +9208,13 @@
         <v>392</v>
       </c>
       <c r="B88" s="74" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C88" s="75">
         <v>40</v>
       </c>
       <c r="D88" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E88" s="73">
         <v>6</v>
@@ -9231,13 +9225,13 @@
         <v>392</v>
       </c>
       <c r="B89" s="74" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C89" s="75">
         <v>3</v>
       </c>
       <c r="D89" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E89" s="73">
         <v>7</v>
@@ -9248,13 +9242,13 @@
         <v>392</v>
       </c>
       <c r="B90" s="74" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C90" s="75">
         <v>300</v>
       </c>
       <c r="D90" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E90" s="73">
         <v>8</v>
@@ -9265,13 +9259,13 @@
         <v>392</v>
       </c>
       <c r="B91" s="74" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C91" s="75">
         <v>300</v>
       </c>
       <c r="D91" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E91" s="73">
         <v>9</v>
@@ -9282,13 +9276,13 @@
         <v>392</v>
       </c>
       <c r="B92" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C92" s="75">
         <v>20</v>
       </c>
       <c r="D92" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E92" s="73">
         <v>10</v>
@@ -9299,13 +9293,13 @@
         <v>392</v>
       </c>
       <c r="B93" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C93" s="75" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D93" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E93" s="73">
         <v>11</v>
@@ -9316,13 +9310,13 @@
         <v>392</v>
       </c>
       <c r="B94" s="74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C94" s="75" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D94" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E94" s="73">
         <v>12</v>
@@ -9333,13 +9327,13 @@
         <v>392</v>
       </c>
       <c r="B95" s="74" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C95" s="75">
         <v>25</v>
       </c>
       <c r="D95" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E95" s="73">
         <v>13</v>
@@ -9350,13 +9344,13 @@
         <v>392</v>
       </c>
       <c r="B96" s="74" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C96" s="75">
         <v>1</v>
       </c>
       <c r="D96" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E96" s="73">
         <v>14</v>
@@ -9367,13 +9361,13 @@
         <v>392</v>
       </c>
       <c r="B97" s="74" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C97" s="75" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D97" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E97" s="73">
         <v>15</v>
@@ -9384,13 +9378,13 @@
         <v>392</v>
       </c>
       <c r="B98" s="74" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C98" s="75" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D98" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E98" s="73">
         <v>16</v>
@@ -9401,13 +9395,13 @@
         <v>392</v>
       </c>
       <c r="B99" s="74" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C99" s="75" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D99" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E99" s="73">
         <v>17</v>
@@ -9418,13 +9412,13 @@
         <v>392</v>
       </c>
       <c r="B100" s="74" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C100" s="75" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D100" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E100" s="73">
         <v>18</v>
@@ -9435,13 +9429,13 @@
         <v>392</v>
       </c>
       <c r="B101" s="74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C101" s="75">
         <v>1</v>
       </c>
       <c r="D101" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E101" s="73">
         <v>19</v>
@@ -9452,13 +9446,13 @@
         <v>392</v>
       </c>
       <c r="B102" s="74" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C102" s="75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D102" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E102" s="73">
         <v>20</v>
@@ -9469,13 +9463,13 @@
         <v>392</v>
       </c>
       <c r="B103" s="74" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C103" s="75">
         <v>2000</v>
       </c>
       <c r="D103" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E103" s="73">
         <v>21</v>
@@ -9486,13 +9480,13 @@
         <v>392</v>
       </c>
       <c r="B104" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C104" s="75">
         <v>10000</v>
       </c>
       <c r="D104" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E104" s="73">
         <v>22</v>
@@ -9503,10 +9497,10 @@
         <v>393</v>
       </c>
       <c r="B105" s="74" t="s">
-        <v>440</v>
-      </c>
-      <c r="C105" s="113" t="s">
-        <v>501</v>
+        <v>438</v>
+      </c>
+      <c r="C105" s="81" t="s">
+        <v>499</v>
       </c>
       <c r="D105" s="80"/>
       <c r="E105" s="73">
@@ -9518,13 +9512,13 @@
         <v>393</v>
       </c>
       <c r="B106" s="74" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C106" s="75">
         <v>2000</v>
       </c>
       <c r="D106" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E106" s="73">
         <v>2</v>
@@ -9535,13 +9529,13 @@
         <v>393</v>
       </c>
       <c r="B107" s="74" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C107" s="75">
         <v>400</v>
       </c>
       <c r="D107" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E107" s="73">
         <v>3</v>
@@ -9552,13 +9546,13 @@
         <v>393</v>
       </c>
       <c r="B108" s="74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D108" s="74" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E108" s="73">
         <v>4</v>
@@ -9569,13 +9563,13 @@
         <v>393</v>
       </c>
       <c r="B109" s="74" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C109" s="75">
         <v>12</v>
       </c>
       <c r="D109" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E109" s="73">
         <v>5</v>
@@ -9586,13 +9580,13 @@
         <v>393</v>
       </c>
       <c r="B110" s="74" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C110" s="75">
         <v>80</v>
       </c>
       <c r="D110" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E110" s="73">
         <v>6</v>
@@ -9603,13 +9597,13 @@
         <v>393</v>
       </c>
       <c r="B111" s="74" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C111" s="75">
         <v>1</v>
       </c>
       <c r="D111" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E111" s="73">
         <v>7</v>
@@ -9620,13 +9614,13 @@
         <v>393</v>
       </c>
       <c r="B112" s="74" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C112" s="75">
         <v>400</v>
       </c>
       <c r="D112" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E112" s="73">
         <v>8</v>
@@ -9637,13 +9631,13 @@
         <v>393</v>
       </c>
       <c r="B113" s="74" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C113" s="75">
         <v>600</v>
       </c>
       <c r="D113" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E113" s="73">
         <v>9</v>
@@ -9654,13 +9648,13 @@
         <v>393</v>
       </c>
       <c r="B114" s="74" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C114" s="75">
         <v>20</v>
       </c>
       <c r="D114" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E114" s="73">
         <v>10</v>
@@ -9671,13 +9665,13 @@
         <v>393</v>
       </c>
       <c r="B115" s="74" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C115" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D115" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E115" s="73">
         <v>11</v>
@@ -9688,13 +9682,13 @@
         <v>393</v>
       </c>
       <c r="B116" s="74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C116" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D116" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E116" s="73">
         <v>12</v>
@@ -9705,13 +9699,13 @@
         <v>393</v>
       </c>
       <c r="B117" s="74" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C117" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D117" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E117" s="73">
         <v>13</v>
@@ -9722,13 +9716,13 @@
         <v>393</v>
       </c>
       <c r="B118" s="74" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C118" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D118" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E118" s="73">
         <v>14</v>
@@ -9739,13 +9733,13 @@
         <v>393</v>
       </c>
       <c r="B119" s="74" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C119" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D119" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E119" s="73">
         <v>15</v>
@@ -9756,13 +9750,13 @@
         <v>393</v>
       </c>
       <c r="B120" s="74" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C120" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D120" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E120" s="73">
         <v>16</v>
@@ -9773,13 +9767,13 @@
         <v>393</v>
       </c>
       <c r="B121" s="74" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C121" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D121" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E121" s="73">
         <v>17</v>
@@ -9790,13 +9784,13 @@
         <v>393</v>
       </c>
       <c r="B122" s="74" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C122" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D122" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E122" s="73">
         <v>18</v>
@@ -9807,13 +9801,13 @@
         <v>393</v>
       </c>
       <c r="B123" s="74" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C123" s="75">
         <v>10</v>
       </c>
       <c r="D123" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E123" s="73">
         <v>19</v>
@@ -9824,13 +9818,13 @@
         <v>393</v>
       </c>
       <c r="B124" s="74" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C124" s="75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D124" s="74" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E124" s="73">
         <v>20</v>
@@ -9841,13 +9835,13 @@
         <v>393</v>
       </c>
       <c r="B125" s="74" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C125" s="75">
         <v>2000</v>
       </c>
       <c r="D125" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E125" s="73">
         <v>21</v>
@@ -9858,13 +9852,13 @@
         <v>393</v>
       </c>
       <c r="B126" s="74" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C126" s="75">
         <v>10000</v>
       </c>
       <c r="D126" s="74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E126" s="73">
         <v>22</v>

</xml_diff>